<commit_message>
small change to EMX_3
</commit_message>
<xml_diff>
--- a/EMX_3.xlsx
+++ b/EMX_3.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\GitHub\docubase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -141,90 +146,6 @@
     <t>Recording from neruons in the AAV-ChR2 injection site. Trying to demonstrate that stimulation in the axon pathway (white matter) can elicit spikes in the absence of poly synaptic effects. And trying to determine the temporal frequencies we can stimulate at in the white matter.</t>
   </si>
   <si>
-    <t>13d02000</t>
-  </si>
-  <si>
-    <t>13d02001</t>
-  </si>
-  <si>
-    <t>13d02002</t>
-  </si>
-  <si>
-    <t>13d02003</t>
-  </si>
-  <si>
-    <t>13d02004</t>
-  </si>
-  <si>
-    <t>13d02005</t>
-  </si>
-  <si>
-    <t>13d02006</t>
-  </si>
-  <si>
-    <t>13d02007</t>
-  </si>
-  <si>
-    <t>13d02008</t>
-  </si>
-  <si>
-    <t>13d02009</t>
-  </si>
-  <si>
-    <t>13d02010</t>
-  </si>
-  <si>
-    <t>13d02011</t>
-  </si>
-  <si>
-    <t>13d02012</t>
-  </si>
-  <si>
-    <t>13d02013</t>
-  </si>
-  <si>
-    <t>13d02014</t>
-  </si>
-  <si>
-    <t>13d02015</t>
-  </si>
-  <si>
-    <t>13d02016</t>
-  </si>
-  <si>
-    <t>13d02017</t>
-  </si>
-  <si>
-    <t>13d02018</t>
-  </si>
-  <si>
-    <t>13d02019</t>
-  </si>
-  <si>
-    <t>13d02020</t>
-  </si>
-  <si>
-    <t>13d02021</t>
-  </si>
-  <si>
-    <t>13d02022</t>
-  </si>
-  <si>
-    <t>13d02023</t>
-  </si>
-  <si>
-    <t>13d02024</t>
-  </si>
-  <si>
-    <t>13d02025</t>
-  </si>
-  <si>
-    <t>13d02026</t>
-  </si>
-  <si>
-    <t>13d02027</t>
-  </si>
-  <si>
     <t>No clipped ears</t>
   </si>
   <si>
@@ -277,6 +198,93 @@
   </si>
   <si>
     <t>Slices per plate               (or list of numbers for each plate)</t>
+  </si>
+  <si>
+    <t>470 nm steps targeting the axon path below L6</t>
+  </si>
+  <si>
+    <t>13d20000</t>
+  </si>
+  <si>
+    <t>13d20001</t>
+  </si>
+  <si>
+    <t>13d20002</t>
+  </si>
+  <si>
+    <t>13d20003</t>
+  </si>
+  <si>
+    <t>13d20004</t>
+  </si>
+  <si>
+    <t>13d20005</t>
+  </si>
+  <si>
+    <t>13d20006</t>
+  </si>
+  <si>
+    <t>13d20007</t>
+  </si>
+  <si>
+    <t>13d20008</t>
+  </si>
+  <si>
+    <t>13d20009</t>
+  </si>
+  <si>
+    <t>13d20010</t>
+  </si>
+  <si>
+    <t>13d20011</t>
+  </si>
+  <si>
+    <t>13d20012</t>
+  </si>
+  <si>
+    <t>13d20013</t>
+  </si>
+  <si>
+    <t>13d20014</t>
+  </si>
+  <si>
+    <t>13d20015</t>
+  </si>
+  <si>
+    <t>13d20016</t>
+  </si>
+  <si>
+    <t>13d20017</t>
+  </si>
+  <si>
+    <t>13d20018</t>
+  </si>
+  <si>
+    <t>13d20019</t>
+  </si>
+  <si>
+    <t>13d20020</t>
+  </si>
+  <si>
+    <t>13d20021</t>
+  </si>
+  <si>
+    <t>13d20022</t>
+  </si>
+  <si>
+    <t>13d20023</t>
+  </si>
+  <si>
+    <t>13d20024</t>
+  </si>
+  <si>
+    <t>13d20025</t>
+  </si>
+  <si>
+    <t>13d20026</t>
+  </si>
+  <si>
+    <t>13d20027</t>
   </si>
 </sst>
 </file>
@@ -1092,6 +1100,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1423,14 +1439,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="62.375" style="28" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1">
+    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +1454,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="38" customHeight="1">
+    <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
@@ -1446,13 +1462,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1">
+    <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1">
+    <row r="4" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1460,15 +1476,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1">
+    <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
@@ -1476,19 +1492,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38" customHeight="1" thickTop="1"/>
-    <row r="8" spans="1:2" ht="38" customHeight="1"/>
-    <row r="9" spans="1:2" ht="38" customHeight="1"/>
-    <row r="10" spans="1:2" ht="38" customHeight="1"/>
-    <row r="11" spans="1:2" ht="38" customHeight="1"/>
-    <row r="12" spans="1:2" ht="38" customHeight="1"/>
-    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1">
+    <row r="7" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1501,24 +1517,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:H35"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="18" customWidth="1"/>
     <col min="6" max="6" width="34.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1">
+    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>7</v>
       </c>
@@ -1536,13 +1552,13 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39" customHeight="1">
+    <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="46" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D2" s="61"/>
       <c r="E2" s="61"/>
@@ -1554,7 +1570,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39" customHeight="1">
+    <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1584,7 @@
       <c r="G3" s="47"/>
       <c r="H3" s="48"/>
     </row>
-    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1">
+    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
         <v>10</v>
       </c>
@@ -1582,7 +1598,7 @@
       <c r="G4" s="51"/>
       <c r="H4" s="52"/>
     </row>
-    <row r="5" spans="1:8" ht="26" customHeight="1" thickTop="1" thickBot="1">
+    <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -1592,7 +1608,7 @@
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
     </row>
-    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1">
+    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1614,132 +1630,134 @@
       <c r="G6" s="42"/>
       <c r="H6" s="43"/>
     </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1">
+    <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>1</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
       <c r="F7" s="35" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="37"/>
     </row>
-    <row r="8" spans="1:8" ht="39" customHeight="1">
+    <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>1</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
       <c r="F8" s="35" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="37"/>
     </row>
-    <row r="9" spans="1:8" ht="39" customHeight="1">
+    <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
       <c r="B9" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>69</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
       <c r="F9" s="35" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="37"/>
     </row>
-    <row r="10" spans="1:8" ht="39" customHeight="1">
+    <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>1</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
       <c r="F10" s="35" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="G10" s="36"/>
       <c r="H10" s="37"/>
     </row>
-    <row r="11" spans="1:8" ht="39" customHeight="1">
+    <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>1</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
       <c r="F11" s="35" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="G11" s="36"/>
       <c r="H11" s="37"/>
     </row>
-    <row r="12" spans="1:8" ht="39" customHeight="1">
+    <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>1</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
       <c r="F12" s="35" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="G12" s="36"/>
       <c r="H12" s="37"/>
     </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1">
+    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>1</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
-      <c r="F13" s="35"/>
+      <c r="F13" s="35" t="s">
+        <v>57</v>
+      </c>
       <c r="G13" s="36"/>
       <c r="H13" s="37"/>
     </row>
-    <row r="14" spans="1:8" ht="39" customHeight="1">
+    <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>1</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
@@ -1748,12 +1766,12 @@
       <c r="G14" s="36"/>
       <c r="H14" s="37"/>
     </row>
-    <row r="15" spans="1:8" ht="39" customHeight="1">
+    <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>1</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="31"/>
@@ -1762,12 +1780,12 @@
       <c r="G15" s="36"/>
       <c r="H15" s="37"/>
     </row>
-    <row r="16" spans="1:8" ht="39" customHeight="1">
+    <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>1</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="31"/>
@@ -1776,12 +1794,12 @@
       <c r="G16" s="36"/>
       <c r="H16" s="37"/>
     </row>
-    <row r="17" spans="1:8" ht="39" customHeight="1">
+    <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>1</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="31"/>
@@ -1790,12 +1808,12 @@
       <c r="G17" s="36"/>
       <c r="H17" s="37"/>
     </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1">
+    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>1</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
@@ -1804,62 +1822,62 @@
       <c r="G18" s="36"/>
       <c r="H18" s="37"/>
     </row>
-    <row r="19" spans="1:8" ht="39" customHeight="1">
+    <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>1</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
       <c r="F19" s="35" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="G19" s="36"/>
       <c r="H19" s="37"/>
     </row>
-    <row r="20" spans="1:8" ht="39" customHeight="1">
+    <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>1</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
       <c r="F20" s="35" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="G20" s="36"/>
       <c r="H20" s="37"/>
     </row>
-    <row r="21" spans="1:8" ht="39" customHeight="1">
+    <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>1</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
       <c r="F21" s="35" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="G21" s="36"/>
       <c r="H21" s="37"/>
     </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1">
+    <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>1</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
@@ -1868,12 +1886,12 @@
       <c r="G22" s="36"/>
       <c r="H22" s="37"/>
     </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1">
+    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>1</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="31"/>
@@ -1882,12 +1900,12 @@
       <c r="G23" s="36"/>
       <c r="H23" s="37"/>
     </row>
-    <row r="24" spans="1:8" ht="39" customHeight="1">
+    <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>1</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
@@ -1896,12 +1914,12 @@
       <c r="G24" s="36"/>
       <c r="H24" s="37"/>
     </row>
-    <row r="25" spans="1:8" ht="39" customHeight="1">
+    <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>1</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
@@ -1910,28 +1928,28 @@
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:8" ht="39" customHeight="1">
+    <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>1</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
       <c r="F26" s="35" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="G26" s="36"/>
       <c r="H26" s="37"/>
     </row>
-    <row r="27" spans="1:8" ht="39" customHeight="1">
+    <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>1</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="31"/>
@@ -1940,12 +1958,12 @@
       <c r="G27" s="36"/>
       <c r="H27" s="37"/>
     </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1">
+    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>1</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="31"/>
@@ -1954,46 +1972,46 @@
       <c r="G28" s="36"/>
       <c r="H28" s="37"/>
     </row>
-    <row r="29" spans="1:8" ht="39" customHeight="1">
+    <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>1</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
       <c r="F29" s="35" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
     </row>
-    <row r="30" spans="1:8" ht="39" customHeight="1">
+    <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>1</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
       <c r="F30" s="35" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
     </row>
-    <row r="31" spans="1:8" ht="39" customHeight="1">
+    <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>1</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="31"/>
@@ -2002,12 +2020,12 @@
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
     </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1">
+    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>1</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="31"/>
@@ -2016,12 +2034,12 @@
       <c r="G32" s="36"/>
       <c r="H32" s="37"/>
     </row>
-    <row r="33" spans="1:8" ht="39" customHeight="1">
+    <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>1</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="31"/>
@@ -2030,23 +2048,23 @@
       <c r="G33" s="36"/>
       <c r="H33" s="37"/>
     </row>
-    <row r="34" spans="1:8" ht="39" customHeight="1">
+    <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
         <v>1</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
       <c r="F34" s="35" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="37"/>
     </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1">
+    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -2056,7 +2074,7 @@
       <c r="G35" s="36"/>
       <c r="H35" s="37"/>
     </row>
-    <row r="36" spans="1:8" ht="39" customHeight="1">
+    <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -2066,7 +2084,7 @@
       <c r="G36" s="36"/>
       <c r="H36" s="37"/>
     </row>
-    <row r="37" spans="1:8" ht="39" customHeight="1">
+    <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -2076,7 +2094,7 @@
       <c r="G37" s="36"/>
       <c r="H37" s="37"/>
     </row>
-    <row r="38" spans="1:8" ht="39" customHeight="1">
+    <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -2086,7 +2104,7 @@
       <c r="G38" s="36"/>
       <c r="H38" s="37"/>
     </row>
-    <row r="39" spans="1:8" ht="39" customHeight="1">
+    <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -2096,7 +2114,7 @@
       <c r="G39" s="36"/>
       <c r="H39" s="37"/>
     </row>
-    <row r="40" spans="1:8" ht="39" customHeight="1">
+    <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -2106,7 +2124,7 @@
       <c r="G40" s="36"/>
       <c r="H40" s="37"/>
     </row>
-    <row r="41" spans="1:8" ht="39" customHeight="1">
+    <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -2116,7 +2134,7 @@
       <c r="G41" s="36"/>
       <c r="H41" s="37"/>
     </row>
-    <row r="42" spans="1:8" ht="39" customHeight="1">
+    <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -2126,7 +2144,7 @@
       <c r="G42" s="36"/>
       <c r="H42" s="37"/>
     </row>
-    <row r="43" spans="1:8" ht="39" customHeight="1">
+    <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
@@ -2136,7 +2154,7 @@
       <c r="G43" s="36"/>
       <c r="H43" s="37"/>
     </row>
-    <row r="44" spans="1:8" ht="39" customHeight="1">
+    <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
@@ -2146,7 +2164,7 @@
       <c r="G44" s="36"/>
       <c r="H44" s="37"/>
     </row>
-    <row r="45" spans="1:8" ht="39" customHeight="1">
+    <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
@@ -2156,7 +2174,7 @@
       <c r="G45" s="36"/>
       <c r="H45" s="37"/>
     </row>
-    <row r="46" spans="1:8" ht="39" customHeight="1">
+    <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="29"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
@@ -2166,7 +2184,7 @@
       <c r="G46" s="36"/>
       <c r="H46" s="37"/>
     </row>
-    <row r="47" spans="1:8" ht="39" customHeight="1">
+    <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="29"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -2176,7 +2194,7 @@
       <c r="G47" s="36"/>
       <c r="H47" s="37"/>
     </row>
-    <row r="48" spans="1:8" ht="39" customHeight="1">
+    <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="29"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
@@ -2186,7 +2204,7 @@
       <c r="G48" s="36"/>
       <c r="H48" s="37"/>
     </row>
-    <row r="49" spans="1:8" ht="39" customHeight="1">
+    <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
@@ -2196,7 +2214,7 @@
       <c r="G49" s="36"/>
       <c r="H49" s="37"/>
     </row>
-    <row r="50" spans="1:8" ht="39" customHeight="1">
+    <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="29"/>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
@@ -2206,7 +2224,7 @@
       <c r="G50" s="36"/>
       <c r="H50" s="37"/>
     </row>
-    <row r="51" spans="1:8" ht="39" customHeight="1">
+    <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
@@ -2216,7 +2234,7 @@
       <c r="G51" s="36"/>
       <c r="H51" s="37"/>
     </row>
-    <row r="52" spans="1:8" ht="39" customHeight="1">
+    <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="29"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
@@ -2226,7 +2244,7 @@
       <c r="G52" s="36"/>
       <c r="H52" s="37"/>
     </row>
-    <row r="53" spans="1:8" ht="39" customHeight="1">
+    <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -2236,7 +2254,7 @@
       <c r="G53" s="36"/>
       <c r="H53" s="37"/>
     </row>
-    <row r="54" spans="1:8" ht="39" customHeight="1">
+    <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="29"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
@@ -2246,7 +2264,7 @@
       <c r="G54" s="36"/>
       <c r="H54" s="37"/>
     </row>
-    <row r="55" spans="1:8" ht="39" customHeight="1">
+    <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="29"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
@@ -2256,7 +2274,7 @@
       <c r="G55" s="36"/>
       <c r="H55" s="37"/>
     </row>
-    <row r="56" spans="1:8" ht="39" customHeight="1">
+    <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
@@ -2266,7 +2284,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="37"/>
     </row>
-    <row r="57" spans="1:8" ht="39" customHeight="1">
+    <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="29"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
@@ -2276,7 +2294,7 @@
       <c r="G57" s="36"/>
       <c r="H57" s="37"/>
     </row>
-    <row r="58" spans="1:8" ht="39" customHeight="1">
+    <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="29"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
@@ -2286,7 +2304,7 @@
       <c r="G58" s="36"/>
       <c r="H58" s="37"/>
     </row>
-    <row r="59" spans="1:8" ht="39" customHeight="1">
+    <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="29"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
@@ -2296,7 +2314,7 @@
       <c r="G59" s="36"/>
       <c r="H59" s="37"/>
     </row>
-    <row r="60" spans="1:8" ht="39" customHeight="1">
+    <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="29"/>
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
@@ -2306,7 +2324,7 @@
       <c r="G60" s="36"/>
       <c r="H60" s="37"/>
     </row>
-    <row r="61" spans="1:8" ht="39" customHeight="1">
+    <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="29"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
@@ -2316,7 +2334,7 @@
       <c r="G61" s="36"/>
       <c r="H61" s="37"/>
     </row>
-    <row r="62" spans="1:8" ht="39" customHeight="1">
+    <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
@@ -2326,7 +2344,7 @@
       <c r="G62" s="36"/>
       <c r="H62" s="37"/>
     </row>
-    <row r="63" spans="1:8" ht="39" customHeight="1">
+    <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="29"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
@@ -2336,7 +2354,7 @@
       <c r="G63" s="36"/>
       <c r="H63" s="37"/>
     </row>
-    <row r="64" spans="1:8" ht="39" customHeight="1">
+    <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
@@ -2346,7 +2364,7 @@
       <c r="G64" s="36"/>
       <c r="H64" s="37"/>
     </row>
-    <row r="65" spans="1:8" ht="39" customHeight="1">
+    <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="29"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
@@ -2356,7 +2374,7 @@
       <c r="G65" s="36"/>
       <c r="H65" s="37"/>
     </row>
-    <row r="66" spans="1:8" ht="39" customHeight="1">
+    <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="29"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
@@ -2366,7 +2384,7 @@
       <c r="G66" s="36"/>
       <c r="H66" s="37"/>
     </row>
-    <row r="67" spans="1:8" ht="39" customHeight="1">
+    <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="29"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
@@ -2376,7 +2394,7 @@
       <c r="G67" s="36"/>
       <c r="H67" s="37"/>
     </row>
-    <row r="68" spans="1:8" ht="39" customHeight="1">
+    <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="29"/>
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
@@ -2386,7 +2404,7 @@
       <c r="G68" s="36"/>
       <c r="H68" s="37"/>
     </row>
-    <row r="69" spans="1:8" ht="39" customHeight="1">
+    <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="29"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
@@ -2396,7 +2414,7 @@
       <c r="G69" s="36"/>
       <c r="H69" s="37"/>
     </row>
-    <row r="70" spans="1:8" ht="39" customHeight="1">
+    <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="29"/>
       <c r="B70" s="30"/>
       <c r="C70" s="30"/>
@@ -2406,7 +2424,7 @@
       <c r="G70" s="36"/>
       <c r="H70" s="37"/>
     </row>
-    <row r="71" spans="1:8" ht="39" customHeight="1">
+    <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="29"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
@@ -2416,7 +2434,7 @@
       <c r="G71" s="36"/>
       <c r="H71" s="37"/>
     </row>
-    <row r="72" spans="1:8" ht="39" customHeight="1">
+    <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="29"/>
       <c r="B72" s="30"/>
       <c r="C72" s="30"/>
@@ -2426,7 +2444,7 @@
       <c r="G72" s="36"/>
       <c r="H72" s="37"/>
     </row>
-    <row r="73" spans="1:8" ht="39" customHeight="1">
+    <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="29"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
@@ -2436,7 +2454,7 @@
       <c r="G73" s="36"/>
       <c r="H73" s="37"/>
     </row>
-    <row r="74" spans="1:8" ht="39" customHeight="1">
+    <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="29"/>
       <c r="B74" s="30"/>
       <c r="C74" s="30"/>
@@ -2446,7 +2464,7 @@
       <c r="G74" s="36"/>
       <c r="H74" s="37"/>
     </row>
-    <row r="75" spans="1:8" ht="39" customHeight="1">
+    <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="29"/>
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
@@ -2456,7 +2474,7 @@
       <c r="G75" s="36"/>
       <c r="H75" s="37"/>
     </row>
-    <row r="76" spans="1:8" ht="39" customHeight="1">
+    <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="29"/>
       <c r="B76" s="30"/>
       <c r="C76" s="30"/>
@@ -2466,7 +2484,7 @@
       <c r="G76" s="36"/>
       <c r="H76" s="37"/>
     </row>
-    <row r="77" spans="1:8" ht="39" customHeight="1">
+    <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="29"/>
       <c r="B77" s="30"/>
       <c r="C77" s="30"/>
@@ -2476,7 +2494,7 @@
       <c r="G77" s="36"/>
       <c r="H77" s="37"/>
     </row>
-    <row r="78" spans="1:8" ht="39" customHeight="1">
+    <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="29"/>
       <c r="B78" s="30"/>
       <c r="C78" s="30"/>
@@ -2486,7 +2504,7 @@
       <c r="G78" s="36"/>
       <c r="H78" s="37"/>
     </row>
-    <row r="79" spans="1:8" ht="39" customHeight="1">
+    <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="29"/>
       <c r="B79" s="30"/>
       <c r="C79" s="30"/>
@@ -2496,7 +2514,7 @@
       <c r="G79" s="36"/>
       <c r="H79" s="37"/>
     </row>
-    <row r="80" spans="1:8" ht="39" customHeight="1">
+    <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="29"/>
       <c r="B80" s="30"/>
       <c r="C80" s="30"/>
@@ -2506,7 +2524,7 @@
       <c r="G80" s="36"/>
       <c r="H80" s="37"/>
     </row>
-    <row r="81" spans="1:8" ht="39" customHeight="1">
+    <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="29"/>
       <c r="B81" s="30"/>
       <c r="C81" s="30"/>
@@ -2516,7 +2534,7 @@
       <c r="G81" s="36"/>
       <c r="H81" s="37"/>
     </row>
-    <row r="82" spans="1:8" ht="39" customHeight="1">
+    <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="29"/>
       <c r="B82" s="30"/>
       <c r="C82" s="30"/>
@@ -2526,7 +2544,7 @@
       <c r="G82" s="36"/>
       <c r="H82" s="37"/>
     </row>
-    <row r="83" spans="1:8" ht="39" customHeight="1">
+    <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="29"/>
       <c r="B83" s="30"/>
       <c r="C83" s="30"/>
@@ -2536,7 +2554,7 @@
       <c r="G83" s="36"/>
       <c r="H83" s="37"/>
     </row>
-    <row r="84" spans="1:8" ht="39" customHeight="1">
+    <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="29"/>
       <c r="B84" s="30"/>
       <c r="C84" s="30"/>
@@ -2546,7 +2564,7 @@
       <c r="G84" s="36"/>
       <c r="H84" s="37"/>
     </row>
-    <row r="85" spans="1:8" ht="39" customHeight="1">
+    <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="29"/>
       <c r="B85" s="30"/>
       <c r="C85" s="30"/>
@@ -2556,7 +2574,7 @@
       <c r="G85" s="36"/>
       <c r="H85" s="37"/>
     </row>
-    <row r="86" spans="1:8" ht="39" customHeight="1">
+    <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
       <c r="C86" s="30"/>
@@ -2566,7 +2584,7 @@
       <c r="G86" s="36"/>
       <c r="H86" s="37"/>
     </row>
-    <row r="87" spans="1:8" ht="39" customHeight="1">
+    <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
       <c r="C87" s="30"/>
@@ -2576,7 +2594,7 @@
       <c r="G87" s="36"/>
       <c r="H87" s="37"/>
     </row>
-    <row r="88" spans="1:8" ht="39" customHeight="1">
+    <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="30"/>
@@ -2586,7 +2604,7 @@
       <c r="G88" s="36"/>
       <c r="H88" s="37"/>
     </row>
-    <row r="89" spans="1:8" ht="39" customHeight="1">
+    <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
       <c r="C89" s="30"/>
@@ -2596,7 +2614,7 @@
       <c r="G89" s="36"/>
       <c r="H89" s="37"/>
     </row>
-    <row r="90" spans="1:8" ht="39" customHeight="1">
+    <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="29"/>
       <c r="B90" s="30"/>
       <c r="C90" s="30"/>
@@ -2606,7 +2624,7 @@
       <c r="G90" s="36"/>
       <c r="H90" s="37"/>
     </row>
-    <row r="91" spans="1:8" ht="39" customHeight="1">
+    <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="29"/>
       <c r="B91" s="30"/>
       <c r="C91" s="30"/>
@@ -2616,7 +2634,7 @@
       <c r="G91" s="36"/>
       <c r="H91" s="37"/>
     </row>
-    <row r="92" spans="1:8" ht="39" customHeight="1">
+    <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="29"/>
       <c r="B92" s="30"/>
       <c r="C92" s="30"/>
@@ -2626,7 +2644,7 @@
       <c r="G92" s="36"/>
       <c r="H92" s="37"/>
     </row>
-    <row r="93" spans="1:8" ht="39" customHeight="1">
+    <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="29"/>
       <c r="B93" s="30"/>
       <c r="C93" s="30"/>
@@ -2636,7 +2654,7 @@
       <c r="G93" s="36"/>
       <c r="H93" s="37"/>
     </row>
-    <row r="94" spans="1:8" ht="39" customHeight="1">
+    <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="29"/>
       <c r="B94" s="30"/>
       <c r="C94" s="30"/>
@@ -2646,7 +2664,7 @@
       <c r="G94" s="36"/>
       <c r="H94" s="37"/>
     </row>
-    <row r="95" spans="1:8" ht="39" customHeight="1">
+    <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
       <c r="B95" s="30"/>
       <c r="C95" s="30"/>
@@ -2656,7 +2674,7 @@
       <c r="G95" s="36"/>
       <c r="H95" s="37"/>
     </row>
-    <row r="96" spans="1:8" ht="39" customHeight="1">
+    <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
       <c r="B96" s="30"/>
       <c r="C96" s="30"/>
@@ -2666,7 +2684,7 @@
       <c r="G96" s="36"/>
       <c r="H96" s="37"/>
     </row>
-    <row r="97" spans="1:8" ht="39" customHeight="1">
+    <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
       <c r="B97" s="30"/>
       <c r="C97" s="30"/>
@@ -2676,7 +2694,7 @@
       <c r="G97" s="36"/>
       <c r="H97" s="37"/>
     </row>
-    <row r="98" spans="1:8" ht="39" customHeight="1">
+    <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
       <c r="C98" s="30"/>
@@ -2686,7 +2704,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="37"/>
     </row>
-    <row r="99" spans="1:8" ht="39" customHeight="1">
+    <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="29"/>
       <c r="B99" s="30"/>
       <c r="C99" s="30"/>
@@ -2696,7 +2714,7 @@
       <c r="G99" s="36"/>
       <c r="H99" s="37"/>
     </row>
-    <row r="100" spans="1:8" ht="39" customHeight="1">
+    <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="29"/>
       <c r="B100" s="30"/>
       <c r="C100" s="30"/>
@@ -2706,7 +2724,7 @@
       <c r="G100" s="36"/>
       <c r="H100" s="37"/>
     </row>
-    <row r="101" spans="1:8" ht="39" customHeight="1">
+    <row r="101" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="29"/>
       <c r="B101" s="30"/>
       <c r="C101" s="30"/>
@@ -2716,7 +2734,7 @@
       <c r="G101" s="36"/>
       <c r="H101" s="37"/>
     </row>
-    <row r="102" spans="1:8" ht="39" customHeight="1">
+    <row r="102" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
       <c r="B102" s="30"/>
       <c r="C102" s="30"/>
@@ -2726,7 +2744,7 @@
       <c r="G102" s="36"/>
       <c r="H102" s="37"/>
     </row>
-    <row r="103" spans="1:8" ht="39" customHeight="1">
+    <row r="103" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29"/>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
@@ -2736,7 +2754,7 @@
       <c r="G103" s="36"/>
       <c r="H103" s="37"/>
     </row>
-    <row r="104" spans="1:8" ht="39" customHeight="1">
+    <row r="104" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
       <c r="B104" s="30"/>
       <c r="C104" s="30"/>
@@ -2746,7 +2764,7 @@
       <c r="G104" s="36"/>
       <c r="H104" s="37"/>
     </row>
-    <row r="105" spans="1:8" ht="39" customHeight="1">
+    <row r="105" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
       <c r="B105" s="30"/>
       <c r="C105" s="30"/>
@@ -2756,7 +2774,7 @@
       <c r="G105" s="36"/>
       <c r="H105" s="37"/>
     </row>
-    <row r="106" spans="1:8" ht="39" customHeight="1">
+    <row r="106" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
       <c r="B106" s="30"/>
       <c r="C106" s="30"/>
@@ -2766,7 +2784,7 @@
       <c r="G106" s="36"/>
       <c r="H106" s="37"/>
     </row>
-    <row r="107" spans="1:8" ht="39" customHeight="1">
+    <row r="107" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="29"/>
       <c r="B107" s="30"/>
       <c r="C107" s="30"/>
@@ -2776,7 +2794,7 @@
       <c r="G107" s="36"/>
       <c r="H107" s="37"/>
     </row>
-    <row r="108" spans="1:8" ht="39" customHeight="1">
+    <row r="108" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="29"/>
       <c r="B108" s="30"/>
       <c r="C108" s="30"/>
@@ -2786,7 +2804,7 @@
       <c r="G108" s="36"/>
       <c r="H108" s="37"/>
     </row>
-    <row r="109" spans="1:8" ht="39" customHeight="1">
+    <row r="109" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="29"/>
       <c r="B109" s="30"/>
       <c r="C109" s="30"/>
@@ -2796,7 +2814,7 @@
       <c r="G109" s="36"/>
       <c r="H109" s="37"/>
     </row>
-    <row r="110" spans="1:8" ht="39" customHeight="1">
+    <row r="110" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="29"/>
       <c r="B110" s="30"/>
       <c r="C110" s="30"/>
@@ -2806,7 +2824,7 @@
       <c r="G110" s="36"/>
       <c r="H110" s="37"/>
     </row>
-    <row r="111" spans="1:8" ht="39" customHeight="1">
+    <row r="111" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="29"/>
       <c r="B111" s="30"/>
       <c r="C111" s="30"/>
@@ -2816,7 +2834,7 @@
       <c r="G111" s="36"/>
       <c r="H111" s="37"/>
     </row>
-    <row r="112" spans="1:8" ht="39" customHeight="1">
+    <row r="112" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="29"/>
       <c r="B112" s="30"/>
       <c r="C112" s="30"/>
@@ -2826,7 +2844,7 @@
       <c r="G112" s="36"/>
       <c r="H112" s="37"/>
     </row>
-    <row r="113" spans="1:8" ht="39" customHeight="1">
+    <row r="113" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="29"/>
       <c r="B113" s="30"/>
       <c r="C113" s="30"/>
@@ -2836,7 +2854,7 @@
       <c r="G113" s="36"/>
       <c r="H113" s="37"/>
     </row>
-    <row r="114" spans="1:8" ht="39" customHeight="1">
+    <row r="114" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="29"/>
       <c r="B114" s="30"/>
       <c r="C114" s="30"/>
@@ -2846,7 +2864,7 @@
       <c r="G114" s="36"/>
       <c r="H114" s="37"/>
     </row>
-    <row r="115" spans="1:8" ht="39" customHeight="1">
+    <row r="115" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="29"/>
       <c r="B115" s="30"/>
       <c r="C115" s="30"/>
@@ -2856,7 +2874,7 @@
       <c r="G115" s="36"/>
       <c r="H115" s="37"/>
     </row>
-    <row r="116" spans="1:8" ht="39" customHeight="1">
+    <row r="116" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="29"/>
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
@@ -2866,7 +2884,7 @@
       <c r="G116" s="36"/>
       <c r="H116" s="37"/>
     </row>
-    <row r="117" spans="1:8" ht="39" customHeight="1">
+    <row r="117" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="29"/>
       <c r="B117" s="30"/>
       <c r="C117" s="30"/>
@@ -2876,7 +2894,7 @@
       <c r="G117" s="36"/>
       <c r="H117" s="37"/>
     </row>
-    <row r="118" spans="1:8" ht="39" customHeight="1">
+    <row r="118" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="29"/>
       <c r="B118" s="30"/>
       <c r="C118" s="30"/>
@@ -2886,7 +2904,7 @@
       <c r="G118" s="36"/>
       <c r="H118" s="37"/>
     </row>
-    <row r="119" spans="1:8" ht="39" customHeight="1">
+    <row r="119" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="29"/>
       <c r="B119" s="30"/>
       <c r="C119" s="30"/>
@@ -2896,7 +2914,7 @@
       <c r="G119" s="36"/>
       <c r="H119" s="37"/>
     </row>
-    <row r="120" spans="1:8" ht="39" customHeight="1">
+    <row r="120" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="29"/>
       <c r="B120" s="30"/>
       <c r="C120" s="30"/>
@@ -2906,7 +2924,7 @@
       <c r="G120" s="36"/>
       <c r="H120" s="37"/>
     </row>
-    <row r="121" spans="1:8" ht="39" customHeight="1">
+    <row r="121" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="29"/>
       <c r="B121" s="30"/>
       <c r="C121" s="30"/>
@@ -2916,7 +2934,7 @@
       <c r="G121" s="36"/>
       <c r="H121" s="37"/>
     </row>
-    <row r="122" spans="1:8" ht="39" customHeight="1">
+    <row r="122" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="29"/>
       <c r="B122" s="30"/>
       <c r="C122" s="30"/>
@@ -2926,7 +2944,7 @@
       <c r="G122" s="36"/>
       <c r="H122" s="37"/>
     </row>
-    <row r="123" spans="1:8" ht="39" customHeight="1">
+    <row r="123" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="29"/>
       <c r="B123" s="30"/>
       <c r="C123" s="30"/>
@@ -2936,7 +2954,7 @@
       <c r="G123" s="36"/>
       <c r="H123" s="37"/>
     </row>
-    <row r="124" spans="1:8" ht="39" customHeight="1">
+    <row r="124" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="29"/>
       <c r="B124" s="30"/>
       <c r="C124" s="30"/>
@@ -2946,7 +2964,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="37"/>
     </row>
-    <row r="125" spans="1:8" ht="39" customHeight="1">
+    <row r="125" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="29"/>
       <c r="B125" s="30"/>
       <c r="C125" s="30"/>
@@ -2956,7 +2974,7 @@
       <c r="G125" s="36"/>
       <c r="H125" s="37"/>
     </row>
-    <row r="126" spans="1:8" ht="39" customHeight="1">
+    <row r="126" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="29"/>
       <c r="B126" s="30"/>
       <c r="C126" s="30"/>
@@ -2966,7 +2984,7 @@
       <c r="G126" s="36"/>
       <c r="H126" s="37"/>
     </row>
-    <row r="127" spans="1:8" ht="39" customHeight="1">
+    <row r="127" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="29"/>
       <c r="B127" s="30"/>
       <c r="C127" s="30"/>
@@ -2976,7 +2994,7 @@
       <c r="G127" s="36"/>
       <c r="H127" s="37"/>
     </row>
-    <row r="128" spans="1:8" ht="39" customHeight="1">
+    <row r="128" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="29"/>
       <c r="B128" s="30"/>
       <c r="C128" s="30"/>
@@ -2986,7 +3004,7 @@
       <c r="G128" s="36"/>
       <c r="H128" s="37"/>
     </row>
-    <row r="129" spans="1:8" ht="39" customHeight="1">
+    <row r="129" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="29"/>
       <c r="B129" s="30"/>
       <c r="C129" s="30"/>
@@ -2996,7 +3014,7 @@
       <c r="G129" s="36"/>
       <c r="H129" s="37"/>
     </row>
-    <row r="130" spans="1:8" ht="39" customHeight="1">
+    <row r="130" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
       <c r="B130" s="30"/>
       <c r="C130" s="30"/>
@@ -3006,7 +3024,7 @@
       <c r="G130" s="36"/>
       <c r="H130" s="37"/>
     </row>
-    <row r="131" spans="1:8" ht="39" customHeight="1">
+    <row r="131" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
       <c r="B131" s="30"/>
       <c r="C131" s="30"/>
@@ -3016,7 +3034,7 @@
       <c r="G131" s="36"/>
       <c r="H131" s="37"/>
     </row>
-    <row r="132" spans="1:8" ht="39" customHeight="1">
+    <row r="132" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
       <c r="B132" s="30"/>
       <c r="C132" s="30"/>
@@ -3026,7 +3044,7 @@
       <c r="G132" s="36"/>
       <c r="H132" s="37"/>
     </row>
-    <row r="133" spans="1:8" ht="39" customHeight="1">
+    <row r="133" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="29"/>
       <c r="B133" s="30"/>
       <c r="C133" s="30"/>
@@ -3036,7 +3054,7 @@
       <c r="G133" s="36"/>
       <c r="H133" s="37"/>
     </row>
-    <row r="134" spans="1:8" ht="39" customHeight="1">
+    <row r="134" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="29"/>
       <c r="B134" s="30"/>
       <c r="C134" s="30"/>
@@ -3046,7 +3064,7 @@
       <c r="G134" s="36"/>
       <c r="H134" s="37"/>
     </row>
-    <row r="135" spans="1:8" ht="39" customHeight="1">
+    <row r="135" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="29"/>
       <c r="B135" s="30"/>
       <c r="C135" s="30"/>
@@ -3056,7 +3074,7 @@
       <c r="G135" s="36"/>
       <c r="H135" s="37"/>
     </row>
-    <row r="136" spans="1:8" ht="39" customHeight="1">
+    <row r="136" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="29"/>
       <c r="B136" s="30"/>
       <c r="C136" s="30"/>
@@ -3066,7 +3084,7 @@
       <c r="G136" s="36"/>
       <c r="H136" s="37"/>
     </row>
-    <row r="137" spans="1:8" ht="39" customHeight="1">
+    <row r="137" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
       <c r="B137" s="30"/>
       <c r="C137" s="30"/>
@@ -3076,7 +3094,7 @@
       <c r="G137" s="36"/>
       <c r="H137" s="37"/>
     </row>
-    <row r="138" spans="1:8" ht="39" customHeight="1">
+    <row r="138" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
       <c r="B138" s="30"/>
       <c r="C138" s="30"/>
@@ -3086,7 +3104,7 @@
       <c r="G138" s="36"/>
       <c r="H138" s="37"/>
     </row>
-    <row r="139" spans="1:8" ht="39" customHeight="1">
+    <row r="139" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
       <c r="B139" s="30"/>
       <c r="C139" s="30"/>
@@ -3096,7 +3114,7 @@
       <c r="G139" s="36"/>
       <c r="H139" s="37"/>
     </row>
-    <row r="140" spans="1:8" ht="39" customHeight="1">
+    <row r="140" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="29"/>
       <c r="B140" s="30"/>
       <c r="C140" s="30"/>
@@ -3106,7 +3124,7 @@
       <c r="G140" s="36"/>
       <c r="H140" s="37"/>
     </row>
-    <row r="141" spans="1:8" ht="39" customHeight="1">
+    <row r="141" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="29"/>
       <c r="B141" s="30"/>
       <c r="C141" s="30"/>
@@ -3116,7 +3134,7 @@
       <c r="G141" s="36"/>
       <c r="H141" s="37"/>
     </row>
-    <row r="142" spans="1:8" ht="39" customHeight="1">
+    <row r="142" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="29"/>
       <c r="B142" s="30"/>
       <c r="C142" s="30"/>
@@ -3126,7 +3144,7 @@
       <c r="G142" s="36"/>
       <c r="H142" s="37"/>
     </row>
-    <row r="143" spans="1:8" ht="39" customHeight="1">
+    <row r="143" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
       <c r="B143" s="30"/>
       <c r="C143" s="30"/>
@@ -3136,7 +3154,7 @@
       <c r="G143" s="36"/>
       <c r="H143" s="37"/>
     </row>
-    <row r="144" spans="1:8" ht="39" customHeight="1">
+    <row r="144" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
       <c r="B144" s="30"/>
       <c r="C144" s="30"/>
@@ -3146,7 +3164,7 @@
       <c r="G144" s="36"/>
       <c r="H144" s="37"/>
     </row>
-    <row r="145" spans="1:8" ht="39" customHeight="1">
+    <row r="145" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
       <c r="B145" s="30"/>
       <c r="C145" s="30"/>
@@ -3156,7 +3174,7 @@
       <c r="G145" s="36"/>
       <c r="H145" s="37"/>
     </row>
-    <row r="146" spans="1:8" ht="39" customHeight="1">
+    <row r="146" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="29"/>
       <c r="B146" s="30"/>
       <c r="C146" s="30"/>
@@ -3166,7 +3184,7 @@
       <c r="G146" s="36"/>
       <c r="H146" s="37"/>
     </row>
-    <row r="147" spans="1:8" ht="39" customHeight="1">
+    <row r="147" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
       <c r="B147" s="30"/>
       <c r="C147" s="30"/>
@@ -3176,7 +3194,7 @@
       <c r="G147" s="36"/>
       <c r="H147" s="37"/>
     </row>
-    <row r="148" spans="1:8" ht="39" customHeight="1">
+    <row r="148" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
       <c r="B148" s="30"/>
       <c r="C148" s="30"/>
@@ -3186,7 +3204,7 @@
       <c r="G148" s="36"/>
       <c r="H148" s="37"/>
     </row>
-    <row r="149" spans="1:8" ht="39" customHeight="1">
+    <row r="149" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
       <c r="B149" s="30"/>
       <c r="C149" s="30"/>
@@ -3196,7 +3214,7 @@
       <c r="G149" s="36"/>
       <c r="H149" s="37"/>
     </row>
-    <row r="150" spans="1:8" ht="39" customHeight="1">
+    <row r="150" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
       <c r="B150" s="30"/>
       <c r="C150" s="30"/>
@@ -3206,7 +3224,7 @@
       <c r="G150" s="36"/>
       <c r="H150" s="37"/>
     </row>
-    <row r="151" spans="1:8" ht="39" customHeight="1">
+    <row r="151" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
       <c r="B151" s="30"/>
       <c r="C151" s="30"/>
@@ -3216,7 +3234,7 @@
       <c r="G151" s="36"/>
       <c r="H151" s="37"/>
     </row>
-    <row r="152" spans="1:8" ht="39" customHeight="1">
+    <row r="152" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="29"/>
       <c r="B152" s="30"/>
       <c r="C152" s="30"/>
@@ -3226,7 +3244,7 @@
       <c r="G152" s="36"/>
       <c r="H152" s="37"/>
     </row>
-    <row r="153" spans="1:8" ht="39" customHeight="1">
+    <row r="153" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="29"/>
       <c r="B153" s="30"/>
       <c r="C153" s="30"/>
@@ -3236,7 +3254,7 @@
       <c r="G153" s="36"/>
       <c r="H153" s="37"/>
     </row>
-    <row r="154" spans="1:8" ht="39" customHeight="1">
+    <row r="154" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="29"/>
       <c r="B154" s="30"/>
       <c r="C154" s="30"/>
@@ -3246,7 +3264,7 @@
       <c r="G154" s="36"/>
       <c r="H154" s="37"/>
     </row>
-    <row r="155" spans="1:8" ht="39" customHeight="1">
+    <row r="155" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="29"/>
       <c r="B155" s="30"/>
       <c r="C155" s="30"/>
@@ -3256,7 +3274,7 @@
       <c r="G155" s="36"/>
       <c r="H155" s="37"/>
     </row>
-    <row r="156" spans="1:8" ht="39" customHeight="1">
+    <row r="156" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="29"/>
       <c r="B156" s="30"/>
       <c r="C156" s="30"/>
@@ -3266,7 +3284,7 @@
       <c r="G156" s="36"/>
       <c r="H156" s="37"/>
     </row>
-    <row r="157" spans="1:8" ht="39" customHeight="1">
+    <row r="157" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
       <c r="B157" s="30"/>
       <c r="C157" s="30"/>
@@ -3276,7 +3294,7 @@
       <c r="G157" s="36"/>
       <c r="H157" s="37"/>
     </row>
-    <row r="158" spans="1:8" ht="39" customHeight="1">
+    <row r="158" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="29"/>
       <c r="B158" s="30"/>
       <c r="C158" s="30"/>
@@ -3286,7 +3304,7 @@
       <c r="G158" s="36"/>
       <c r="H158" s="37"/>
     </row>
-    <row r="159" spans="1:8" ht="39" customHeight="1">
+    <row r="159" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="29"/>
       <c r="B159" s="30"/>
       <c r="C159" s="30"/>
@@ -3296,7 +3314,7 @@
       <c r="G159" s="36"/>
       <c r="H159" s="37"/>
     </row>
-    <row r="160" spans="1:8" ht="39" customHeight="1">
+    <row r="160" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="29"/>
       <c r="B160" s="30"/>
       <c r="C160" s="30"/>
@@ -3306,7 +3324,7 @@
       <c r="G160" s="36"/>
       <c r="H160" s="37"/>
     </row>
-    <row r="161" spans="1:8" ht="39" customHeight="1">
+    <row r="161" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="29"/>
       <c r="B161" s="30"/>
       <c r="C161" s="30"/>
@@ -3316,7 +3334,7 @@
       <c r="G161" s="36"/>
       <c r="H161" s="37"/>
     </row>
-    <row r="162" spans="1:8" ht="39" customHeight="1">
+    <row r="162" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
       <c r="B162" s="30"/>
       <c r="C162" s="30"/>
@@ -3326,7 +3344,7 @@
       <c r="G162" s="36"/>
       <c r="H162" s="37"/>
     </row>
-    <row r="163" spans="1:8" ht="39" customHeight="1">
+    <row r="163" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
       <c r="B163" s="30"/>
       <c r="C163" s="30"/>
@@ -3336,7 +3354,7 @@
       <c r="G163" s="36"/>
       <c r="H163" s="37"/>
     </row>
-    <row r="164" spans="1:8" ht="39" customHeight="1">
+    <row r="164" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
       <c r="B164" s="30"/>
       <c r="C164" s="30"/>
@@ -3346,7 +3364,7 @@
       <c r="G164" s="36"/>
       <c r="H164" s="37"/>
     </row>
-    <row r="165" spans="1:8" ht="39" customHeight="1">
+    <row r="165" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
       <c r="B165" s="30"/>
       <c r="C165" s="30"/>
@@ -3356,7 +3374,7 @@
       <c r="G165" s="36"/>
       <c r="H165" s="37"/>
     </row>
-    <row r="166" spans="1:8" ht="39" customHeight="1">
+    <row r="166" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="29"/>
       <c r="B166" s="30"/>
       <c r="C166" s="30"/>
@@ -3366,7 +3384,7 @@
       <c r="G166" s="36"/>
       <c r="H166" s="37"/>
     </row>
-    <row r="167" spans="1:8" ht="39" customHeight="1">
+    <row r="167" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="29"/>
       <c r="B167" s="30"/>
       <c r="C167" s="30"/>
@@ -3376,7 +3394,7 @@
       <c r="G167" s="36"/>
       <c r="H167" s="37"/>
     </row>
-    <row r="168" spans="1:8" ht="39" customHeight="1">
+    <row r="168" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="29"/>
       <c r="B168" s="30"/>
       <c r="C168" s="30"/>
@@ -3386,7 +3404,7 @@
       <c r="G168" s="36"/>
       <c r="H168" s="37"/>
     </row>
-    <row r="169" spans="1:8" ht="39" customHeight="1">
+    <row r="169" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="29"/>
       <c r="B169" s="30"/>
       <c r="C169" s="30"/>
@@ -3396,7 +3414,7 @@
       <c r="G169" s="36"/>
       <c r="H169" s="37"/>
     </row>
-    <row r="170" spans="1:8" ht="39" customHeight="1">
+    <row r="170" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="29"/>
       <c r="B170" s="30"/>
       <c r="C170" s="30"/>
@@ -3406,7 +3424,7 @@
       <c r="G170" s="36"/>
       <c r="H170" s="37"/>
     </row>
-    <row r="171" spans="1:8" ht="39" customHeight="1">
+    <row r="171" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="29"/>
       <c r="B171" s="30"/>
       <c r="C171" s="30"/>
@@ -3416,7 +3434,7 @@
       <c r="G171" s="36"/>
       <c r="H171" s="37"/>
     </row>
-    <row r="172" spans="1:8" ht="39" customHeight="1">
+    <row r="172" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="29"/>
       <c r="B172" s="30"/>
       <c r="C172" s="30"/>
@@ -3426,7 +3444,7 @@
       <c r="G172" s="36"/>
       <c r="H172" s="37"/>
     </row>
-    <row r="173" spans="1:8" ht="39" customHeight="1">
+    <row r="173" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="29"/>
       <c r="B173" s="30"/>
       <c r="C173" s="30"/>
@@ -3436,7 +3454,7 @@
       <c r="G173" s="36"/>
       <c r="H173" s="37"/>
     </row>
-    <row r="174" spans="1:8" ht="39" customHeight="1">
+    <row r="174" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="29"/>
       <c r="B174" s="30"/>
       <c r="C174" s="30"/>
@@ -3446,7 +3464,7 @@
       <c r="G174" s="36"/>
       <c r="H174" s="37"/>
     </row>
-    <row r="175" spans="1:8" ht="39" customHeight="1">
+    <row r="175" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="29"/>
       <c r="B175" s="30"/>
       <c r="C175" s="30"/>
@@ -3456,7 +3474,7 @@
       <c r="G175" s="36"/>
       <c r="H175" s="37"/>
     </row>
-    <row r="176" spans="1:8" ht="39" customHeight="1">
+    <row r="176" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="29"/>
       <c r="B176" s="30"/>
       <c r="C176" s="30"/>
@@ -3466,7 +3484,7 @@
       <c r="G176" s="36"/>
       <c r="H176" s="37"/>
     </row>
-    <row r="177" spans="1:8" ht="39" customHeight="1">
+    <row r="177" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
       <c r="B177" s="30"/>
       <c r="C177" s="30"/>
@@ -3476,7 +3494,7 @@
       <c r="G177" s="36"/>
       <c r="H177" s="37"/>
     </row>
-    <row r="178" spans="1:8" ht="39" customHeight="1">
+    <row r="178" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
       <c r="B178" s="30"/>
       <c r="C178" s="30"/>
@@ -3486,7 +3504,7 @@
       <c r="G178" s="36"/>
       <c r="H178" s="37"/>
     </row>
-    <row r="179" spans="1:8" ht="39" customHeight="1">
+    <row r="179" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
       <c r="B179" s="30"/>
       <c r="C179" s="30"/>
@@ -3496,7 +3514,7 @@
       <c r="G179" s="36"/>
       <c r="H179" s="37"/>
     </row>
-    <row r="180" spans="1:8" ht="39" customHeight="1">
+    <row r="180" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="29"/>
       <c r="B180" s="30"/>
       <c r="C180" s="30"/>
@@ -3506,7 +3524,7 @@
       <c r="G180" s="36"/>
       <c r="H180" s="37"/>
     </row>
-    <row r="181" spans="1:8" ht="39" customHeight="1">
+    <row r="181" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="29"/>
       <c r="B181" s="30"/>
       <c r="C181" s="30"/>
@@ -3516,7 +3534,7 @@
       <c r="G181" s="36"/>
       <c r="H181" s="37"/>
     </row>
-    <row r="182" spans="1:8" ht="39" customHeight="1">
+    <row r="182" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="29"/>
       <c r="B182" s="30"/>
       <c r="C182" s="30"/>
@@ -3526,7 +3544,7 @@
       <c r="G182" s="36"/>
       <c r="H182" s="37"/>
     </row>
-    <row r="183" spans="1:8" ht="39" customHeight="1">
+    <row r="183" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
       <c r="B183" s="30"/>
       <c r="C183" s="30"/>
@@ -3536,7 +3554,7 @@
       <c r="G183" s="36"/>
       <c r="H183" s="37"/>
     </row>
-    <row r="184" spans="1:8" ht="39" customHeight="1">
+    <row r="184" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
       <c r="B184" s="30"/>
       <c r="C184" s="30"/>
@@ -3546,7 +3564,7 @@
       <c r="G184" s="36"/>
       <c r="H184" s="37"/>
     </row>
-    <row r="185" spans="1:8" ht="39" customHeight="1">
+    <row r="185" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
       <c r="B185" s="30"/>
       <c r="C185" s="30"/>
@@ -3556,7 +3574,7 @@
       <c r="G185" s="36"/>
       <c r="H185" s="37"/>
     </row>
-    <row r="186" spans="1:8" ht="39" customHeight="1">
+    <row r="186" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="29"/>
       <c r="B186" s="30"/>
       <c r="C186" s="30"/>
@@ -3566,7 +3584,7 @@
       <c r="G186" s="36"/>
       <c r="H186" s="37"/>
     </row>
-    <row r="187" spans="1:8" ht="39" customHeight="1">
+    <row r="187" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="29"/>
       <c r="B187" s="30"/>
       <c r="C187" s="30"/>
@@ -3576,7 +3594,7 @@
       <c r="G187" s="36"/>
       <c r="H187" s="37"/>
     </row>
-    <row r="188" spans="1:8" ht="39" customHeight="1">
+    <row r="188" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="29"/>
       <c r="B188" s="30"/>
       <c r="C188" s="30"/>
@@ -3586,7 +3604,7 @@
       <c r="G188" s="36"/>
       <c r="H188" s="37"/>
     </row>
-    <row r="189" spans="1:8" ht="39" customHeight="1">
+    <row r="189" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="29"/>
       <c r="B189" s="30"/>
       <c r="C189" s="30"/>
@@ -3596,7 +3614,7 @@
       <c r="G189" s="36"/>
       <c r="H189" s="37"/>
     </row>
-    <row r="190" spans="1:8" ht="39" customHeight="1">
+    <row r="190" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="29"/>
       <c r="B190" s="30"/>
       <c r="C190" s="30"/>
@@ -3606,7 +3624,7 @@
       <c r="G190" s="36"/>
       <c r="H190" s="37"/>
     </row>
-    <row r="191" spans="1:8" ht="39" customHeight="1">
+    <row r="191" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="29"/>
       <c r="B191" s="30"/>
       <c r="C191" s="30"/>
@@ -3616,7 +3634,7 @@
       <c r="G191" s="36"/>
       <c r="H191" s="37"/>
     </row>
-    <row r="192" spans="1:8" ht="39" customHeight="1">
+    <row r="192" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="29"/>
       <c r="B192" s="30"/>
       <c r="C192" s="30"/>
@@ -3626,7 +3644,7 @@
       <c r="G192" s="36"/>
       <c r="H192" s="37"/>
     </row>
-    <row r="193" spans="1:8" ht="39" customHeight="1">
+    <row r="193" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="29"/>
       <c r="B193" s="30"/>
       <c r="C193" s="30"/>
@@ -3636,7 +3654,7 @@
       <c r="G193" s="36"/>
       <c r="H193" s="37"/>
     </row>
-    <row r="194" spans="1:8" ht="39" customHeight="1">
+    <row r="194" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="29"/>
       <c r="B194" s="30"/>
       <c r="C194" s="30"/>
@@ -3646,7 +3664,7 @@
       <c r="G194" s="36"/>
       <c r="H194" s="37"/>
     </row>
-    <row r="195" spans="1:8" ht="39" customHeight="1">
+    <row r="195" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="29"/>
       <c r="B195" s="30"/>
       <c r="C195" s="30"/>
@@ -3656,7 +3674,7 @@
       <c r="G195" s="36"/>
       <c r="H195" s="37"/>
     </row>
-    <row r="196" spans="1:8" ht="39" customHeight="1">
+    <row r="196" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="29"/>
       <c r="B196" s="30"/>
       <c r="C196" s="30"/>
@@ -3666,7 +3684,7 @@
       <c r="G196" s="36"/>
       <c r="H196" s="37"/>
     </row>
-    <row r="197" spans="1:8" ht="39" customHeight="1">
+    <row r="197" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="29"/>
       <c r="B197" s="30"/>
       <c r="C197" s="30"/>
@@ -3676,7 +3694,7 @@
       <c r="G197" s="36"/>
       <c r="H197" s="37"/>
     </row>
-    <row r="198" spans="1:8" ht="39" customHeight="1">
+    <row r="198" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="29"/>
       <c r="B198" s="30"/>
       <c r="C198" s="30"/>
@@ -3686,7 +3704,7 @@
       <c r="G198" s="36"/>
       <c r="H198" s="37"/>
     </row>
-    <row r="199" spans="1:8" ht="39" customHeight="1">
+    <row r="199" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="29"/>
       <c r="B199" s="30"/>
       <c r="C199" s="30"/>
@@ -3696,7 +3714,7 @@
       <c r="G199" s="36"/>
       <c r="H199" s="37"/>
     </row>
-    <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1">
+    <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="32"/>
       <c r="B200" s="33"/>
       <c r="C200" s="33"/>
@@ -3706,7 +3724,7 @@
       <c r="G200" s="39"/>
       <c r="H200" s="40"/>
     </row>
-    <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1"/>
+    <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="204">
     <mergeCell ref="F6:H6"/>
@@ -3916,7 +3934,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -3929,19 +3947,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="21.875" style="14" customWidth="1"/>
     <col min="2" max="4" width="15" style="14" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="14" customWidth="1"/>
     <col min="6" max="16384" width="15" style="14" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1">
+    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -3952,7 +3970,7 @@
       <c r="D1" s="62"/>
       <c r="E1" s="63"/>
     </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1">
+    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
@@ -3963,7 +3981,7 @@
       <c r="D2" s="64"/>
       <c r="E2" s="65"/>
     </row>
-    <row r="3" spans="1:5" ht="136" customHeight="1">
+    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -3972,7 +3990,7 @@
       <c r="D3" s="66"/>
       <c r="E3" s="67"/>
     </row>
-    <row r="4" spans="1:5" ht="46" customHeight="1">
+    <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -3981,7 +3999,7 @@
       <c r="D4" s="71"/>
       <c r="E4" s="72"/>
     </row>
-    <row r="5" spans="1:5" ht="46" customHeight="1">
+    <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
@@ -3990,7 +4008,7 @@
       <c r="D5" s="66"/>
       <c r="E5" s="67"/>
     </row>
-    <row r="6" spans="1:5" ht="46" customHeight="1">
+    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -3999,16 +4017,16 @@
       <c r="D6" s="66"/>
       <c r="E6" s="67"/>
     </row>
-    <row r="7" spans="1:5" ht="46" customHeight="1">
+    <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B7" s="70"/>
       <c r="C7" s="71"/>
       <c r="D7" s="71"/>
       <c r="E7" s="72"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1">
+    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>30</v>
       </c>
@@ -4030,7 +4048,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -4047,15 +4065,15 @@
       <selection activeCell="B15" sqref="B15:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>23</v>
       </c>
@@ -4066,7 +4084,7 @@
       <c r="F1" s="74"/>
       <c r="G1" s="75"/>
     </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1">
+    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
@@ -4077,7 +4095,7 @@
       <c r="F2" s="76"/>
       <c r="G2" s="77"/>
     </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1">
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
@@ -4088,7 +4106,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="77"/>
     </row>
-    <row r="4" spans="1:7" ht="112" customHeight="1">
+    <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -4099,7 +4117,7 @@
       <c r="F4" s="76"/>
       <c r="G4" s="77"/>
     </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1">
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>26</v>
       </c>
@@ -4110,8 +4128,8 @@
       <c r="F5" s="78"/>
       <c r="G5" s="79"/>
     </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
-    <row r="7" spans="1:7" ht="36" customHeight="1">
+    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="73" t="s">
         <v>27</v>
       </c>
@@ -4122,7 +4140,7 @@
       <c r="F7" s="74"/>
       <c r="G7" s="75"/>
     </row>
-    <row r="8" spans="1:7" ht="36" customHeight="1">
+    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -4133,7 +4151,7 @@
       <c r="F8" s="66"/>
       <c r="G8" s="67"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1">
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
@@ -4144,7 +4162,7 @@
       <c r="F9" s="66"/>
       <c r="G9" s="67"/>
     </row>
-    <row r="10" spans="1:7" ht="112" customHeight="1">
+    <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
@@ -4155,7 +4173,7 @@
       <c r="F10" s="66"/>
       <c r="G10" s="67"/>
     </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1">
+    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -4166,9 +4184,9 @@
       <c r="F11" s="68"/>
       <c r="G11" s="69"/>
     </row>
-    <row r="12" spans="1:7" ht="36" customHeight="1"/>
-    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
-    <row r="14" spans="1:7" ht="36" customHeight="1">
+    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="73" t="s">
         <v>28</v>
       </c>
@@ -4179,7 +4197,7 @@
       <c r="F14" s="74"/>
       <c r="G14" s="75"/>
     </row>
-    <row r="15" spans="1:7" ht="36" customHeight="1">
+    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
@@ -4190,7 +4208,7 @@
       <c r="F15" s="66"/>
       <c r="G15" s="67"/>
     </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1">
+    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
@@ -4201,7 +4219,7 @@
       <c r="F16" s="66"/>
       <c r="G16" s="67"/>
     </row>
-    <row r="17" spans="1:7" ht="113" customHeight="1">
+    <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>6</v>
       </c>
@@ -4212,7 +4230,7 @@
       <c r="F17" s="66"/>
       <c r="G17" s="67"/>
     </row>
-    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1">
+    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>26</v>
       </c>
@@ -4223,8 +4241,8 @@
       <c r="F18" s="68"/>
       <c r="G18" s="69"/>
     </row>
-    <row r="19" spans="1:7" ht="36" customHeight="1"/>
-    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
+    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A1:G1"/>
@@ -4245,7 +4263,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Minor mods to a few files
</commit_message>
<xml_diff>
--- a/EMX_3.xlsx
+++ b/EMX_3.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\GitHub\docubase\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1180" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -285,6 +280,9 @@
   </si>
   <si>
     <t>13d20027</t>
+  </si>
+  <si>
+    <t>Burr hole injection</t>
   </si>
 </sst>
 </file>
@@ -847,7 +845,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -951,6 +949,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -960,6 +967,60 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -969,69 +1030,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1073,18 +1071,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1439,14 +1425,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="62.375" style="28" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" style="28" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1440,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="38" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
@@ -1462,13 +1448,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="38" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="38" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1476,7 +1462,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="38" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1470,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
@@ -1492,19 +1478,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="38" customHeight="1" thickTop="1"/>
+    <row r="8" spans="1:2" ht="38" customHeight="1"/>
+    <row r="9" spans="1:2" ht="38" customHeight="1"/>
+    <row r="10" spans="1:2" ht="38" customHeight="1"/>
+    <row r="11" spans="1:2" ht="38" customHeight="1"/>
+    <row r="12" spans="1:2" ht="38" customHeight="1"/>
+    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1">
       <c r="A13" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1517,34 +1503,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A30" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="18" customWidth="1"/>
     <col min="6" max="6" width="34.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="8.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1">
+      <c r="A1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="59" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
       <c r="G1" s="21" t="s">
         <v>31</v>
       </c>
@@ -1552,17 +1538,17 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:8" ht="39" customHeight="1">
+      <c r="A2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="22" t="s">
         <v>31</v>
       </c>
@@ -1570,45 +1556,45 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+    <row r="3" spans="1:8" ht="39" customHeight="1">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48"/>
-    </row>
-    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+    </row>
+    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
-    </row>
-    <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-    </row>
-    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
+    </row>
+    <row r="5" spans="1:8" ht="26" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+    </row>
+    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1624,13 +1610,13 @@
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
-    </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" ht="39" customHeight="1">
       <c r="A7" s="29">
         <v>1</v>
       </c>
@@ -1640,13 +1626,13 @@
       <c r="C7" s="30"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="39"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:8" ht="39" customHeight="1">
       <c r="A8" s="29">
         <v>1</v>
       </c>
@@ -1658,13 +1644,13 @@
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-    </row>
-    <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:8" ht="39" customHeight="1">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1676,13 +1662,13 @@
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:8" ht="39" customHeight="1">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -1694,13 +1680,13 @@
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" ht="39" customHeight="1">
       <c r="A11" s="29">
         <v>1</v>
       </c>
@@ -1712,13 +1698,13 @@
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
-    </row>
-    <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
+    </row>
+    <row r="12" spans="1:8" ht="39" customHeight="1">
       <c r="A12" s="29">
         <v>1</v>
       </c>
@@ -1730,13 +1716,13 @@
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
-    </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
+    </row>
+    <row r="13" spans="1:8" ht="39" customHeight="1">
       <c r="A13" s="29">
         <v>1</v>
       </c>
@@ -1746,13 +1732,13 @@
       <c r="C13" s="30"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
-    </row>
-    <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
+    </row>
+    <row r="14" spans="1:8" ht="39" customHeight="1">
       <c r="A14" s="29">
         <v>1</v>
       </c>
@@ -1762,11 +1748,11 @@
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
+    </row>
+    <row r="15" spans="1:8" ht="39" customHeight="1">
       <c r="A15" s="29">
         <v>1</v>
       </c>
@@ -1776,11 +1762,11 @@
       <c r="C15" s="30"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="40"/>
+    </row>
+    <row r="16" spans="1:8" ht="39" customHeight="1">
       <c r="A16" s="29">
         <v>1</v>
       </c>
@@ -1790,11 +1776,11 @@
       <c r="C16" s="30"/>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-    </row>
-    <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
+    </row>
+    <row r="17" spans="1:8" ht="39" customHeight="1">
       <c r="A17" s="29">
         <v>1</v>
       </c>
@@ -1804,11 +1790,11 @@
       <c r="C17" s="30"/>
       <c r="D17" s="31"/>
       <c r="E17" s="31"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
+    </row>
+    <row r="18" spans="1:8" ht="39" customHeight="1">
       <c r="A18" s="29">
         <v>1</v>
       </c>
@@ -1818,11 +1804,11 @@
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
-    </row>
-    <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
+    </row>
+    <row r="19" spans="1:8" ht="39" customHeight="1">
       <c r="A19" s="29">
         <v>1</v>
       </c>
@@ -1834,13 +1820,13 @@
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
-    </row>
-    <row r="20" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" ht="39" customHeight="1">
       <c r="A20" s="29">
         <v>1</v>
       </c>
@@ -1850,13 +1836,13 @@
       <c r="C20" s="30"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
-    </row>
-    <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="39"/>
+      <c r="H20" s="40"/>
+    </row>
+    <row r="21" spans="1:8" ht="39" customHeight="1">
       <c r="A21" s="29">
         <v>1</v>
       </c>
@@ -1866,13 +1852,13 @@
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="37"/>
-    </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
+    </row>
+    <row r="22" spans="1:8" ht="39" customHeight="1">
       <c r="A22" s="29">
         <v>1</v>
       </c>
@@ -1882,11 +1868,11 @@
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
-    </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="40"/>
+    </row>
+    <row r="23" spans="1:8" ht="39" customHeight="1">
       <c r="A23" s="29">
         <v>1</v>
       </c>
@@ -1896,11 +1882,11 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
-    </row>
-    <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="40"/>
+    </row>
+    <row r="24" spans="1:8" ht="39" customHeight="1">
       <c r="A24" s="29">
         <v>1</v>
       </c>
@@ -1910,11 +1896,11 @@
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
-    </row>
-    <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
+    </row>
+    <row r="25" spans="1:8" ht="39" customHeight="1">
       <c r="A25" s="29">
         <v>1</v>
       </c>
@@ -1924,11 +1910,11 @@
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="37"/>
-    </row>
-    <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
+    </row>
+    <row r="26" spans="1:8" ht="39" customHeight="1">
       <c r="A26" s="29">
         <v>1</v>
       </c>
@@ -1938,13 +1924,13 @@
       <c r="C26" s="30"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
-    </row>
-    <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:8" ht="39" customHeight="1">
       <c r="A27" s="29">
         <v>1</v>
       </c>
@@ -1954,11 +1940,11 @@
       <c r="C27" s="30"/>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
-    </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
+    </row>
+    <row r="28" spans="1:8" ht="39" customHeight="1">
       <c r="A28" s="29">
         <v>1</v>
       </c>
@@ -1968,11 +1954,11 @@
       <c r="C28" s="30"/>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
-    </row>
-    <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="1:8" ht="39" customHeight="1">
       <c r="A29" s="29">
         <v>1</v>
       </c>
@@ -1982,13 +1968,13 @@
       <c r="C29" s="30"/>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-    </row>
-    <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
+    </row>
+    <row r="30" spans="1:8" ht="39" customHeight="1">
       <c r="A30" s="29">
         <v>1</v>
       </c>
@@ -2000,13 +1986,13 @@
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
-    </row>
-    <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
+    </row>
+    <row r="31" spans="1:8" ht="39" customHeight="1">
       <c r="A31" s="29">
         <v>1</v>
       </c>
@@ -2016,11 +2002,11 @@
       <c r="C31" s="30"/>
       <c r="D31" s="31"/>
       <c r="E31" s="31"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
-    </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="38"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
+    </row>
+    <row r="32" spans="1:8" ht="39" customHeight="1">
       <c r="A32" s="29">
         <v>1</v>
       </c>
@@ -2030,11 +2016,11 @@
       <c r="C32" s="30"/>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
-    </row>
-    <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="38"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
+    </row>
+    <row r="33" spans="1:8" ht="39" customHeight="1">
       <c r="A33" s="29">
         <v>1</v>
       </c>
@@ -2044,11 +2030,11 @@
       <c r="C33" s="30"/>
       <c r="D33" s="31"/>
       <c r="E33" s="31"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
-    </row>
-    <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
+    </row>
+    <row r="34" spans="1:8" ht="39" customHeight="1">
       <c r="A34" s="29">
         <v>1</v>
       </c>
@@ -2058,1675 +2044,1865 @@
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
-    </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="39"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="1:8" ht="39" customHeight="1">
       <c r="A35" s="29"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
-    </row>
-    <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="40"/>
+    </row>
+    <row r="36" spans="1:8" ht="39" customHeight="1">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
-    </row>
-    <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="40"/>
+    </row>
+    <row r="37" spans="1:8" ht="39" customHeight="1">
       <c r="A37" s="29"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
-    </row>
-    <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="40"/>
+    </row>
+    <row r="38" spans="1:8" ht="39" customHeight="1">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37"/>
-    </row>
-    <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
+    </row>
+    <row r="39" spans="1:8" ht="39" customHeight="1">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
       <c r="D39" s="31"/>
       <c r="E39" s="31"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
-    </row>
-    <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="38"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="40"/>
+    </row>
+    <row r="40" spans="1:8" ht="39" customHeight="1">
       <c r="A40" s="29"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
       <c r="D40" s="31"/>
       <c r="E40" s="31"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="37"/>
-    </row>
-    <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="38"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
+    </row>
+    <row r="41" spans="1:8" ht="39" customHeight="1">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
       <c r="D41" s="31"/>
       <c r="E41" s="31"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
-    </row>
-    <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="38"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="40"/>
+    </row>
+    <row r="42" spans="1:8" ht="39" customHeight="1">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
       <c r="D42" s="31"/>
       <c r="E42" s="31"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="37"/>
-    </row>
-    <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="38"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="40"/>
+    </row>
+    <row r="43" spans="1:8" ht="39" customHeight="1">
       <c r="A43" s="29"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="37"/>
-    </row>
-    <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="38"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="40"/>
+    </row>
+    <row r="44" spans="1:8" ht="39" customHeight="1">
       <c r="A44" s="29"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
       <c r="D44" s="31"/>
       <c r="E44" s="31"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="37"/>
-    </row>
-    <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="40"/>
+    </row>
+    <row r="45" spans="1:8" ht="39" customHeight="1">
       <c r="A45" s="29"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
       <c r="D45" s="31"/>
       <c r="E45" s="31"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
-    </row>
-    <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="38"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="40"/>
+    </row>
+    <row r="46" spans="1:8" ht="39" customHeight="1">
       <c r="A46" s="29"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37"/>
-    </row>
-    <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="38"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
+    </row>
+    <row r="47" spans="1:8" ht="39" customHeight="1">
       <c r="A47" s="29"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
       <c r="D47" s="31"/>
       <c r="E47" s="31"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="37"/>
-    </row>
-    <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="38"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
+    </row>
+    <row r="48" spans="1:8" ht="39" customHeight="1">
       <c r="A48" s="29"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="37"/>
-    </row>
-    <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="38"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="40"/>
+    </row>
+    <row r="49" spans="1:8" ht="39" customHeight="1">
       <c r="A49" s="29"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
       <c r="D49" s="31"/>
       <c r="E49" s="31"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="37"/>
-    </row>
-    <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="38"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="40"/>
+    </row>
+    <row r="50" spans="1:8" ht="39" customHeight="1">
       <c r="A50" s="29"/>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
       <c r="D50" s="31"/>
       <c r="E50" s="31"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="37"/>
-    </row>
-    <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="40"/>
+    </row>
+    <row r="51" spans="1:8" ht="39" customHeight="1">
       <c r="A51" s="29"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
       <c r="D51" s="31"/>
       <c r="E51" s="31"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="37"/>
-    </row>
-    <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="38"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="40"/>
+    </row>
+    <row r="52" spans="1:8" ht="39" customHeight="1">
       <c r="A52" s="29"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
       <c r="D52" s="31"/>
       <c r="E52" s="31"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="37"/>
-    </row>
-    <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="38"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="40"/>
+    </row>
+    <row r="53" spans="1:8" ht="39" customHeight="1">
       <c r="A53" s="29"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
       <c r="D53" s="31"/>
       <c r="E53" s="31"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
-    </row>
-    <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="38"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="40"/>
+    </row>
+    <row r="54" spans="1:8" ht="39" customHeight="1">
       <c r="A54" s="29"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
       <c r="D54" s="31"/>
       <c r="E54" s="31"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="37"/>
-    </row>
-    <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F54" s="38"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="40"/>
+    </row>
+    <row r="55" spans="1:8" ht="39" customHeight="1">
       <c r="A55" s="29"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="37"/>
-    </row>
-    <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="38"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="40"/>
+    </row>
+    <row r="56" spans="1:8" ht="39" customHeight="1">
       <c r="A56" s="29"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="37"/>
-    </row>
-    <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="38"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="40"/>
+    </row>
+    <row r="57" spans="1:8" ht="39" customHeight="1">
       <c r="A57" s="29"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="37"/>
-    </row>
-    <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="38"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="40"/>
+    </row>
+    <row r="58" spans="1:8" ht="39" customHeight="1">
       <c r="A58" s="29"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="37"/>
-    </row>
-    <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="38"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="40"/>
+    </row>
+    <row r="59" spans="1:8" ht="39" customHeight="1">
       <c r="A59" s="29"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="37"/>
-    </row>
-    <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="38"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="40"/>
+    </row>
+    <row r="60" spans="1:8" ht="39" customHeight="1">
       <c r="A60" s="29"/>
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="37"/>
-    </row>
-    <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="38"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="40"/>
+    </row>
+    <row r="61" spans="1:8" ht="39" customHeight="1">
       <c r="A61" s="29"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="37"/>
-    </row>
-    <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="40"/>
+    </row>
+    <row r="62" spans="1:8" ht="39" customHeight="1">
       <c r="A62" s="29"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="37"/>
-    </row>
-    <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="38"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="40"/>
+    </row>
+    <row r="63" spans="1:8" ht="39" customHeight="1">
       <c r="A63" s="29"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="37"/>
-    </row>
-    <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="40"/>
+    </row>
+    <row r="64" spans="1:8" ht="39" customHeight="1">
       <c r="A64" s="29"/>
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="37"/>
-    </row>
-    <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="40"/>
+    </row>
+    <row r="65" spans="1:8" ht="39" customHeight="1">
       <c r="A65" s="29"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="37"/>
-    </row>
-    <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="38"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="40"/>
+    </row>
+    <row r="66" spans="1:8" ht="39" customHeight="1">
       <c r="A66" s="29"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="37"/>
-    </row>
-    <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="38"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="40"/>
+    </row>
+    <row r="67" spans="1:8" ht="39" customHeight="1">
       <c r="A67" s="29"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="37"/>
-    </row>
-    <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="38"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="40"/>
+    </row>
+    <row r="68" spans="1:8" ht="39" customHeight="1">
       <c r="A68" s="29"/>
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="37"/>
-    </row>
-    <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="40"/>
+    </row>
+    <row r="69" spans="1:8" ht="39" customHeight="1">
       <c r="A69" s="29"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="37"/>
-    </row>
-    <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="40"/>
+    </row>
+    <row r="70" spans="1:8" ht="39" customHeight="1">
       <c r="A70" s="29"/>
       <c r="B70" s="30"/>
       <c r="C70" s="30"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="37"/>
-    </row>
-    <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F70" s="38"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="40"/>
+    </row>
+    <row r="71" spans="1:8" ht="39" customHeight="1">
       <c r="A71" s="29"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="37"/>
-    </row>
-    <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F71" s="38"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="40"/>
+    </row>
+    <row r="72" spans="1:8" ht="39" customHeight="1">
       <c r="A72" s="29"/>
       <c r="B72" s="30"/>
       <c r="C72" s="30"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="37"/>
-    </row>
-    <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F72" s="38"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="40"/>
+    </row>
+    <row r="73" spans="1:8" ht="39" customHeight="1">
       <c r="A73" s="29"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="37"/>
-    </row>
-    <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="40"/>
+    </row>
+    <row r="74" spans="1:8" ht="39" customHeight="1">
       <c r="A74" s="29"/>
       <c r="B74" s="30"/>
       <c r="C74" s="30"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="37"/>
-    </row>
-    <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="40"/>
+    </row>
+    <row r="75" spans="1:8" ht="39" customHeight="1">
       <c r="A75" s="29"/>
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="37"/>
-    </row>
-    <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F75" s="38"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="40"/>
+    </row>
+    <row r="76" spans="1:8" ht="39" customHeight="1">
       <c r="A76" s="29"/>
       <c r="B76" s="30"/>
       <c r="C76" s="30"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
-      <c r="F76" s="35"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="37"/>
-    </row>
-    <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F76" s="38"/>
+      <c r="G76" s="39"/>
+      <c r="H76" s="40"/>
+    </row>
+    <row r="77" spans="1:8" ht="39" customHeight="1">
       <c r="A77" s="29"/>
       <c r="B77" s="30"/>
       <c r="C77" s="30"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="37"/>
-    </row>
-    <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F77" s="38"/>
+      <c r="G77" s="39"/>
+      <c r="H77" s="40"/>
+    </row>
+    <row r="78" spans="1:8" ht="39" customHeight="1">
       <c r="A78" s="29"/>
       <c r="B78" s="30"/>
       <c r="C78" s="30"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="37"/>
-    </row>
-    <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F78" s="38"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="40"/>
+    </row>
+    <row r="79" spans="1:8" ht="39" customHeight="1">
       <c r="A79" s="29"/>
       <c r="B79" s="30"/>
       <c r="C79" s="30"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="36"/>
-      <c r="H79" s="37"/>
-    </row>
-    <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="40"/>
+    </row>
+    <row r="80" spans="1:8" ht="39" customHeight="1">
       <c r="A80" s="29"/>
       <c r="B80" s="30"/>
       <c r="C80" s="30"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="37"/>
-    </row>
-    <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F80" s="38"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="40"/>
+    </row>
+    <row r="81" spans="1:8" ht="39" customHeight="1">
       <c r="A81" s="29"/>
       <c r="B81" s="30"/>
       <c r="C81" s="30"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="37"/>
-    </row>
-    <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F81" s="38"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="40"/>
+    </row>
+    <row r="82" spans="1:8" ht="39" customHeight="1">
       <c r="A82" s="29"/>
       <c r="B82" s="30"/>
       <c r="C82" s="30"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="37"/>
-    </row>
-    <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="40"/>
+    </row>
+    <row r="83" spans="1:8" ht="39" customHeight="1">
       <c r="A83" s="29"/>
       <c r="B83" s="30"/>
       <c r="C83" s="30"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="37"/>
-    </row>
-    <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F83" s="38"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="40"/>
+    </row>
+    <row r="84" spans="1:8" ht="39" customHeight="1">
       <c r="A84" s="29"/>
       <c r="B84" s="30"/>
       <c r="C84" s="30"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
-      <c r="F84" s="35"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="37"/>
-    </row>
-    <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
+      <c r="H84" s="40"/>
+    </row>
+    <row r="85" spans="1:8" ht="39" customHeight="1">
       <c r="A85" s="29"/>
       <c r="B85" s="30"/>
       <c r="C85" s="30"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="37"/>
-    </row>
-    <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F85" s="38"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="40"/>
+    </row>
+    <row r="86" spans="1:8" ht="39" customHeight="1">
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
       <c r="C86" s="30"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="37"/>
-    </row>
-    <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F86" s="38"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="40"/>
+    </row>
+    <row r="87" spans="1:8" ht="39" customHeight="1">
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
       <c r="C87" s="30"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="36"/>
-      <c r="H87" s="37"/>
-    </row>
-    <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="40"/>
+    </row>
+    <row r="88" spans="1:8" ht="39" customHeight="1">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="30"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="37"/>
-    </row>
-    <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F88" s="38"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="40"/>
+    </row>
+    <row r="89" spans="1:8" ht="39" customHeight="1">
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
       <c r="C89" s="30"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="36"/>
-      <c r="H89" s="37"/>
-    </row>
-    <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F89" s="38"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="40"/>
+    </row>
+    <row r="90" spans="1:8" ht="39" customHeight="1">
       <c r="A90" s="29"/>
       <c r="B90" s="30"/>
       <c r="C90" s="30"/>
       <c r="D90" s="31"/>
       <c r="E90" s="31"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="36"/>
-      <c r="H90" s="37"/>
-    </row>
-    <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="40"/>
+    </row>
+    <row r="91" spans="1:8" ht="39" customHeight="1">
       <c r="A91" s="29"/>
       <c r="B91" s="30"/>
       <c r="C91" s="30"/>
       <c r="D91" s="31"/>
       <c r="E91" s="31"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="36"/>
-      <c r="H91" s="37"/>
-    </row>
-    <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="40"/>
+    </row>
+    <row r="92" spans="1:8" ht="39" customHeight="1">
       <c r="A92" s="29"/>
       <c r="B92" s="30"/>
       <c r="C92" s="30"/>
       <c r="D92" s="31"/>
       <c r="E92" s="31"/>
-      <c r="F92" s="35"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="37"/>
-    </row>
-    <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="40"/>
+    </row>
+    <row r="93" spans="1:8" ht="39" customHeight="1">
       <c r="A93" s="29"/>
       <c r="B93" s="30"/>
       <c r="C93" s="30"/>
       <c r="D93" s="31"/>
       <c r="E93" s="31"/>
-      <c r="F93" s="35"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="37"/>
-    </row>
-    <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F93" s="38"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="40"/>
+    </row>
+    <row r="94" spans="1:8" ht="39" customHeight="1">
       <c r="A94" s="29"/>
       <c r="B94" s="30"/>
       <c r="C94" s="30"/>
       <c r="D94" s="31"/>
       <c r="E94" s="31"/>
-      <c r="F94" s="35"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="37"/>
-    </row>
-    <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94" s="38"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="40"/>
+    </row>
+    <row r="95" spans="1:8" ht="39" customHeight="1">
       <c r="A95" s="29"/>
       <c r="B95" s="30"/>
       <c r="C95" s="30"/>
       <c r="D95" s="31"/>
       <c r="E95" s="31"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="37"/>
-    </row>
-    <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F95" s="38"/>
+      <c r="G95" s="39"/>
+      <c r="H95" s="40"/>
+    </row>
+    <row r="96" spans="1:8" ht="39" customHeight="1">
       <c r="A96" s="29"/>
       <c r="B96" s="30"/>
       <c r="C96" s="30"/>
       <c r="D96" s="31"/>
       <c r="E96" s="31"/>
-      <c r="F96" s="35"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="37"/>
-    </row>
-    <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F96" s="38"/>
+      <c r="G96" s="39"/>
+      <c r="H96" s="40"/>
+    </row>
+    <row r="97" spans="1:8" ht="39" customHeight="1">
       <c r="A97" s="29"/>
       <c r="B97" s="30"/>
       <c r="C97" s="30"/>
       <c r="D97" s="31"/>
       <c r="E97" s="31"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="36"/>
-      <c r="H97" s="37"/>
-    </row>
-    <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="38"/>
+      <c r="G97" s="39"/>
+      <c r="H97" s="40"/>
+    </row>
+    <row r="98" spans="1:8" ht="39" customHeight="1">
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
       <c r="C98" s="30"/>
       <c r="D98" s="31"/>
       <c r="E98" s="31"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="37"/>
-    </row>
-    <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F98" s="38"/>
+      <c r="G98" s="39"/>
+      <c r="H98" s="40"/>
+    </row>
+    <row r="99" spans="1:8" ht="39" customHeight="1">
       <c r="A99" s="29"/>
       <c r="B99" s="30"/>
       <c r="C99" s="30"/>
       <c r="D99" s="31"/>
       <c r="E99" s="31"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="37"/>
-    </row>
-    <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F99" s="38"/>
+      <c r="G99" s="39"/>
+      <c r="H99" s="40"/>
+    </row>
+    <row r="100" spans="1:8" ht="39" customHeight="1">
       <c r="A100" s="29"/>
       <c r="B100" s="30"/>
       <c r="C100" s="30"/>
       <c r="D100" s="31"/>
       <c r="E100" s="31"/>
-      <c r="F100" s="35"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="37"/>
-    </row>
-    <row r="101" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F100" s="38"/>
+      <c r="G100" s="39"/>
+      <c r="H100" s="40"/>
+    </row>
+    <row r="101" spans="1:8" ht="39" customHeight="1">
       <c r="A101" s="29"/>
       <c r="B101" s="30"/>
       <c r="C101" s="30"/>
       <c r="D101" s="31"/>
       <c r="E101" s="31"/>
-      <c r="F101" s="35"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="37"/>
-    </row>
-    <row r="102" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F101" s="38"/>
+      <c r="G101" s="39"/>
+      <c r="H101" s="40"/>
+    </row>
+    <row r="102" spans="1:8" ht="39" customHeight="1">
       <c r="A102" s="29"/>
       <c r="B102" s="30"/>
       <c r="C102" s="30"/>
       <c r="D102" s="31"/>
       <c r="E102" s="31"/>
-      <c r="F102" s="35"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="37"/>
-    </row>
-    <row r="103" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F102" s="38"/>
+      <c r="G102" s="39"/>
+      <c r="H102" s="40"/>
+    </row>
+    <row r="103" spans="1:8" ht="39" customHeight="1">
       <c r="A103" s="29"/>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
       <c r="D103" s="31"/>
       <c r="E103" s="31"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="37"/>
-    </row>
-    <row r="104" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F103" s="38"/>
+      <c r="G103" s="39"/>
+      <c r="H103" s="40"/>
+    </row>
+    <row r="104" spans="1:8" ht="39" customHeight="1">
       <c r="A104" s="29"/>
       <c r="B104" s="30"/>
       <c r="C104" s="30"/>
       <c r="D104" s="31"/>
       <c r="E104" s="31"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="36"/>
-      <c r="H104" s="37"/>
-    </row>
-    <row r="105" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F104" s="38"/>
+      <c r="G104" s="39"/>
+      <c r="H104" s="40"/>
+    </row>
+    <row r="105" spans="1:8" ht="39" customHeight="1">
       <c r="A105" s="29"/>
       <c r="B105" s="30"/>
       <c r="C105" s="30"/>
       <c r="D105" s="31"/>
       <c r="E105" s="31"/>
-      <c r="F105" s="35"/>
-      <c r="G105" s="36"/>
-      <c r="H105" s="37"/>
-    </row>
-    <row r="106" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F105" s="38"/>
+      <c r="G105" s="39"/>
+      <c r="H105" s="40"/>
+    </row>
+    <row r="106" spans="1:8" ht="39" customHeight="1">
       <c r="A106" s="29"/>
       <c r="B106" s="30"/>
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="31"/>
-      <c r="F106" s="35"/>
-      <c r="G106" s="36"/>
-      <c r="H106" s="37"/>
-    </row>
-    <row r="107" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F106" s="38"/>
+      <c r="G106" s="39"/>
+      <c r="H106" s="40"/>
+    </row>
+    <row r="107" spans="1:8" ht="39" customHeight="1">
       <c r="A107" s="29"/>
       <c r="B107" s="30"/>
       <c r="C107" s="30"/>
       <c r="D107" s="31"/>
       <c r="E107" s="31"/>
-      <c r="F107" s="35"/>
-      <c r="G107" s="36"/>
-      <c r="H107" s="37"/>
-    </row>
-    <row r="108" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F107" s="38"/>
+      <c r="G107" s="39"/>
+      <c r="H107" s="40"/>
+    </row>
+    <row r="108" spans="1:8" ht="39" customHeight="1">
       <c r="A108" s="29"/>
       <c r="B108" s="30"/>
       <c r="C108" s="30"/>
       <c r="D108" s="31"/>
       <c r="E108" s="31"/>
-      <c r="F108" s="35"/>
-      <c r="G108" s="36"/>
-      <c r="H108" s="37"/>
-    </row>
-    <row r="109" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F108" s="38"/>
+      <c r="G108" s="39"/>
+      <c r="H108" s="40"/>
+    </row>
+    <row r="109" spans="1:8" ht="39" customHeight="1">
       <c r="A109" s="29"/>
       <c r="B109" s="30"/>
       <c r="C109" s="30"/>
       <c r="D109" s="31"/>
       <c r="E109" s="31"/>
-      <c r="F109" s="35"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="37"/>
-    </row>
-    <row r="110" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F109" s="38"/>
+      <c r="G109" s="39"/>
+      <c r="H109" s="40"/>
+    </row>
+    <row r="110" spans="1:8" ht="39" customHeight="1">
       <c r="A110" s="29"/>
       <c r="B110" s="30"/>
       <c r="C110" s="30"/>
       <c r="D110" s="31"/>
       <c r="E110" s="31"/>
-      <c r="F110" s="35"/>
-      <c r="G110" s="36"/>
-      <c r="H110" s="37"/>
-    </row>
-    <row r="111" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F110" s="38"/>
+      <c r="G110" s="39"/>
+      <c r="H110" s="40"/>
+    </row>
+    <row r="111" spans="1:8" ht="39" customHeight="1">
       <c r="A111" s="29"/>
       <c r="B111" s="30"/>
       <c r="C111" s="30"/>
       <c r="D111" s="31"/>
       <c r="E111" s="31"/>
-      <c r="F111" s="35"/>
-      <c r="G111" s="36"/>
-      <c r="H111" s="37"/>
-    </row>
-    <row r="112" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111" s="38"/>
+      <c r="G111" s="39"/>
+      <c r="H111" s="40"/>
+    </row>
+    <row r="112" spans="1:8" ht="39" customHeight="1">
       <c r="A112" s="29"/>
       <c r="B112" s="30"/>
       <c r="C112" s="30"/>
       <c r="D112" s="31"/>
       <c r="E112" s="31"/>
-      <c r="F112" s="35"/>
-      <c r="G112" s="36"/>
-      <c r="H112" s="37"/>
-    </row>
-    <row r="113" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F112" s="38"/>
+      <c r="G112" s="39"/>
+      <c r="H112" s="40"/>
+    </row>
+    <row r="113" spans="1:8" ht="39" customHeight="1">
       <c r="A113" s="29"/>
       <c r="B113" s="30"/>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
       <c r="E113" s="31"/>
-      <c r="F113" s="35"/>
-      <c r="G113" s="36"/>
-      <c r="H113" s="37"/>
-    </row>
-    <row r="114" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F113" s="38"/>
+      <c r="G113" s="39"/>
+      <c r="H113" s="40"/>
+    </row>
+    <row r="114" spans="1:8" ht="39" customHeight="1">
       <c r="A114" s="29"/>
       <c r="B114" s="30"/>
       <c r="C114" s="30"/>
       <c r="D114" s="31"/>
       <c r="E114" s="31"/>
-      <c r="F114" s="35"/>
-      <c r="G114" s="36"/>
-      <c r="H114" s="37"/>
-    </row>
-    <row r="115" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F114" s="38"/>
+      <c r="G114" s="39"/>
+      <c r="H114" s="40"/>
+    </row>
+    <row r="115" spans="1:8" ht="39" customHeight="1">
       <c r="A115" s="29"/>
       <c r="B115" s="30"/>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
       <c r="E115" s="31"/>
-      <c r="F115" s="35"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="37"/>
-    </row>
-    <row r="116" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F115" s="38"/>
+      <c r="G115" s="39"/>
+      <c r="H115" s="40"/>
+    </row>
+    <row r="116" spans="1:8" ht="39" customHeight="1">
       <c r="A116" s="29"/>
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
       <c r="D116" s="31"/>
       <c r="E116" s="31"/>
-      <c r="F116" s="35"/>
-      <c r="G116" s="36"/>
-      <c r="H116" s="37"/>
-    </row>
-    <row r="117" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F116" s="38"/>
+      <c r="G116" s="39"/>
+      <c r="H116" s="40"/>
+    </row>
+    <row r="117" spans="1:8" ht="39" customHeight="1">
       <c r="A117" s="29"/>
       <c r="B117" s="30"/>
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
       <c r="E117" s="31"/>
-      <c r="F117" s="35"/>
-      <c r="G117" s="36"/>
-      <c r="H117" s="37"/>
-    </row>
-    <row r="118" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F117" s="38"/>
+      <c r="G117" s="39"/>
+      <c r="H117" s="40"/>
+    </row>
+    <row r="118" spans="1:8" ht="39" customHeight="1">
       <c r="A118" s="29"/>
       <c r="B118" s="30"/>
       <c r="C118" s="30"/>
       <c r="D118" s="31"/>
       <c r="E118" s="31"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="37"/>
-    </row>
-    <row r="119" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F118" s="38"/>
+      <c r="G118" s="39"/>
+      <c r="H118" s="40"/>
+    </row>
+    <row r="119" spans="1:8" ht="39" customHeight="1">
       <c r="A119" s="29"/>
       <c r="B119" s="30"/>
       <c r="C119" s="30"/>
       <c r="D119" s="31"/>
       <c r="E119" s="31"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="36"/>
-      <c r="H119" s="37"/>
-    </row>
-    <row r="120" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F119" s="38"/>
+      <c r="G119" s="39"/>
+      <c r="H119" s="40"/>
+    </row>
+    <row r="120" spans="1:8" ht="39" customHeight="1">
       <c r="A120" s="29"/>
       <c r="B120" s="30"/>
       <c r="C120" s="30"/>
       <c r="D120" s="31"/>
       <c r="E120" s="31"/>
-      <c r="F120" s="35"/>
-      <c r="G120" s="36"/>
-      <c r="H120" s="37"/>
-    </row>
-    <row r="121" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F120" s="38"/>
+      <c r="G120" s="39"/>
+      <c r="H120" s="40"/>
+    </row>
+    <row r="121" spans="1:8" ht="39" customHeight="1">
       <c r="A121" s="29"/>
       <c r="B121" s="30"/>
       <c r="C121" s="30"/>
       <c r="D121" s="31"/>
       <c r="E121" s="31"/>
-      <c r="F121" s="35"/>
-      <c r="G121" s="36"/>
-      <c r="H121" s="37"/>
-    </row>
-    <row r="122" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F121" s="38"/>
+      <c r="G121" s="39"/>
+      <c r="H121" s="40"/>
+    </row>
+    <row r="122" spans="1:8" ht="39" customHeight="1">
       <c r="A122" s="29"/>
       <c r="B122" s="30"/>
       <c r="C122" s="30"/>
       <c r="D122" s="31"/>
       <c r="E122" s="31"/>
-      <c r="F122" s="35"/>
-      <c r="G122" s="36"/>
-      <c r="H122" s="37"/>
-    </row>
-    <row r="123" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F122" s="38"/>
+      <c r="G122" s="39"/>
+      <c r="H122" s="40"/>
+    </row>
+    <row r="123" spans="1:8" ht="39" customHeight="1">
       <c r="A123" s="29"/>
       <c r="B123" s="30"/>
       <c r="C123" s="30"/>
       <c r="D123" s="31"/>
       <c r="E123" s="31"/>
-      <c r="F123" s="35"/>
-      <c r="G123" s="36"/>
-      <c r="H123" s="37"/>
-    </row>
-    <row r="124" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="38"/>
+      <c r="G123" s="39"/>
+      <c r="H123" s="40"/>
+    </row>
+    <row r="124" spans="1:8" ht="39" customHeight="1">
       <c r="A124" s="29"/>
       <c r="B124" s="30"/>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
       <c r="E124" s="31"/>
-      <c r="F124" s="35"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="37"/>
-    </row>
-    <row r="125" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F124" s="38"/>
+      <c r="G124" s="39"/>
+      <c r="H124" s="40"/>
+    </row>
+    <row r="125" spans="1:8" ht="39" customHeight="1">
       <c r="A125" s="29"/>
       <c r="B125" s="30"/>
       <c r="C125" s="30"/>
       <c r="D125" s="31"/>
       <c r="E125" s="31"/>
-      <c r="F125" s="35"/>
-      <c r="G125" s="36"/>
-      <c r="H125" s="37"/>
-    </row>
-    <row r="126" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F125" s="38"/>
+      <c r="G125" s="39"/>
+      <c r="H125" s="40"/>
+    </row>
+    <row r="126" spans="1:8" ht="39" customHeight="1">
       <c r="A126" s="29"/>
       <c r="B126" s="30"/>
       <c r="C126" s="30"/>
       <c r="D126" s="31"/>
       <c r="E126" s="31"/>
-      <c r="F126" s="35"/>
-      <c r="G126" s="36"/>
-      <c r="H126" s="37"/>
-    </row>
-    <row r="127" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F126" s="38"/>
+      <c r="G126" s="39"/>
+      <c r="H126" s="40"/>
+    </row>
+    <row r="127" spans="1:8" ht="39" customHeight="1">
       <c r="A127" s="29"/>
       <c r="B127" s="30"/>
       <c r="C127" s="30"/>
       <c r="D127" s="31"/>
       <c r="E127" s="31"/>
-      <c r="F127" s="35"/>
-      <c r="G127" s="36"/>
-      <c r="H127" s="37"/>
-    </row>
-    <row r="128" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F127" s="38"/>
+      <c r="G127" s="39"/>
+      <c r="H127" s="40"/>
+    </row>
+    <row r="128" spans="1:8" ht="39" customHeight="1">
       <c r="A128" s="29"/>
       <c r="B128" s="30"/>
       <c r="C128" s="30"/>
       <c r="D128" s="31"/>
       <c r="E128" s="31"/>
-      <c r="F128" s="35"/>
-      <c r="G128" s="36"/>
-      <c r="H128" s="37"/>
-    </row>
-    <row r="129" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F128" s="38"/>
+      <c r="G128" s="39"/>
+      <c r="H128" s="40"/>
+    </row>
+    <row r="129" spans="1:8" ht="39" customHeight="1">
       <c r="A129" s="29"/>
       <c r="B129" s="30"/>
       <c r="C129" s="30"/>
       <c r="D129" s="31"/>
       <c r="E129" s="31"/>
-      <c r="F129" s="35"/>
-      <c r="G129" s="36"/>
-      <c r="H129" s="37"/>
-    </row>
-    <row r="130" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F129" s="38"/>
+      <c r="G129" s="39"/>
+      <c r="H129" s="40"/>
+    </row>
+    <row r="130" spans="1:8" ht="39" customHeight="1">
       <c r="A130" s="29"/>
       <c r="B130" s="30"/>
       <c r="C130" s="30"/>
       <c r="D130" s="31"/>
       <c r="E130" s="31"/>
-      <c r="F130" s="35"/>
-      <c r="G130" s="36"/>
-      <c r="H130" s="37"/>
-    </row>
-    <row r="131" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F130" s="38"/>
+      <c r="G130" s="39"/>
+      <c r="H130" s="40"/>
+    </row>
+    <row r="131" spans="1:8" ht="39" customHeight="1">
       <c r="A131" s="29"/>
       <c r="B131" s="30"/>
       <c r="C131" s="30"/>
       <c r="D131" s="31"/>
       <c r="E131" s="31"/>
-      <c r="F131" s="35"/>
-      <c r="G131" s="36"/>
-      <c r="H131" s="37"/>
-    </row>
-    <row r="132" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F131" s="38"/>
+      <c r="G131" s="39"/>
+      <c r="H131" s="40"/>
+    </row>
+    <row r="132" spans="1:8" ht="39" customHeight="1">
       <c r="A132" s="29"/>
       <c r="B132" s="30"/>
       <c r="C132" s="30"/>
       <c r="D132" s="31"/>
       <c r="E132" s="31"/>
-      <c r="F132" s="35"/>
-      <c r="G132" s="36"/>
-      <c r="H132" s="37"/>
-    </row>
-    <row r="133" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F132" s="38"/>
+      <c r="G132" s="39"/>
+      <c r="H132" s="40"/>
+    </row>
+    <row r="133" spans="1:8" ht="39" customHeight="1">
       <c r="A133" s="29"/>
       <c r="B133" s="30"/>
       <c r="C133" s="30"/>
       <c r="D133" s="31"/>
       <c r="E133" s="31"/>
-      <c r="F133" s="35"/>
-      <c r="G133" s="36"/>
-      <c r="H133" s="37"/>
-    </row>
-    <row r="134" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F133" s="38"/>
+      <c r="G133" s="39"/>
+      <c r="H133" s="40"/>
+    </row>
+    <row r="134" spans="1:8" ht="39" customHeight="1">
       <c r="A134" s="29"/>
       <c r="B134" s="30"/>
       <c r="C134" s="30"/>
       <c r="D134" s="31"/>
       <c r="E134" s="31"/>
-      <c r="F134" s="35"/>
-      <c r="G134" s="36"/>
-      <c r="H134" s="37"/>
-    </row>
-    <row r="135" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F134" s="38"/>
+      <c r="G134" s="39"/>
+      <c r="H134" s="40"/>
+    </row>
+    <row r="135" spans="1:8" ht="39" customHeight="1">
       <c r="A135" s="29"/>
       <c r="B135" s="30"/>
       <c r="C135" s="30"/>
       <c r="D135" s="31"/>
       <c r="E135" s="31"/>
-      <c r="F135" s="35"/>
-      <c r="G135" s="36"/>
-      <c r="H135" s="37"/>
-    </row>
-    <row r="136" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F135" s="38"/>
+      <c r="G135" s="39"/>
+      <c r="H135" s="40"/>
+    </row>
+    <row r="136" spans="1:8" ht="39" customHeight="1">
       <c r="A136" s="29"/>
       <c r="B136" s="30"/>
       <c r="C136" s="30"/>
       <c r="D136" s="31"/>
       <c r="E136" s="31"/>
-      <c r="F136" s="35"/>
-      <c r="G136" s="36"/>
-      <c r="H136" s="37"/>
-    </row>
-    <row r="137" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F136" s="38"/>
+      <c r="G136" s="39"/>
+      <c r="H136" s="40"/>
+    </row>
+    <row r="137" spans="1:8" ht="39" customHeight="1">
       <c r="A137" s="29"/>
       <c r="B137" s="30"/>
       <c r="C137" s="30"/>
       <c r="D137" s="31"/>
       <c r="E137" s="31"/>
-      <c r="F137" s="35"/>
-      <c r="G137" s="36"/>
-      <c r="H137" s="37"/>
-    </row>
-    <row r="138" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F137" s="38"/>
+      <c r="G137" s="39"/>
+      <c r="H137" s="40"/>
+    </row>
+    <row r="138" spans="1:8" ht="39" customHeight="1">
       <c r="A138" s="29"/>
       <c r="B138" s="30"/>
       <c r="C138" s="30"/>
       <c r="D138" s="31"/>
       <c r="E138" s="31"/>
-      <c r="F138" s="35"/>
-      <c r="G138" s="36"/>
-      <c r="H138" s="37"/>
-    </row>
-    <row r="139" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F138" s="38"/>
+      <c r="G138" s="39"/>
+      <c r="H138" s="40"/>
+    </row>
+    <row r="139" spans="1:8" ht="39" customHeight="1">
       <c r="A139" s="29"/>
       <c r="B139" s="30"/>
       <c r="C139" s="30"/>
       <c r="D139" s="31"/>
       <c r="E139" s="31"/>
-      <c r="F139" s="35"/>
-      <c r="G139" s="36"/>
-      <c r="H139" s="37"/>
-    </row>
-    <row r="140" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F139" s="38"/>
+      <c r="G139" s="39"/>
+      <c r="H139" s="40"/>
+    </row>
+    <row r="140" spans="1:8" ht="39" customHeight="1">
       <c r="A140" s="29"/>
       <c r="B140" s="30"/>
       <c r="C140" s="30"/>
       <c r="D140" s="31"/>
       <c r="E140" s="31"/>
-      <c r="F140" s="35"/>
-      <c r="G140" s="36"/>
-      <c r="H140" s="37"/>
-    </row>
-    <row r="141" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F140" s="38"/>
+      <c r="G140" s="39"/>
+      <c r="H140" s="40"/>
+    </row>
+    <row r="141" spans="1:8" ht="39" customHeight="1">
       <c r="A141" s="29"/>
       <c r="B141" s="30"/>
       <c r="C141" s="30"/>
       <c r="D141" s="31"/>
       <c r="E141" s="31"/>
-      <c r="F141" s="35"/>
-      <c r="G141" s="36"/>
-      <c r="H141" s="37"/>
-    </row>
-    <row r="142" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F141" s="38"/>
+      <c r="G141" s="39"/>
+      <c r="H141" s="40"/>
+    </row>
+    <row r="142" spans="1:8" ht="39" customHeight="1">
       <c r="A142" s="29"/>
       <c r="B142" s="30"/>
       <c r="C142" s="30"/>
       <c r="D142" s="31"/>
       <c r="E142" s="31"/>
-      <c r="F142" s="35"/>
-      <c r="G142" s="36"/>
-      <c r="H142" s="37"/>
-    </row>
-    <row r="143" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F142" s="38"/>
+      <c r="G142" s="39"/>
+      <c r="H142" s="40"/>
+    </row>
+    <row r="143" spans="1:8" ht="39" customHeight="1">
       <c r="A143" s="29"/>
       <c r="B143" s="30"/>
       <c r="C143" s="30"/>
       <c r="D143" s="31"/>
       <c r="E143" s="31"/>
-      <c r="F143" s="35"/>
-      <c r="G143" s="36"/>
-      <c r="H143" s="37"/>
-    </row>
-    <row r="144" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F143" s="38"/>
+      <c r="G143" s="39"/>
+      <c r="H143" s="40"/>
+    </row>
+    <row r="144" spans="1:8" ht="39" customHeight="1">
       <c r="A144" s="29"/>
       <c r="B144" s="30"/>
       <c r="C144" s="30"/>
       <c r="D144" s="31"/>
       <c r="E144" s="31"/>
-      <c r="F144" s="35"/>
-      <c r="G144" s="36"/>
-      <c r="H144" s="37"/>
-    </row>
-    <row r="145" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F144" s="38"/>
+      <c r="G144" s="39"/>
+      <c r="H144" s="40"/>
+    </row>
+    <row r="145" spans="1:8" ht="39" customHeight="1">
       <c r="A145" s="29"/>
       <c r="B145" s="30"/>
       <c r="C145" s="30"/>
       <c r="D145" s="31"/>
       <c r="E145" s="31"/>
-      <c r="F145" s="35"/>
-      <c r="G145" s="36"/>
-      <c r="H145" s="37"/>
-    </row>
-    <row r="146" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F145" s="38"/>
+      <c r="G145" s="39"/>
+      <c r="H145" s="40"/>
+    </row>
+    <row r="146" spans="1:8" ht="39" customHeight="1">
       <c r="A146" s="29"/>
       <c r="B146" s="30"/>
       <c r="C146" s="30"/>
       <c r="D146" s="31"/>
       <c r="E146" s="31"/>
-      <c r="F146" s="35"/>
-      <c r="G146" s="36"/>
-      <c r="H146" s="37"/>
-    </row>
-    <row r="147" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F146" s="38"/>
+      <c r="G146" s="39"/>
+      <c r="H146" s="40"/>
+    </row>
+    <row r="147" spans="1:8" ht="39" customHeight="1">
       <c r="A147" s="29"/>
       <c r="B147" s="30"/>
       <c r="C147" s="30"/>
       <c r="D147" s="31"/>
       <c r="E147" s="31"/>
-      <c r="F147" s="35"/>
-      <c r="G147" s="36"/>
-      <c r="H147" s="37"/>
-    </row>
-    <row r="148" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F147" s="38"/>
+      <c r="G147" s="39"/>
+      <c r="H147" s="40"/>
+    </row>
+    <row r="148" spans="1:8" ht="39" customHeight="1">
       <c r="A148" s="29"/>
       <c r="B148" s="30"/>
       <c r="C148" s="30"/>
       <c r="D148" s="31"/>
       <c r="E148" s="31"/>
-      <c r="F148" s="35"/>
-      <c r="G148" s="36"/>
-      <c r="H148" s="37"/>
-    </row>
-    <row r="149" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F148" s="38"/>
+      <c r="G148" s="39"/>
+      <c r="H148" s="40"/>
+    </row>
+    <row r="149" spans="1:8" ht="39" customHeight="1">
       <c r="A149" s="29"/>
       <c r="B149" s="30"/>
       <c r="C149" s="30"/>
       <c r="D149" s="31"/>
       <c r="E149" s="31"/>
-      <c r="F149" s="35"/>
-      <c r="G149" s="36"/>
-      <c r="H149" s="37"/>
-    </row>
-    <row r="150" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F149" s="38"/>
+      <c r="G149" s="39"/>
+      <c r="H149" s="40"/>
+    </row>
+    <row r="150" spans="1:8" ht="39" customHeight="1">
       <c r="A150" s="29"/>
       <c r="B150" s="30"/>
       <c r="C150" s="30"/>
       <c r="D150" s="31"/>
       <c r="E150" s="31"/>
-      <c r="F150" s="35"/>
-      <c r="G150" s="36"/>
-      <c r="H150" s="37"/>
-    </row>
-    <row r="151" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F150" s="38"/>
+      <c r="G150" s="39"/>
+      <c r="H150" s="40"/>
+    </row>
+    <row r="151" spans="1:8" ht="39" customHeight="1">
       <c r="A151" s="29"/>
       <c r="B151" s="30"/>
       <c r="C151" s="30"/>
       <c r="D151" s="31"/>
       <c r="E151" s="31"/>
-      <c r="F151" s="35"/>
-      <c r="G151" s="36"/>
-      <c r="H151" s="37"/>
-    </row>
-    <row r="152" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F151" s="38"/>
+      <c r="G151" s="39"/>
+      <c r="H151" s="40"/>
+    </row>
+    <row r="152" spans="1:8" ht="39" customHeight="1">
       <c r="A152" s="29"/>
       <c r="B152" s="30"/>
       <c r="C152" s="30"/>
       <c r="D152" s="31"/>
       <c r="E152" s="31"/>
-      <c r="F152" s="35"/>
-      <c r="G152" s="36"/>
-      <c r="H152" s="37"/>
-    </row>
-    <row r="153" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F152" s="38"/>
+      <c r="G152" s="39"/>
+      <c r="H152" s="40"/>
+    </row>
+    <row r="153" spans="1:8" ht="39" customHeight="1">
       <c r="A153" s="29"/>
       <c r="B153" s="30"/>
       <c r="C153" s="30"/>
       <c r="D153" s="31"/>
       <c r="E153" s="31"/>
-      <c r="F153" s="35"/>
-      <c r="G153" s="36"/>
-      <c r="H153" s="37"/>
-    </row>
-    <row r="154" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F153" s="38"/>
+      <c r="G153" s="39"/>
+      <c r="H153" s="40"/>
+    </row>
+    <row r="154" spans="1:8" ht="39" customHeight="1">
       <c r="A154" s="29"/>
       <c r="B154" s="30"/>
       <c r="C154" s="30"/>
       <c r="D154" s="31"/>
       <c r="E154" s="31"/>
-      <c r="F154" s="35"/>
-      <c r="G154" s="36"/>
-      <c r="H154" s="37"/>
-    </row>
-    <row r="155" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F154" s="38"/>
+      <c r="G154" s="39"/>
+      <c r="H154" s="40"/>
+    </row>
+    <row r="155" spans="1:8" ht="39" customHeight="1">
       <c r="A155" s="29"/>
       <c r="B155" s="30"/>
       <c r="C155" s="30"/>
       <c r="D155" s="31"/>
       <c r="E155" s="31"/>
-      <c r="F155" s="35"/>
-      <c r="G155" s="36"/>
-      <c r="H155" s="37"/>
-    </row>
-    <row r="156" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F155" s="38"/>
+      <c r="G155" s="39"/>
+      <c r="H155" s="40"/>
+    </row>
+    <row r="156" spans="1:8" ht="39" customHeight="1">
       <c r="A156" s="29"/>
       <c r="B156" s="30"/>
       <c r="C156" s="30"/>
       <c r="D156" s="31"/>
       <c r="E156" s="31"/>
-      <c r="F156" s="35"/>
-      <c r="G156" s="36"/>
-      <c r="H156" s="37"/>
-    </row>
-    <row r="157" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F156" s="38"/>
+      <c r="G156" s="39"/>
+      <c r="H156" s="40"/>
+    </row>
+    <row r="157" spans="1:8" ht="39" customHeight="1">
       <c r="A157" s="29"/>
       <c r="B157" s="30"/>
       <c r="C157" s="30"/>
       <c r="D157" s="31"/>
       <c r="E157" s="31"/>
-      <c r="F157" s="35"/>
-      <c r="G157" s="36"/>
-      <c r="H157" s="37"/>
-    </row>
-    <row r="158" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F157" s="38"/>
+      <c r="G157" s="39"/>
+      <c r="H157" s="40"/>
+    </row>
+    <row r="158" spans="1:8" ht="39" customHeight="1">
       <c r="A158" s="29"/>
       <c r="B158" s="30"/>
       <c r="C158" s="30"/>
       <c r="D158" s="31"/>
       <c r="E158" s="31"/>
-      <c r="F158" s="35"/>
-      <c r="G158" s="36"/>
-      <c r="H158" s="37"/>
-    </row>
-    <row r="159" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F158" s="38"/>
+      <c r="G158" s="39"/>
+      <c r="H158" s="40"/>
+    </row>
+    <row r="159" spans="1:8" ht="39" customHeight="1">
       <c r="A159" s="29"/>
       <c r="B159" s="30"/>
       <c r="C159" s="30"/>
       <c r="D159" s="31"/>
       <c r="E159" s="31"/>
-      <c r="F159" s="35"/>
-      <c r="G159" s="36"/>
-      <c r="H159" s="37"/>
-    </row>
-    <row r="160" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F159" s="38"/>
+      <c r="G159" s="39"/>
+      <c r="H159" s="40"/>
+    </row>
+    <row r="160" spans="1:8" ht="39" customHeight="1">
       <c r="A160" s="29"/>
       <c r="B160" s="30"/>
       <c r="C160" s="30"/>
       <c r="D160" s="31"/>
       <c r="E160" s="31"/>
-      <c r="F160" s="35"/>
-      <c r="G160" s="36"/>
-      <c r="H160" s="37"/>
-    </row>
-    <row r="161" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F160" s="38"/>
+      <c r="G160" s="39"/>
+      <c r="H160" s="40"/>
+    </row>
+    <row r="161" spans="1:8" ht="39" customHeight="1">
       <c r="A161" s="29"/>
       <c r="B161" s="30"/>
       <c r="C161" s="30"/>
       <c r="D161" s="31"/>
       <c r="E161" s="31"/>
-      <c r="F161" s="35"/>
-      <c r="G161" s="36"/>
-      <c r="H161" s="37"/>
-    </row>
-    <row r="162" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F161" s="38"/>
+      <c r="G161" s="39"/>
+      <c r="H161" s="40"/>
+    </row>
+    <row r="162" spans="1:8" ht="39" customHeight="1">
       <c r="A162" s="29"/>
       <c r="B162" s="30"/>
       <c r="C162" s="30"/>
       <c r="D162" s="31"/>
       <c r="E162" s="31"/>
-      <c r="F162" s="35"/>
-      <c r="G162" s="36"/>
-      <c r="H162" s="37"/>
-    </row>
-    <row r="163" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F162" s="38"/>
+      <c r="G162" s="39"/>
+      <c r="H162" s="40"/>
+    </row>
+    <row r="163" spans="1:8" ht="39" customHeight="1">
       <c r="A163" s="29"/>
       <c r="B163" s="30"/>
       <c r="C163" s="30"/>
       <c r="D163" s="31"/>
       <c r="E163" s="31"/>
-      <c r="F163" s="35"/>
-      <c r="G163" s="36"/>
-      <c r="H163" s="37"/>
-    </row>
-    <row r="164" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F163" s="38"/>
+      <c r="G163" s="39"/>
+      <c r="H163" s="40"/>
+    </row>
+    <row r="164" spans="1:8" ht="39" customHeight="1">
       <c r="A164" s="29"/>
       <c r="B164" s="30"/>
       <c r="C164" s="30"/>
       <c r="D164" s="31"/>
       <c r="E164" s="31"/>
-      <c r="F164" s="35"/>
-      <c r="G164" s="36"/>
-      <c r="H164" s="37"/>
-    </row>
-    <row r="165" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F164" s="38"/>
+      <c r="G164" s="39"/>
+      <c r="H164" s="40"/>
+    </row>
+    <row r="165" spans="1:8" ht="39" customHeight="1">
       <c r="A165" s="29"/>
       <c r="B165" s="30"/>
       <c r="C165" s="30"/>
       <c r="D165" s="31"/>
       <c r="E165" s="31"/>
-      <c r="F165" s="35"/>
-      <c r="G165" s="36"/>
-      <c r="H165" s="37"/>
-    </row>
-    <row r="166" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F165" s="38"/>
+      <c r="G165" s="39"/>
+      <c r="H165" s="40"/>
+    </row>
+    <row r="166" spans="1:8" ht="39" customHeight="1">
       <c r="A166" s="29"/>
       <c r="B166" s="30"/>
       <c r="C166" s="30"/>
       <c r="D166" s="31"/>
       <c r="E166" s="31"/>
-      <c r="F166" s="35"/>
-      <c r="G166" s="36"/>
-      <c r="H166" s="37"/>
-    </row>
-    <row r="167" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F166" s="38"/>
+      <c r="G166" s="39"/>
+      <c r="H166" s="40"/>
+    </row>
+    <row r="167" spans="1:8" ht="39" customHeight="1">
       <c r="A167" s="29"/>
       <c r="B167" s="30"/>
       <c r="C167" s="30"/>
       <c r="D167" s="31"/>
       <c r="E167" s="31"/>
-      <c r="F167" s="35"/>
-      <c r="G167" s="36"/>
-      <c r="H167" s="37"/>
-    </row>
-    <row r="168" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F167" s="38"/>
+      <c r="G167" s="39"/>
+      <c r="H167" s="40"/>
+    </row>
+    <row r="168" spans="1:8" ht="39" customHeight="1">
       <c r="A168" s="29"/>
       <c r="B168" s="30"/>
       <c r="C168" s="30"/>
       <c r="D168" s="31"/>
       <c r="E168" s="31"/>
-      <c r="F168" s="35"/>
-      <c r="G168" s="36"/>
-      <c r="H168" s="37"/>
-    </row>
-    <row r="169" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F168" s="38"/>
+      <c r="G168" s="39"/>
+      <c r="H168" s="40"/>
+    </row>
+    <row r="169" spans="1:8" ht="39" customHeight="1">
       <c r="A169" s="29"/>
       <c r="B169" s="30"/>
       <c r="C169" s="30"/>
       <c r="D169" s="31"/>
       <c r="E169" s="31"/>
-      <c r="F169" s="35"/>
-      <c r="G169" s="36"/>
-      <c r="H169" s="37"/>
-    </row>
-    <row r="170" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F169" s="38"/>
+      <c r="G169" s="39"/>
+      <c r="H169" s="40"/>
+    </row>
+    <row r="170" spans="1:8" ht="39" customHeight="1">
       <c r="A170" s="29"/>
       <c r="B170" s="30"/>
       <c r="C170" s="30"/>
       <c r="D170" s="31"/>
       <c r="E170" s="31"/>
-      <c r="F170" s="35"/>
-      <c r="G170" s="36"/>
-      <c r="H170" s="37"/>
-    </row>
-    <row r="171" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F170" s="38"/>
+      <c r="G170" s="39"/>
+      <c r="H170" s="40"/>
+    </row>
+    <row r="171" spans="1:8" ht="39" customHeight="1">
       <c r="A171" s="29"/>
       <c r="B171" s="30"/>
       <c r="C171" s="30"/>
       <c r="D171" s="31"/>
       <c r="E171" s="31"/>
-      <c r="F171" s="35"/>
-      <c r="G171" s="36"/>
-      <c r="H171" s="37"/>
-    </row>
-    <row r="172" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F171" s="38"/>
+      <c r="G171" s="39"/>
+      <c r="H171" s="40"/>
+    </row>
+    <row r="172" spans="1:8" ht="39" customHeight="1">
       <c r="A172" s="29"/>
       <c r="B172" s="30"/>
       <c r="C172" s="30"/>
       <c r="D172" s="31"/>
       <c r="E172" s="31"/>
-      <c r="F172" s="35"/>
-      <c r="G172" s="36"/>
-      <c r="H172" s="37"/>
-    </row>
-    <row r="173" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F172" s="38"/>
+      <c r="G172" s="39"/>
+      <c r="H172" s="40"/>
+    </row>
+    <row r="173" spans="1:8" ht="39" customHeight="1">
       <c r="A173" s="29"/>
       <c r="B173" s="30"/>
       <c r="C173" s="30"/>
       <c r="D173" s="31"/>
       <c r="E173" s="31"/>
-      <c r="F173" s="35"/>
-      <c r="G173" s="36"/>
-      <c r="H173" s="37"/>
-    </row>
-    <row r="174" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F173" s="38"/>
+      <c r="G173" s="39"/>
+      <c r="H173" s="40"/>
+    </row>
+    <row r="174" spans="1:8" ht="39" customHeight="1">
       <c r="A174" s="29"/>
       <c r="B174" s="30"/>
       <c r="C174" s="30"/>
       <c r="D174" s="31"/>
       <c r="E174" s="31"/>
-      <c r="F174" s="35"/>
-      <c r="G174" s="36"/>
-      <c r="H174" s="37"/>
-    </row>
-    <row r="175" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F174" s="38"/>
+      <c r="G174" s="39"/>
+      <c r="H174" s="40"/>
+    </row>
+    <row r="175" spans="1:8" ht="39" customHeight="1">
       <c r="A175" s="29"/>
       <c r="B175" s="30"/>
       <c r="C175" s="30"/>
       <c r="D175" s="31"/>
       <c r="E175" s="31"/>
-      <c r="F175" s="35"/>
-      <c r="G175" s="36"/>
-      <c r="H175" s="37"/>
-    </row>
-    <row r="176" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F175" s="38"/>
+      <c r="G175" s="39"/>
+      <c r="H175" s="40"/>
+    </row>
+    <row r="176" spans="1:8" ht="39" customHeight="1">
       <c r="A176" s="29"/>
       <c r="B176" s="30"/>
       <c r="C176" s="30"/>
       <c r="D176" s="31"/>
       <c r="E176" s="31"/>
-      <c r="F176" s="35"/>
-      <c r="G176" s="36"/>
-      <c r="H176" s="37"/>
-    </row>
-    <row r="177" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F176" s="38"/>
+      <c r="G176" s="39"/>
+      <c r="H176" s="40"/>
+    </row>
+    <row r="177" spans="1:8" ht="39" customHeight="1">
       <c r="A177" s="29"/>
       <c r="B177" s="30"/>
       <c r="C177" s="30"/>
       <c r="D177" s="31"/>
       <c r="E177" s="31"/>
-      <c r="F177" s="35"/>
-      <c r="G177" s="36"/>
-      <c r="H177" s="37"/>
-    </row>
-    <row r="178" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F177" s="38"/>
+      <c r="G177" s="39"/>
+      <c r="H177" s="40"/>
+    </row>
+    <row r="178" spans="1:8" ht="39" customHeight="1">
       <c r="A178" s="29"/>
       <c r="B178" s="30"/>
       <c r="C178" s="30"/>
       <c r="D178" s="31"/>
       <c r="E178" s="31"/>
-      <c r="F178" s="35"/>
-      <c r="G178" s="36"/>
-      <c r="H178" s="37"/>
-    </row>
-    <row r="179" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F178" s="38"/>
+      <c r="G178" s="39"/>
+      <c r="H178" s="40"/>
+    </row>
+    <row r="179" spans="1:8" ht="39" customHeight="1">
       <c r="A179" s="29"/>
       <c r="B179" s="30"/>
       <c r="C179" s="30"/>
       <c r="D179" s="31"/>
       <c r="E179" s="31"/>
-      <c r="F179" s="35"/>
-      <c r="G179" s="36"/>
-      <c r="H179" s="37"/>
-    </row>
-    <row r="180" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F179" s="38"/>
+      <c r="G179" s="39"/>
+      <c r="H179" s="40"/>
+    </row>
+    <row r="180" spans="1:8" ht="39" customHeight="1">
       <c r="A180" s="29"/>
       <c r="B180" s="30"/>
       <c r="C180" s="30"/>
       <c r="D180" s="31"/>
       <c r="E180" s="31"/>
-      <c r="F180" s="35"/>
-      <c r="G180" s="36"/>
-      <c r="H180" s="37"/>
-    </row>
-    <row r="181" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F180" s="38"/>
+      <c r="G180" s="39"/>
+      <c r="H180" s="40"/>
+    </row>
+    <row r="181" spans="1:8" ht="39" customHeight="1">
       <c r="A181" s="29"/>
       <c r="B181" s="30"/>
       <c r="C181" s="30"/>
       <c r="D181" s="31"/>
       <c r="E181" s="31"/>
-      <c r="F181" s="35"/>
-      <c r="G181" s="36"/>
-      <c r="H181" s="37"/>
-    </row>
-    <row r="182" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F181" s="38"/>
+      <c r="G181" s="39"/>
+      <c r="H181" s="40"/>
+    </row>
+    <row r="182" spans="1:8" ht="39" customHeight="1">
       <c r="A182" s="29"/>
       <c r="B182" s="30"/>
       <c r="C182" s="30"/>
       <c r="D182" s="31"/>
       <c r="E182" s="31"/>
-      <c r="F182" s="35"/>
-      <c r="G182" s="36"/>
-      <c r="H182" s="37"/>
-    </row>
-    <row r="183" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F182" s="38"/>
+      <c r="G182" s="39"/>
+      <c r="H182" s="40"/>
+    </row>
+    <row r="183" spans="1:8" ht="39" customHeight="1">
       <c r="A183" s="29"/>
       <c r="B183" s="30"/>
       <c r="C183" s="30"/>
       <c r="D183" s="31"/>
       <c r="E183" s="31"/>
-      <c r="F183" s="35"/>
-      <c r="G183" s="36"/>
-      <c r="H183" s="37"/>
-    </row>
-    <row r="184" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F183" s="38"/>
+      <c r="G183" s="39"/>
+      <c r="H183" s="40"/>
+    </row>
+    <row r="184" spans="1:8" ht="39" customHeight="1">
       <c r="A184" s="29"/>
       <c r="B184" s="30"/>
       <c r="C184" s="30"/>
       <c r="D184" s="31"/>
       <c r="E184" s="31"/>
-      <c r="F184" s="35"/>
-      <c r="G184" s="36"/>
-      <c r="H184" s="37"/>
-    </row>
-    <row r="185" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F184" s="38"/>
+      <c r="G184" s="39"/>
+      <c r="H184" s="40"/>
+    </row>
+    <row r="185" spans="1:8" ht="39" customHeight="1">
       <c r="A185" s="29"/>
       <c r="B185" s="30"/>
       <c r="C185" s="30"/>
       <c r="D185" s="31"/>
       <c r="E185" s="31"/>
-      <c r="F185" s="35"/>
-      <c r="G185" s="36"/>
-      <c r="H185" s="37"/>
-    </row>
-    <row r="186" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F185" s="38"/>
+      <c r="G185" s="39"/>
+      <c r="H185" s="40"/>
+    </row>
+    <row r="186" spans="1:8" ht="39" customHeight="1">
       <c r="A186" s="29"/>
       <c r="B186" s="30"/>
       <c r="C186" s="30"/>
       <c r="D186" s="31"/>
       <c r="E186" s="31"/>
-      <c r="F186" s="35"/>
-      <c r="G186" s="36"/>
-      <c r="H186" s="37"/>
-    </row>
-    <row r="187" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F186" s="38"/>
+      <c r="G186" s="39"/>
+      <c r="H186" s="40"/>
+    </row>
+    <row r="187" spans="1:8" ht="39" customHeight="1">
       <c r="A187" s="29"/>
       <c r="B187" s="30"/>
       <c r="C187" s="30"/>
       <c r="D187" s="31"/>
       <c r="E187" s="31"/>
-      <c r="F187" s="35"/>
-      <c r="G187" s="36"/>
-      <c r="H187" s="37"/>
-    </row>
-    <row r="188" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F187" s="38"/>
+      <c r="G187" s="39"/>
+      <c r="H187" s="40"/>
+    </row>
+    <row r="188" spans="1:8" ht="39" customHeight="1">
       <c r="A188" s="29"/>
       <c r="B188" s="30"/>
       <c r="C188" s="30"/>
       <c r="D188" s="31"/>
       <c r="E188" s="31"/>
-      <c r="F188" s="35"/>
-      <c r="G188" s="36"/>
-      <c r="H188" s="37"/>
-    </row>
-    <row r="189" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F188" s="38"/>
+      <c r="G188" s="39"/>
+      <c r="H188" s="40"/>
+    </row>
+    <row r="189" spans="1:8" ht="39" customHeight="1">
       <c r="A189" s="29"/>
       <c r="B189" s="30"/>
       <c r="C189" s="30"/>
       <c r="D189" s="31"/>
       <c r="E189" s="31"/>
-      <c r="F189" s="35"/>
-      <c r="G189" s="36"/>
-      <c r="H189" s="37"/>
-    </row>
-    <row r="190" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F189" s="38"/>
+      <c r="G189" s="39"/>
+      <c r="H189" s="40"/>
+    </row>
+    <row r="190" spans="1:8" ht="39" customHeight="1">
       <c r="A190" s="29"/>
       <c r="B190" s="30"/>
       <c r="C190" s="30"/>
       <c r="D190" s="31"/>
       <c r="E190" s="31"/>
-      <c r="F190" s="35"/>
-      <c r="G190" s="36"/>
-      <c r="H190" s="37"/>
-    </row>
-    <row r="191" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F190" s="38"/>
+      <c r="G190" s="39"/>
+      <c r="H190" s="40"/>
+    </row>
+    <row r="191" spans="1:8" ht="39" customHeight="1">
       <c r="A191" s="29"/>
       <c r="B191" s="30"/>
       <c r="C191" s="30"/>
       <c r="D191" s="31"/>
       <c r="E191" s="31"/>
-      <c r="F191" s="35"/>
-      <c r="G191" s="36"/>
-      <c r="H191" s="37"/>
-    </row>
-    <row r="192" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F191" s="38"/>
+      <c r="G191" s="39"/>
+      <c r="H191" s="40"/>
+    </row>
+    <row r="192" spans="1:8" ht="39" customHeight="1">
       <c r="A192" s="29"/>
       <c r="B192" s="30"/>
       <c r="C192" s="30"/>
       <c r="D192" s="31"/>
       <c r="E192" s="31"/>
-      <c r="F192" s="35"/>
-      <c r="G192" s="36"/>
-      <c r="H192" s="37"/>
-    </row>
-    <row r="193" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F192" s="38"/>
+      <c r="G192" s="39"/>
+      <c r="H192" s="40"/>
+    </row>
+    <row r="193" spans="1:8" ht="39" customHeight="1">
       <c r="A193" s="29"/>
       <c r="B193" s="30"/>
       <c r="C193" s="30"/>
       <c r="D193" s="31"/>
       <c r="E193" s="31"/>
-      <c r="F193" s="35"/>
-      <c r="G193" s="36"/>
-      <c r="H193" s="37"/>
-    </row>
-    <row r="194" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F193" s="38"/>
+      <c r="G193" s="39"/>
+      <c r="H193" s="40"/>
+    </row>
+    <row r="194" spans="1:8" ht="39" customHeight="1">
       <c r="A194" s="29"/>
       <c r="B194" s="30"/>
       <c r="C194" s="30"/>
       <c r="D194" s="31"/>
       <c r="E194" s="31"/>
-      <c r="F194" s="35"/>
-      <c r="G194" s="36"/>
-      <c r="H194" s="37"/>
-    </row>
-    <row r="195" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F194" s="38"/>
+      <c r="G194" s="39"/>
+      <c r="H194" s="40"/>
+    </row>
+    <row r="195" spans="1:8" ht="39" customHeight="1">
       <c r="A195" s="29"/>
       <c r="B195" s="30"/>
       <c r="C195" s="30"/>
       <c r="D195" s="31"/>
       <c r="E195" s="31"/>
-      <c r="F195" s="35"/>
-      <c r="G195" s="36"/>
-      <c r="H195" s="37"/>
-    </row>
-    <row r="196" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F195" s="38"/>
+      <c r="G195" s="39"/>
+      <c r="H195" s="40"/>
+    </row>
+    <row r="196" spans="1:8" ht="39" customHeight="1">
       <c r="A196" s="29"/>
       <c r="B196" s="30"/>
       <c r="C196" s="30"/>
       <c r="D196" s="31"/>
       <c r="E196" s="31"/>
-      <c r="F196" s="35"/>
-      <c r="G196" s="36"/>
-      <c r="H196" s="37"/>
-    </row>
-    <row r="197" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F196" s="38"/>
+      <c r="G196" s="39"/>
+      <c r="H196" s="40"/>
+    </row>
+    <row r="197" spans="1:8" ht="39" customHeight="1">
       <c r="A197" s="29"/>
       <c r="B197" s="30"/>
       <c r="C197" s="30"/>
       <c r="D197" s="31"/>
       <c r="E197" s="31"/>
-      <c r="F197" s="35"/>
-      <c r="G197" s="36"/>
-      <c r="H197" s="37"/>
-    </row>
-    <row r="198" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F197" s="38"/>
+      <c r="G197" s="39"/>
+      <c r="H197" s="40"/>
+    </row>
+    <row r="198" spans="1:8" ht="39" customHeight="1">
       <c r="A198" s="29"/>
       <c r="B198" s="30"/>
       <c r="C198" s="30"/>
       <c r="D198" s="31"/>
       <c r="E198" s="31"/>
-      <c r="F198" s="35"/>
-      <c r="G198" s="36"/>
-      <c r="H198" s="37"/>
-    </row>
-    <row r="199" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F198" s="38"/>
+      <c r="G198" s="39"/>
+      <c r="H198" s="40"/>
+    </row>
+    <row r="199" spans="1:8" ht="39" customHeight="1">
       <c r="A199" s="29"/>
       <c r="B199" s="30"/>
       <c r="C199" s="30"/>
       <c r="D199" s="31"/>
       <c r="E199" s="31"/>
-      <c r="F199" s="35"/>
-      <c r="G199" s="36"/>
-      <c r="H199" s="37"/>
-    </row>
-    <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F199" s="38"/>
+      <c r="G199" s="39"/>
+      <c r="H199" s="40"/>
+    </row>
+    <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1">
       <c r="A200" s="32"/>
       <c r="B200" s="33"/>
       <c r="C200" s="33"/>
       <c r="D200" s="34"/>
       <c r="E200" s="34"/>
-      <c r="F200" s="38"/>
-      <c r="G200" s="39"/>
-      <c r="H200" s="40"/>
-    </row>
-    <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F200" s="59"/>
+      <c r="G200" s="60"/>
+      <c r="H200" s="61"/>
+    </row>
+    <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="204">
+    <mergeCell ref="F196:H196"/>
+    <mergeCell ref="F197:H197"/>
+    <mergeCell ref="F198:H198"/>
+    <mergeCell ref="F199:H199"/>
+    <mergeCell ref="F200:H200"/>
+    <mergeCell ref="F191:H191"/>
+    <mergeCell ref="F192:H192"/>
+    <mergeCell ref="F193:H193"/>
+    <mergeCell ref="F194:H194"/>
+    <mergeCell ref="F195:H195"/>
+    <mergeCell ref="F186:H186"/>
+    <mergeCell ref="F187:H187"/>
+    <mergeCell ref="F188:H188"/>
+    <mergeCell ref="F189:H189"/>
+    <mergeCell ref="F190:H190"/>
+    <mergeCell ref="F181:H181"/>
+    <mergeCell ref="F182:H182"/>
+    <mergeCell ref="F183:H183"/>
+    <mergeCell ref="F184:H184"/>
+    <mergeCell ref="F185:H185"/>
+    <mergeCell ref="F176:H176"/>
+    <mergeCell ref="F177:H177"/>
+    <mergeCell ref="F178:H178"/>
+    <mergeCell ref="F179:H179"/>
+    <mergeCell ref="F180:H180"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="F172:H172"/>
+    <mergeCell ref="F173:H173"/>
+    <mergeCell ref="F174:H174"/>
+    <mergeCell ref="F175:H175"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="F167:H167"/>
+    <mergeCell ref="F168:H168"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="F170:H170"/>
+    <mergeCell ref="F161:H161"/>
+    <mergeCell ref="F162:H162"/>
+    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="F164:H164"/>
+    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="F156:H156"/>
+    <mergeCell ref="F157:H157"/>
+    <mergeCell ref="F158:H158"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="F152:H152"/>
+    <mergeCell ref="F153:H153"/>
+    <mergeCell ref="F154:H154"/>
+    <mergeCell ref="F155:H155"/>
+    <mergeCell ref="F146:H146"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F148:H148"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="F150:H150"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="F144:H144"/>
+    <mergeCell ref="F145:H145"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -3741,200 +3917,10 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F146:H146"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F148:H148"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="F150:H150"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="F143:H143"/>
-    <mergeCell ref="F144:H144"/>
-    <mergeCell ref="F145:H145"/>
-    <mergeCell ref="F156:H156"/>
-    <mergeCell ref="F157:H157"/>
-    <mergeCell ref="F158:H158"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="F151:H151"/>
-    <mergeCell ref="F152:H152"/>
-    <mergeCell ref="F153:H153"/>
-    <mergeCell ref="F154:H154"/>
-    <mergeCell ref="F155:H155"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="F167:H167"/>
-    <mergeCell ref="F168:H168"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="F170:H170"/>
-    <mergeCell ref="F161:H161"/>
-    <mergeCell ref="F162:H162"/>
-    <mergeCell ref="F163:H163"/>
-    <mergeCell ref="F164:H164"/>
-    <mergeCell ref="F165:H165"/>
-    <mergeCell ref="F176:H176"/>
-    <mergeCell ref="F177:H177"/>
-    <mergeCell ref="F178:H178"/>
-    <mergeCell ref="F179:H179"/>
-    <mergeCell ref="F180:H180"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="F172:H172"/>
-    <mergeCell ref="F173:H173"/>
-    <mergeCell ref="F174:H174"/>
-    <mergeCell ref="F175:H175"/>
-    <mergeCell ref="F186:H186"/>
-    <mergeCell ref="F187:H187"/>
-    <mergeCell ref="F188:H188"/>
-    <mergeCell ref="F189:H189"/>
-    <mergeCell ref="F190:H190"/>
-    <mergeCell ref="F181:H181"/>
-    <mergeCell ref="F182:H182"/>
-    <mergeCell ref="F183:H183"/>
-    <mergeCell ref="F184:H184"/>
-    <mergeCell ref="F185:H185"/>
-    <mergeCell ref="F196:H196"/>
-    <mergeCell ref="F197:H197"/>
-    <mergeCell ref="F198:H198"/>
-    <mergeCell ref="F199:H199"/>
-    <mergeCell ref="F200:H200"/>
-    <mergeCell ref="F191:H191"/>
-    <mergeCell ref="F192:H192"/>
-    <mergeCell ref="F193:H193"/>
-    <mergeCell ref="F194:H194"/>
-    <mergeCell ref="F195:H195"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -3951,15 +3937,15 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="14" customWidth="1"/>
     <col min="2" max="4" width="15" style="14" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="14" customWidth="1"/>
     <col min="6" max="16384" width="15" style="14" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="36" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -3970,7 +3956,7 @@
       <c r="D1" s="62"/>
       <c r="E1" s="63"/>
     </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="36" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
@@ -3981,7 +3967,7 @@
       <c r="D2" s="64"/>
       <c r="E2" s="65"/>
     </row>
-    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="136" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -3990,7 +3976,7 @@
       <c r="D3" s="66"/>
       <c r="E3" s="67"/>
     </row>
-    <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="46" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -3999,7 +3985,7 @@
       <c r="D4" s="71"/>
       <c r="E4" s="72"/>
     </row>
-    <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="46" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
@@ -4008,7 +3994,7 @@
       <c r="D5" s="66"/>
       <c r="E5" s="67"/>
     </row>
-    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="46" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -4017,7 +4003,7 @@
       <c r="D6" s="66"/>
       <c r="E6" s="67"/>
     </row>
-    <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="46" customHeight="1">
       <c r="A7" s="17" t="s">
         <v>56</v>
       </c>
@@ -4026,7 +4012,7 @@
       <c r="D7" s="71"/>
       <c r="E7" s="72"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>30</v>
       </c>
@@ -4048,7 +4034,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -4061,19 +4047,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G18"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="36" customHeight="1">
       <c r="A1" s="73" t="s">
         <v>23</v>
       </c>
@@ -4084,52 +4070,54 @@
       <c r="F1" s="74"/>
       <c r="G1" s="75"/>
     </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="36" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="77"/>
-    </row>
-    <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="67"/>
+    </row>
+    <row r="4" spans="1:7" ht="112" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="77"/>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67"/>
+    </row>
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="79"/>
-    </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="69"/>
+    </row>
+    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:7" ht="36" customHeight="1">
       <c r="A7" s="73" t="s">
         <v>27</v>
       </c>
@@ -4140,7 +4128,7 @@
       <c r="F7" s="74"/>
       <c r="G7" s="75"/>
     </row>
-    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="36" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -4151,7 +4139,7 @@
       <c r="F8" s="66"/>
       <c r="G8" s="67"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="36" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
@@ -4162,7 +4150,7 @@
       <c r="F9" s="66"/>
       <c r="G9" s="67"/>
     </row>
-    <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="112" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
@@ -4173,7 +4161,7 @@
       <c r="F10" s="66"/>
       <c r="G10" s="67"/>
     </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -4184,9 +4172,9 @@
       <c r="F11" s="68"/>
       <c r="G11" s="69"/>
     </row>
-    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="36" customHeight="1"/>
+    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
+    <row r="14" spans="1:7" ht="36" customHeight="1">
       <c r="A14" s="73" t="s">
         <v>28</v>
       </c>
@@ -4197,7 +4185,7 @@
       <c r="F14" s="74"/>
       <c r="G14" s="75"/>
     </row>
-    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="36" customHeight="1">
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
@@ -4208,7 +4196,7 @@
       <c r="F15" s="66"/>
       <c r="G15" s="67"/>
     </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="36" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
@@ -4219,7 +4207,7 @@
       <c r="F16" s="66"/>
       <c r="G16" s="67"/>
     </row>
-    <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="113" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>6</v>
       </c>
@@ -4230,7 +4218,7 @@
       <c r="F17" s="66"/>
       <c r="G17" s="67"/>
     </row>
-    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A18" s="16" t="s">
         <v>26</v>
       </c>
@@ -4241,29 +4229,29 @@
       <c r="F18" s="68"/>
       <c r="G18" s="69"/>
     </row>
-    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="36" customHeight="1"/>
+    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added a small amount of analysis code
</commit_message>
<xml_diff>
--- a/EMX_3.xlsx
+++ b/EMX_3.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
     <sheet name="Physiology" sheetId="2" r:id="rId2"/>
-    <sheet name="Histology" sheetId="3" r:id="rId3"/>
-    <sheet name="Surgery" sheetId="4" r:id="rId4"/>
+    <sheet name="Analysis" sheetId="5" r:id="rId3"/>
+    <sheet name="Histology" sheetId="3" r:id="rId4"/>
+    <sheet name="Surgery" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -288,6 +289,15 @@
   </si>
   <si>
     <t>Burr hole injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED </t>
+  </si>
+  <si>
+    <t>Vcmd to led</t>
+  </si>
+  <si>
+    <t>epsc peak</t>
   </si>
 </sst>
 </file>
@@ -954,6 +964,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -963,6 +982,60 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -971,69 +1044,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1508,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1526,16 +1536,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="59" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
       <c r="G1" s="21" t="s">
         <v>31</v>
       </c>
@@ -1544,16 +1554,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="22" t="s">
         <v>31</v>
       </c>
@@ -1562,42 +1572,42 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1615,11 +1625,11 @@
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
@@ -1631,11 +1641,11 @@
       <c r="C7" s="30"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
@@ -1649,11 +1659,11 @@
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
@@ -1667,11 +1677,11 @@
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
     </row>
     <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
@@ -1685,11 +1695,11 @@
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
@@ -1703,11 +1713,11 @@
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
@@ -1721,11 +1731,11 @@
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
@@ -1737,11 +1747,11 @@
       <c r="C13" s="30"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="37"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
@@ -1753,9 +1763,9 @@
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
     </row>
     <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
@@ -1767,9 +1777,9 @@
       <c r="C15" s="30"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
@@ -1781,9 +1791,9 @@
       <c r="C16" s="30"/>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
     </row>
     <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
@@ -1795,9 +1805,9 @@
       <c r="C17" s="30"/>
       <c r="D17" s="31"/>
       <c r="E17" s="31"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
@@ -1809,9 +1819,9 @@
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
     </row>
     <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
@@ -1825,11 +1835,11 @@
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
@@ -1841,11 +1851,11 @@
       <c r="C20" s="30"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
@@ -1857,11 +1867,11 @@
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="37"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
@@ -1873,9 +1883,9 @@
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="40"/>
     </row>
     <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
@@ -1887,9 +1897,9 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="40"/>
     </row>
     <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
@@ -1901,9 +1911,9 @@
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
@@ -1915,9 +1925,9 @@
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="37"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
@@ -1929,11 +1939,11 @@
       <c r="C26" s="30"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
@@ -1945,9 +1955,9 @@
       <c r="C27" s="30"/>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
@@ -1959,9 +1969,9 @@
       <c r="C28" s="30"/>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
     </row>
     <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
@@ -1973,11 +1983,11 @@
       <c r="C29" s="30"/>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
@@ -1991,11 +2001,11 @@
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
@@ -2007,9 +2017,9 @@
       <c r="C31" s="30"/>
       <c r="D31" s="31"/>
       <c r="E31" s="31"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
@@ -2021,9 +2031,9 @@
       <c r="C32" s="30"/>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
@@ -2035,9 +2045,9 @@
       <c r="C33" s="30"/>
       <c r="D33" s="31"/>
       <c r="E33" s="31"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
@@ -2049,11 +2059,11 @@
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="40"/>
     </row>
     <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29"/>
@@ -2061,9 +2071,9 @@
       <c r="C35" s="30"/>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="40"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29"/>
@@ -2071,9 +2081,9 @@
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="40"/>
     </row>
     <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
@@ -2081,9 +2091,9 @@
       <c r="C37" s="30"/>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29"/>
@@ -2091,9 +2101,9 @@
       <c r="C38" s="30"/>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="37"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
     </row>
     <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
@@ -2101,9 +2111,9 @@
       <c r="C39" s="30"/>
       <c r="D39" s="31"/>
       <c r="E39" s="31"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
@@ -2111,9 +2121,9 @@
       <c r="C40" s="30"/>
       <c r="D40" s="31"/>
       <c r="E40" s="31"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="37"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
     </row>
     <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
@@ -2121,9 +2131,9 @@
       <c r="C41" s="30"/>
       <c r="D41" s="31"/>
       <c r="E41" s="31"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="37"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="40"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29"/>
@@ -2131,9 +2141,9 @@
       <c r="C42" s="30"/>
       <c r="D42" s="31"/>
       <c r="E42" s="31"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="37"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="40"/>
     </row>
     <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
@@ -2141,9 +2151,9 @@
       <c r="C43" s="30"/>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="37"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="40"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
@@ -2151,9 +2161,9 @@
       <c r="C44" s="30"/>
       <c r="D44" s="31"/>
       <c r="E44" s="31"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="37"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="40"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29"/>
@@ -2161,9 +2171,9 @@
       <c r="C45" s="30"/>
       <c r="D45" s="31"/>
       <c r="E45" s="31"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="40"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="29"/>
@@ -2171,9 +2181,9 @@
       <c r="C46" s="30"/>
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="29"/>
@@ -2181,9 +2191,9 @@
       <c r="C47" s="30"/>
       <c r="D47" s="31"/>
       <c r="E47" s="31"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="37"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
     </row>
     <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="29"/>
@@ -2191,9 +2201,9 @@
       <c r="C48" s="30"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="37"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="40"/>
     </row>
     <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
@@ -2201,9 +2211,9 @@
       <c r="C49" s="30"/>
       <c r="D49" s="31"/>
       <c r="E49" s="31"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="37"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="40"/>
     </row>
     <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="29"/>
@@ -2211,9 +2221,9 @@
       <c r="C50" s="30"/>
       <c r="D50" s="31"/>
       <c r="E50" s="31"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="37"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="40"/>
     </row>
     <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="29"/>
@@ -2221,9 +2231,9 @@
       <c r="C51" s="30"/>
       <c r="D51" s="31"/>
       <c r="E51" s="31"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="37"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="40"/>
     </row>
     <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="29"/>
@@ -2231,9 +2241,9 @@
       <c r="C52" s="30"/>
       <c r="D52" s="31"/>
       <c r="E52" s="31"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="37"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="40"/>
     </row>
     <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="29"/>
@@ -2241,9 +2251,9 @@
       <c r="C53" s="30"/>
       <c r="D53" s="31"/>
       <c r="E53" s="31"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="40"/>
     </row>
     <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="29"/>
@@ -2251,9 +2261,9 @@
       <c r="C54" s="30"/>
       <c r="D54" s="31"/>
       <c r="E54" s="31"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="37"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="40"/>
     </row>
     <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="29"/>
@@ -2261,9 +2271,9 @@
       <c r="C55" s="30"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="37"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="40"/>
     </row>
     <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29"/>
@@ -2271,9 +2281,9 @@
       <c r="C56" s="30"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="37"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="40"/>
     </row>
     <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="29"/>
@@ -2281,9 +2291,9 @@
       <c r="C57" s="30"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="37"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="40"/>
     </row>
     <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="29"/>
@@ -2291,9 +2301,9 @@
       <c r="C58" s="30"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="37"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="40"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="29"/>
@@ -2301,9 +2311,9 @@
       <c r="C59" s="30"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="37"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="40"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="29"/>
@@ -2311,9 +2321,9 @@
       <c r="C60" s="30"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="37"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="40"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="29"/>
@@ -2321,9 +2331,9 @@
       <c r="C61" s="30"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="37"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="40"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
@@ -2331,9 +2341,9 @@
       <c r="C62" s="30"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="37"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="40"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="29"/>
@@ -2341,9 +2351,9 @@
       <c r="C63" s="30"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="37"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="40"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
@@ -2351,9 +2361,9 @@
       <c r="C64" s="30"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="37"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="40"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="29"/>
@@ -2361,9 +2371,9 @@
       <c r="C65" s="30"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="37"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="40"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="29"/>
@@ -2371,9 +2381,9 @@
       <c r="C66" s="30"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="37"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="40"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="29"/>
@@ -2381,9 +2391,9 @@
       <c r="C67" s="30"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="37"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="40"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="29"/>
@@ -2391,9 +2401,9 @@
       <c r="C68" s="30"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="37"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="40"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="29"/>
@@ -2401,9 +2411,9 @@
       <c r="C69" s="30"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="37"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="29"/>
@@ -2411,9 +2421,9 @@
       <c r="C70" s="30"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="37"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="40"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="29"/>
@@ -2421,9 +2431,9 @@
       <c r="C71" s="30"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="37"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="40"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="29"/>
@@ -2431,9 +2441,9 @@
       <c r="C72" s="30"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="37"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="40"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="29"/>
@@ -2441,9 +2451,9 @@
       <c r="C73" s="30"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="37"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="40"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="29"/>
@@ -2451,9 +2461,9 @@
       <c r="C74" s="30"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="37"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="40"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="29"/>
@@ -2461,9 +2471,9 @@
       <c r="C75" s="30"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="37"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="40"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="29"/>
@@ -2471,9 +2481,9 @@
       <c r="C76" s="30"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
-      <c r="F76" s="35"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="37"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="39"/>
+      <c r="H76" s="40"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="29"/>
@@ -2481,9 +2491,9 @@
       <c r="C77" s="30"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="37"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="39"/>
+      <c r="H77" s="40"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="29"/>
@@ -2491,9 +2501,9 @@
       <c r="C78" s="30"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="37"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="40"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="29"/>
@@ -2501,9 +2511,9 @@
       <c r="C79" s="30"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="36"/>
-      <c r="H79" s="37"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="40"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="29"/>
@@ -2511,9 +2521,9 @@
       <c r="C80" s="30"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="37"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="40"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="29"/>
@@ -2521,9 +2531,9 @@
       <c r="C81" s="30"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="37"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="40"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="29"/>
@@ -2531,9 +2541,9 @@
       <c r="C82" s="30"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="37"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="40"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="29"/>
@@ -2541,9 +2551,9 @@
       <c r="C83" s="30"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="37"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="40"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="29"/>
@@ -2551,9 +2561,9 @@
       <c r="C84" s="30"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
-      <c r="F84" s="35"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="37"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
+      <c r="H84" s="40"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="29"/>
@@ -2561,9 +2571,9 @@
       <c r="C85" s="30"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="37"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="40"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="29"/>
@@ -2571,9 +2581,9 @@
       <c r="C86" s="30"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="37"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="40"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="29"/>
@@ -2581,9 +2591,9 @@
       <c r="C87" s="30"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="36"/>
-      <c r="H87" s="37"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="40"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="29"/>
@@ -2591,9 +2601,9 @@
       <c r="C88" s="30"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="37"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="40"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="29"/>
@@ -2601,9 +2611,9 @@
       <c r="C89" s="30"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="36"/>
-      <c r="H89" s="37"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="40"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="29"/>
@@ -2611,9 +2621,9 @@
       <c r="C90" s="30"/>
       <c r="D90" s="31"/>
       <c r="E90" s="31"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="36"/>
-      <c r="H90" s="37"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="40"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="29"/>
@@ -2621,9 +2631,9 @@
       <c r="C91" s="30"/>
       <c r="D91" s="31"/>
       <c r="E91" s="31"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="36"/>
-      <c r="H91" s="37"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="40"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="29"/>
@@ -2631,9 +2641,9 @@
       <c r="C92" s="30"/>
       <c r="D92" s="31"/>
       <c r="E92" s="31"/>
-      <c r="F92" s="35"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="37"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="40"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="29"/>
@@ -2641,9 +2651,9 @@
       <c r="C93" s="30"/>
       <c r="D93" s="31"/>
       <c r="E93" s="31"/>
-      <c r="F93" s="35"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="37"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="40"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="29"/>
@@ -2651,9 +2661,9 @@
       <c r="C94" s="30"/>
       <c r="D94" s="31"/>
       <c r="E94" s="31"/>
-      <c r="F94" s="35"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="37"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="40"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
@@ -2661,9 +2671,9 @@
       <c r="C95" s="30"/>
       <c r="D95" s="31"/>
       <c r="E95" s="31"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="37"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="39"/>
+      <c r="H95" s="40"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
@@ -2671,9 +2681,9 @@
       <c r="C96" s="30"/>
       <c r="D96" s="31"/>
       <c r="E96" s="31"/>
-      <c r="F96" s="35"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="37"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="39"/>
+      <c r="H96" s="40"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
@@ -2681,9 +2691,9 @@
       <c r="C97" s="30"/>
       <c r="D97" s="31"/>
       <c r="E97" s="31"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="36"/>
-      <c r="H97" s="37"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="39"/>
+      <c r="H97" s="40"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="29"/>
@@ -2691,9 +2701,9 @@
       <c r="C98" s="30"/>
       <c r="D98" s="31"/>
       <c r="E98" s="31"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="37"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="39"/>
+      <c r="H98" s="40"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="29"/>
@@ -2701,9 +2711,9 @@
       <c r="C99" s="30"/>
       <c r="D99" s="31"/>
       <c r="E99" s="31"/>
-      <c r="F99" s="35"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="37"/>
+      <c r="F99" s="38"/>
+      <c r="G99" s="39"/>
+      <c r="H99" s="40"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="29"/>
@@ -2711,9 +2721,9 @@
       <c r="C100" s="30"/>
       <c r="D100" s="31"/>
       <c r="E100" s="31"/>
-      <c r="F100" s="35"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="37"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="39"/>
+      <c r="H100" s="40"/>
     </row>
     <row r="101" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="29"/>
@@ -2721,9 +2731,9 @@
       <c r="C101" s="30"/>
       <c r="D101" s="31"/>
       <c r="E101" s="31"/>
-      <c r="F101" s="35"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="37"/>
+      <c r="F101" s="38"/>
+      <c r="G101" s="39"/>
+      <c r="H101" s="40"/>
     </row>
     <row r="102" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
@@ -2731,9 +2741,9 @@
       <c r="C102" s="30"/>
       <c r="D102" s="31"/>
       <c r="E102" s="31"/>
-      <c r="F102" s="35"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="37"/>
+      <c r="F102" s="38"/>
+      <c r="G102" s="39"/>
+      <c r="H102" s="40"/>
     </row>
     <row r="103" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29"/>
@@ -2741,9 +2751,9 @@
       <c r="C103" s="30"/>
       <c r="D103" s="31"/>
       <c r="E103" s="31"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="37"/>
+      <c r="F103" s="38"/>
+      <c r="G103" s="39"/>
+      <c r="H103" s="40"/>
     </row>
     <row r="104" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
@@ -2751,9 +2761,9 @@
       <c r="C104" s="30"/>
       <c r="D104" s="31"/>
       <c r="E104" s="31"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="36"/>
-      <c r="H104" s="37"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="39"/>
+      <c r="H104" s="40"/>
     </row>
     <row r="105" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
@@ -2761,9 +2771,9 @@
       <c r="C105" s="30"/>
       <c r="D105" s="31"/>
       <c r="E105" s="31"/>
-      <c r="F105" s="35"/>
-      <c r="G105" s="36"/>
-      <c r="H105" s="37"/>
+      <c r="F105" s="38"/>
+      <c r="G105" s="39"/>
+      <c r="H105" s="40"/>
     </row>
     <row r="106" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
@@ -2771,9 +2781,9 @@
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="31"/>
-      <c r="F106" s="35"/>
-      <c r="G106" s="36"/>
-      <c r="H106" s="37"/>
+      <c r="F106" s="38"/>
+      <c r="G106" s="39"/>
+      <c r="H106" s="40"/>
     </row>
     <row r="107" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="29"/>
@@ -2781,9 +2791,9 @@
       <c r="C107" s="30"/>
       <c r="D107" s="31"/>
       <c r="E107" s="31"/>
-      <c r="F107" s="35"/>
-      <c r="G107" s="36"/>
-      <c r="H107" s="37"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="39"/>
+      <c r="H107" s="40"/>
     </row>
     <row r="108" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="29"/>
@@ -2791,9 +2801,9 @@
       <c r="C108" s="30"/>
       <c r="D108" s="31"/>
       <c r="E108" s="31"/>
-      <c r="F108" s="35"/>
-      <c r="G108" s="36"/>
-      <c r="H108" s="37"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="39"/>
+      <c r="H108" s="40"/>
     </row>
     <row r="109" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="29"/>
@@ -2801,9 +2811,9 @@
       <c r="C109" s="30"/>
       <c r="D109" s="31"/>
       <c r="E109" s="31"/>
-      <c r="F109" s="35"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="37"/>
+      <c r="F109" s="38"/>
+      <c r="G109" s="39"/>
+      <c r="H109" s="40"/>
     </row>
     <row r="110" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="29"/>
@@ -2811,9 +2821,9 @@
       <c r="C110" s="30"/>
       <c r="D110" s="31"/>
       <c r="E110" s="31"/>
-      <c r="F110" s="35"/>
-      <c r="G110" s="36"/>
-      <c r="H110" s="37"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="39"/>
+      <c r="H110" s="40"/>
     </row>
     <row r="111" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="29"/>
@@ -2821,9 +2831,9 @@
       <c r="C111" s="30"/>
       <c r="D111" s="31"/>
       <c r="E111" s="31"/>
-      <c r="F111" s="35"/>
-      <c r="G111" s="36"/>
-      <c r="H111" s="37"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="39"/>
+      <c r="H111" s="40"/>
     </row>
     <row r="112" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="29"/>
@@ -2831,9 +2841,9 @@
       <c r="C112" s="30"/>
       <c r="D112" s="31"/>
       <c r="E112" s="31"/>
-      <c r="F112" s="35"/>
-      <c r="G112" s="36"/>
-      <c r="H112" s="37"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="39"/>
+      <c r="H112" s="40"/>
     </row>
     <row r="113" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="29"/>
@@ -2841,9 +2851,9 @@
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
       <c r="E113" s="31"/>
-      <c r="F113" s="35"/>
-      <c r="G113" s="36"/>
-      <c r="H113" s="37"/>
+      <c r="F113" s="38"/>
+      <c r="G113" s="39"/>
+      <c r="H113" s="40"/>
     </row>
     <row r="114" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="29"/>
@@ -2851,9 +2861,9 @@
       <c r="C114" s="30"/>
       <c r="D114" s="31"/>
       <c r="E114" s="31"/>
-      <c r="F114" s="35"/>
-      <c r="G114" s="36"/>
-      <c r="H114" s="37"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="39"/>
+      <c r="H114" s="40"/>
     </row>
     <row r="115" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="29"/>
@@ -2861,9 +2871,9 @@
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
       <c r="E115" s="31"/>
-      <c r="F115" s="35"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="37"/>
+      <c r="F115" s="38"/>
+      <c r="G115" s="39"/>
+      <c r="H115" s="40"/>
     </row>
     <row r="116" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="29"/>
@@ -2871,9 +2881,9 @@
       <c r="C116" s="30"/>
       <c r="D116" s="31"/>
       <c r="E116" s="31"/>
-      <c r="F116" s="35"/>
-      <c r="G116" s="36"/>
-      <c r="H116" s="37"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="39"/>
+      <c r="H116" s="40"/>
     </row>
     <row r="117" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="29"/>
@@ -2881,9 +2891,9 @@
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
       <c r="E117" s="31"/>
-      <c r="F117" s="35"/>
-      <c r="G117" s="36"/>
-      <c r="H117" s="37"/>
+      <c r="F117" s="38"/>
+      <c r="G117" s="39"/>
+      <c r="H117" s="40"/>
     </row>
     <row r="118" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="29"/>
@@ -2891,9 +2901,9 @@
       <c r="C118" s="30"/>
       <c r="D118" s="31"/>
       <c r="E118" s="31"/>
-      <c r="F118" s="35"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="37"/>
+      <c r="F118" s="38"/>
+      <c r="G118" s="39"/>
+      <c r="H118" s="40"/>
     </row>
     <row r="119" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="29"/>
@@ -2901,9 +2911,9 @@
       <c r="C119" s="30"/>
       <c r="D119" s="31"/>
       <c r="E119" s="31"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="36"/>
-      <c r="H119" s="37"/>
+      <c r="F119" s="38"/>
+      <c r="G119" s="39"/>
+      <c r="H119" s="40"/>
     </row>
     <row r="120" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="29"/>
@@ -2911,9 +2921,9 @@
       <c r="C120" s="30"/>
       <c r="D120" s="31"/>
       <c r="E120" s="31"/>
-      <c r="F120" s="35"/>
-      <c r="G120" s="36"/>
-      <c r="H120" s="37"/>
+      <c r="F120" s="38"/>
+      <c r="G120" s="39"/>
+      <c r="H120" s="40"/>
     </row>
     <row r="121" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="29"/>
@@ -2921,9 +2931,9 @@
       <c r="C121" s="30"/>
       <c r="D121" s="31"/>
       <c r="E121" s="31"/>
-      <c r="F121" s="35"/>
-      <c r="G121" s="36"/>
-      <c r="H121" s="37"/>
+      <c r="F121" s="38"/>
+      <c r="G121" s="39"/>
+      <c r="H121" s="40"/>
     </row>
     <row r="122" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="29"/>
@@ -2931,9 +2941,9 @@
       <c r="C122" s="30"/>
       <c r="D122" s="31"/>
       <c r="E122" s="31"/>
-      <c r="F122" s="35"/>
-      <c r="G122" s="36"/>
-      <c r="H122" s="37"/>
+      <c r="F122" s="38"/>
+      <c r="G122" s="39"/>
+      <c r="H122" s="40"/>
     </row>
     <row r="123" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="29"/>
@@ -2941,9 +2951,9 @@
       <c r="C123" s="30"/>
       <c r="D123" s="31"/>
       <c r="E123" s="31"/>
-      <c r="F123" s="35"/>
-      <c r="G123" s="36"/>
-      <c r="H123" s="37"/>
+      <c r="F123" s="38"/>
+      <c r="G123" s="39"/>
+      <c r="H123" s="40"/>
     </row>
     <row r="124" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="29"/>
@@ -2951,9 +2961,9 @@
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
       <c r="E124" s="31"/>
-      <c r="F124" s="35"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="37"/>
+      <c r="F124" s="38"/>
+      <c r="G124" s="39"/>
+      <c r="H124" s="40"/>
     </row>
     <row r="125" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="29"/>
@@ -2961,9 +2971,9 @@
       <c r="C125" s="30"/>
       <c r="D125" s="31"/>
       <c r="E125" s="31"/>
-      <c r="F125" s="35"/>
-      <c r="G125" s="36"/>
-      <c r="H125" s="37"/>
+      <c r="F125" s="38"/>
+      <c r="G125" s="39"/>
+      <c r="H125" s="40"/>
     </row>
     <row r="126" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="29"/>
@@ -2971,9 +2981,9 @@
       <c r="C126" s="30"/>
       <c r="D126" s="31"/>
       <c r="E126" s="31"/>
-      <c r="F126" s="35"/>
-      <c r="G126" s="36"/>
-      <c r="H126" s="37"/>
+      <c r="F126" s="38"/>
+      <c r="G126" s="39"/>
+      <c r="H126" s="40"/>
     </row>
     <row r="127" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="29"/>
@@ -2981,9 +2991,9 @@
       <c r="C127" s="30"/>
       <c r="D127" s="31"/>
       <c r="E127" s="31"/>
-      <c r="F127" s="35"/>
-      <c r="G127" s="36"/>
-      <c r="H127" s="37"/>
+      <c r="F127" s="38"/>
+      <c r="G127" s="39"/>
+      <c r="H127" s="40"/>
     </row>
     <row r="128" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="29"/>
@@ -2991,9 +3001,9 @@
       <c r="C128" s="30"/>
       <c r="D128" s="31"/>
       <c r="E128" s="31"/>
-      <c r="F128" s="35"/>
-      <c r="G128" s="36"/>
-      <c r="H128" s="37"/>
+      <c r="F128" s="38"/>
+      <c r="G128" s="39"/>
+      <c r="H128" s="40"/>
     </row>
     <row r="129" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="29"/>
@@ -3001,9 +3011,9 @@
       <c r="C129" s="30"/>
       <c r="D129" s="31"/>
       <c r="E129" s="31"/>
-      <c r="F129" s="35"/>
-      <c r="G129" s="36"/>
-      <c r="H129" s="37"/>
+      <c r="F129" s="38"/>
+      <c r="G129" s="39"/>
+      <c r="H129" s="40"/>
     </row>
     <row r="130" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
@@ -3011,9 +3021,9 @@
       <c r="C130" s="30"/>
       <c r="D130" s="31"/>
       <c r="E130" s="31"/>
-      <c r="F130" s="35"/>
-      <c r="G130" s="36"/>
-      <c r="H130" s="37"/>
+      <c r="F130" s="38"/>
+      <c r="G130" s="39"/>
+      <c r="H130" s="40"/>
     </row>
     <row r="131" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
@@ -3021,9 +3031,9 @@
       <c r="C131" s="30"/>
       <c r="D131" s="31"/>
       <c r="E131" s="31"/>
-      <c r="F131" s="35"/>
-      <c r="G131" s="36"/>
-      <c r="H131" s="37"/>
+      <c r="F131" s="38"/>
+      <c r="G131" s="39"/>
+      <c r="H131" s="40"/>
     </row>
     <row r="132" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
@@ -3031,9 +3041,9 @@
       <c r="C132" s="30"/>
       <c r="D132" s="31"/>
       <c r="E132" s="31"/>
-      <c r="F132" s="35"/>
-      <c r="G132" s="36"/>
-      <c r="H132" s="37"/>
+      <c r="F132" s="38"/>
+      <c r="G132" s="39"/>
+      <c r="H132" s="40"/>
     </row>
     <row r="133" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="29"/>
@@ -3041,9 +3051,9 @@
       <c r="C133" s="30"/>
       <c r="D133" s="31"/>
       <c r="E133" s="31"/>
-      <c r="F133" s="35"/>
-      <c r="G133" s="36"/>
-      <c r="H133" s="37"/>
+      <c r="F133" s="38"/>
+      <c r="G133" s="39"/>
+      <c r="H133" s="40"/>
     </row>
     <row r="134" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="29"/>
@@ -3051,9 +3061,9 @@
       <c r="C134" s="30"/>
       <c r="D134" s="31"/>
       <c r="E134" s="31"/>
-      <c r="F134" s="35"/>
-      <c r="G134" s="36"/>
-      <c r="H134" s="37"/>
+      <c r="F134" s="38"/>
+      <c r="G134" s="39"/>
+      <c r="H134" s="40"/>
     </row>
     <row r="135" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="29"/>
@@ -3061,9 +3071,9 @@
       <c r="C135" s="30"/>
       <c r="D135" s="31"/>
       <c r="E135" s="31"/>
-      <c r="F135" s="35"/>
-      <c r="G135" s="36"/>
-      <c r="H135" s="37"/>
+      <c r="F135" s="38"/>
+      <c r="G135" s="39"/>
+      <c r="H135" s="40"/>
     </row>
     <row r="136" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="29"/>
@@ -3071,9 +3081,9 @@
       <c r="C136" s="30"/>
       <c r="D136" s="31"/>
       <c r="E136" s="31"/>
-      <c r="F136" s="35"/>
-      <c r="G136" s="36"/>
-      <c r="H136" s="37"/>
+      <c r="F136" s="38"/>
+      <c r="G136" s="39"/>
+      <c r="H136" s="40"/>
     </row>
     <row r="137" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
@@ -3081,9 +3091,9 @@
       <c r="C137" s="30"/>
       <c r="D137" s="31"/>
       <c r="E137" s="31"/>
-      <c r="F137" s="35"/>
-      <c r="G137" s="36"/>
-      <c r="H137" s="37"/>
+      <c r="F137" s="38"/>
+      <c r="G137" s="39"/>
+      <c r="H137" s="40"/>
     </row>
     <row r="138" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
@@ -3091,9 +3101,9 @@
       <c r="C138" s="30"/>
       <c r="D138" s="31"/>
       <c r="E138" s="31"/>
-      <c r="F138" s="35"/>
-      <c r="G138" s="36"/>
-      <c r="H138" s="37"/>
+      <c r="F138" s="38"/>
+      <c r="G138" s="39"/>
+      <c r="H138" s="40"/>
     </row>
     <row r="139" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
@@ -3101,9 +3111,9 @@
       <c r="C139" s="30"/>
       <c r="D139" s="31"/>
       <c r="E139" s="31"/>
-      <c r="F139" s="35"/>
-      <c r="G139" s="36"/>
-      <c r="H139" s="37"/>
+      <c r="F139" s="38"/>
+      <c r="G139" s="39"/>
+      <c r="H139" s="40"/>
     </row>
     <row r="140" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="29"/>
@@ -3111,9 +3121,9 @@
       <c r="C140" s="30"/>
       <c r="D140" s="31"/>
       <c r="E140" s="31"/>
-      <c r="F140" s="35"/>
-      <c r="G140" s="36"/>
-      <c r="H140" s="37"/>
+      <c r="F140" s="38"/>
+      <c r="G140" s="39"/>
+      <c r="H140" s="40"/>
     </row>
     <row r="141" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="29"/>
@@ -3121,9 +3131,9 @@
       <c r="C141" s="30"/>
       <c r="D141" s="31"/>
       <c r="E141" s="31"/>
-      <c r="F141" s="35"/>
-      <c r="G141" s="36"/>
-      <c r="H141" s="37"/>
+      <c r="F141" s="38"/>
+      <c r="G141" s="39"/>
+      <c r="H141" s="40"/>
     </row>
     <row r="142" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="29"/>
@@ -3131,9 +3141,9 @@
       <c r="C142" s="30"/>
       <c r="D142" s="31"/>
       <c r="E142" s="31"/>
-      <c r="F142" s="35"/>
-      <c r="G142" s="36"/>
-      <c r="H142" s="37"/>
+      <c r="F142" s="38"/>
+      <c r="G142" s="39"/>
+      <c r="H142" s="40"/>
     </row>
     <row r="143" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
@@ -3141,9 +3151,9 @@
       <c r="C143" s="30"/>
       <c r="D143" s="31"/>
       <c r="E143" s="31"/>
-      <c r="F143" s="35"/>
-      <c r="G143" s="36"/>
-      <c r="H143" s="37"/>
+      <c r="F143" s="38"/>
+      <c r="G143" s="39"/>
+      <c r="H143" s="40"/>
     </row>
     <row r="144" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
@@ -3151,9 +3161,9 @@
       <c r="C144" s="30"/>
       <c r="D144" s="31"/>
       <c r="E144" s="31"/>
-      <c r="F144" s="35"/>
-      <c r="G144" s="36"/>
-      <c r="H144" s="37"/>
+      <c r="F144" s="38"/>
+      <c r="G144" s="39"/>
+      <c r="H144" s="40"/>
     </row>
     <row r="145" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
@@ -3161,9 +3171,9 @@
       <c r="C145" s="30"/>
       <c r="D145" s="31"/>
       <c r="E145" s="31"/>
-      <c r="F145" s="35"/>
-      <c r="G145" s="36"/>
-      <c r="H145" s="37"/>
+      <c r="F145" s="38"/>
+      <c r="G145" s="39"/>
+      <c r="H145" s="40"/>
     </row>
     <row r="146" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="29"/>
@@ -3171,9 +3181,9 @@
       <c r="C146" s="30"/>
       <c r="D146" s="31"/>
       <c r="E146" s="31"/>
-      <c r="F146" s="35"/>
-      <c r="G146" s="36"/>
-      <c r="H146" s="37"/>
+      <c r="F146" s="38"/>
+      <c r="G146" s="39"/>
+      <c r="H146" s="40"/>
     </row>
     <row r="147" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
@@ -3181,9 +3191,9 @@
       <c r="C147" s="30"/>
       <c r="D147" s="31"/>
       <c r="E147" s="31"/>
-      <c r="F147" s="35"/>
-      <c r="G147" s="36"/>
-      <c r="H147" s="37"/>
+      <c r="F147" s="38"/>
+      <c r="G147" s="39"/>
+      <c r="H147" s="40"/>
     </row>
     <row r="148" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
@@ -3191,9 +3201,9 @@
       <c r="C148" s="30"/>
       <c r="D148" s="31"/>
       <c r="E148" s="31"/>
-      <c r="F148" s="35"/>
-      <c r="G148" s="36"/>
-      <c r="H148" s="37"/>
+      <c r="F148" s="38"/>
+      <c r="G148" s="39"/>
+      <c r="H148" s="40"/>
     </row>
     <row r="149" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
@@ -3201,9 +3211,9 @@
       <c r="C149" s="30"/>
       <c r="D149" s="31"/>
       <c r="E149" s="31"/>
-      <c r="F149" s="35"/>
-      <c r="G149" s="36"/>
-      <c r="H149" s="37"/>
+      <c r="F149" s="38"/>
+      <c r="G149" s="39"/>
+      <c r="H149" s="40"/>
     </row>
     <row r="150" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
@@ -3211,9 +3221,9 @@
       <c r="C150" s="30"/>
       <c r="D150" s="31"/>
       <c r="E150" s="31"/>
-      <c r="F150" s="35"/>
-      <c r="G150" s="36"/>
-      <c r="H150" s="37"/>
+      <c r="F150" s="38"/>
+      <c r="G150" s="39"/>
+      <c r="H150" s="40"/>
     </row>
     <row r="151" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
@@ -3221,9 +3231,9 @@
       <c r="C151" s="30"/>
       <c r="D151" s="31"/>
       <c r="E151" s="31"/>
-      <c r="F151" s="35"/>
-      <c r="G151" s="36"/>
-      <c r="H151" s="37"/>
+      <c r="F151" s="38"/>
+      <c r="G151" s="39"/>
+      <c r="H151" s="40"/>
     </row>
     <row r="152" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="29"/>
@@ -3231,9 +3241,9 @@
       <c r="C152" s="30"/>
       <c r="D152" s="31"/>
       <c r="E152" s="31"/>
-      <c r="F152" s="35"/>
-      <c r="G152" s="36"/>
-      <c r="H152" s="37"/>
+      <c r="F152" s="38"/>
+      <c r="G152" s="39"/>
+      <c r="H152" s="40"/>
     </row>
     <row r="153" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="29"/>
@@ -3241,9 +3251,9 @@
       <c r="C153" s="30"/>
       <c r="D153" s="31"/>
       <c r="E153" s="31"/>
-      <c r="F153" s="35"/>
-      <c r="G153" s="36"/>
-      <c r="H153" s="37"/>
+      <c r="F153" s="38"/>
+      <c r="G153" s="39"/>
+      <c r="H153" s="40"/>
     </row>
     <row r="154" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="29"/>
@@ -3251,9 +3261,9 @@
       <c r="C154" s="30"/>
       <c r="D154" s="31"/>
       <c r="E154" s="31"/>
-      <c r="F154" s="35"/>
-      <c r="G154" s="36"/>
-      <c r="H154" s="37"/>
+      <c r="F154" s="38"/>
+      <c r="G154" s="39"/>
+      <c r="H154" s="40"/>
     </row>
     <row r="155" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="29"/>
@@ -3261,9 +3271,9 @@
       <c r="C155" s="30"/>
       <c r="D155" s="31"/>
       <c r="E155" s="31"/>
-      <c r="F155" s="35"/>
-      <c r="G155" s="36"/>
-      <c r="H155" s="37"/>
+      <c r="F155" s="38"/>
+      <c r="G155" s="39"/>
+      <c r="H155" s="40"/>
     </row>
     <row r="156" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="29"/>
@@ -3271,9 +3281,9 @@
       <c r="C156" s="30"/>
       <c r="D156" s="31"/>
       <c r="E156" s="31"/>
-      <c r="F156" s="35"/>
-      <c r="G156" s="36"/>
-      <c r="H156" s="37"/>
+      <c r="F156" s="38"/>
+      <c r="G156" s="39"/>
+      <c r="H156" s="40"/>
     </row>
     <row r="157" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
@@ -3281,9 +3291,9 @@
       <c r="C157" s="30"/>
       <c r="D157" s="31"/>
       <c r="E157" s="31"/>
-      <c r="F157" s="35"/>
-      <c r="G157" s="36"/>
-      <c r="H157" s="37"/>
+      <c r="F157" s="38"/>
+      <c r="G157" s="39"/>
+      <c r="H157" s="40"/>
     </row>
     <row r="158" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="29"/>
@@ -3291,9 +3301,9 @@
       <c r="C158" s="30"/>
       <c r="D158" s="31"/>
       <c r="E158" s="31"/>
-      <c r="F158" s="35"/>
-      <c r="G158" s="36"/>
-      <c r="H158" s="37"/>
+      <c r="F158" s="38"/>
+      <c r="G158" s="39"/>
+      <c r="H158" s="40"/>
     </row>
     <row r="159" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="29"/>
@@ -3301,9 +3311,9 @@
       <c r="C159" s="30"/>
       <c r="D159" s="31"/>
       <c r="E159" s="31"/>
-      <c r="F159" s="35"/>
-      <c r="G159" s="36"/>
-      <c r="H159" s="37"/>
+      <c r="F159" s="38"/>
+      <c r="G159" s="39"/>
+      <c r="H159" s="40"/>
     </row>
     <row r="160" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="29"/>
@@ -3311,9 +3321,9 @@
       <c r="C160" s="30"/>
       <c r="D160" s="31"/>
       <c r="E160" s="31"/>
-      <c r="F160" s="35"/>
-      <c r="G160" s="36"/>
-      <c r="H160" s="37"/>
+      <c r="F160" s="38"/>
+      <c r="G160" s="39"/>
+      <c r="H160" s="40"/>
     </row>
     <row r="161" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="29"/>
@@ -3321,9 +3331,9 @@
       <c r="C161" s="30"/>
       <c r="D161" s="31"/>
       <c r="E161" s="31"/>
-      <c r="F161" s="35"/>
-      <c r="G161" s="36"/>
-      <c r="H161" s="37"/>
+      <c r="F161" s="38"/>
+      <c r="G161" s="39"/>
+      <c r="H161" s="40"/>
     </row>
     <row r="162" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
@@ -3331,9 +3341,9 @@
       <c r="C162" s="30"/>
       <c r="D162" s="31"/>
       <c r="E162" s="31"/>
-      <c r="F162" s="35"/>
-      <c r="G162" s="36"/>
-      <c r="H162" s="37"/>
+      <c r="F162" s="38"/>
+      <c r="G162" s="39"/>
+      <c r="H162" s="40"/>
     </row>
     <row r="163" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
@@ -3341,9 +3351,9 @@
       <c r="C163" s="30"/>
       <c r="D163" s="31"/>
       <c r="E163" s="31"/>
-      <c r="F163" s="35"/>
-      <c r="G163" s="36"/>
-      <c r="H163" s="37"/>
+      <c r="F163" s="38"/>
+      <c r="G163" s="39"/>
+      <c r="H163" s="40"/>
     </row>
     <row r="164" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
@@ -3351,9 +3361,9 @@
       <c r="C164" s="30"/>
       <c r="D164" s="31"/>
       <c r="E164" s="31"/>
-      <c r="F164" s="35"/>
-      <c r="G164" s="36"/>
-      <c r="H164" s="37"/>
+      <c r="F164" s="38"/>
+      <c r="G164" s="39"/>
+      <c r="H164" s="40"/>
     </row>
     <row r="165" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
@@ -3361,9 +3371,9 @@
       <c r="C165" s="30"/>
       <c r="D165" s="31"/>
       <c r="E165" s="31"/>
-      <c r="F165" s="35"/>
-      <c r="G165" s="36"/>
-      <c r="H165" s="37"/>
+      <c r="F165" s="38"/>
+      <c r="G165" s="39"/>
+      <c r="H165" s="40"/>
     </row>
     <row r="166" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="29"/>
@@ -3371,9 +3381,9 @@
       <c r="C166" s="30"/>
       <c r="D166" s="31"/>
       <c r="E166" s="31"/>
-      <c r="F166" s="35"/>
-      <c r="G166" s="36"/>
-      <c r="H166" s="37"/>
+      <c r="F166" s="38"/>
+      <c r="G166" s="39"/>
+      <c r="H166" s="40"/>
     </row>
     <row r="167" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="29"/>
@@ -3381,9 +3391,9 @@
       <c r="C167" s="30"/>
       <c r="D167" s="31"/>
       <c r="E167" s="31"/>
-      <c r="F167" s="35"/>
-      <c r="G167" s="36"/>
-      <c r="H167" s="37"/>
+      <c r="F167" s="38"/>
+      <c r="G167" s="39"/>
+      <c r="H167" s="40"/>
     </row>
     <row r="168" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="29"/>
@@ -3391,9 +3401,9 @@
       <c r="C168" s="30"/>
       <c r="D168" s="31"/>
       <c r="E168" s="31"/>
-      <c r="F168" s="35"/>
-      <c r="G168" s="36"/>
-      <c r="H168" s="37"/>
+      <c r="F168" s="38"/>
+      <c r="G168" s="39"/>
+      <c r="H168" s="40"/>
     </row>
     <row r="169" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="29"/>
@@ -3401,9 +3411,9 @@
       <c r="C169" s="30"/>
       <c r="D169" s="31"/>
       <c r="E169" s="31"/>
-      <c r="F169" s="35"/>
-      <c r="G169" s="36"/>
-      <c r="H169" s="37"/>
+      <c r="F169" s="38"/>
+      <c r="G169" s="39"/>
+      <c r="H169" s="40"/>
     </row>
     <row r="170" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="29"/>
@@ -3411,9 +3421,9 @@
       <c r="C170" s="30"/>
       <c r="D170" s="31"/>
       <c r="E170" s="31"/>
-      <c r="F170" s="35"/>
-      <c r="G170" s="36"/>
-      <c r="H170" s="37"/>
+      <c r="F170" s="38"/>
+      <c r="G170" s="39"/>
+      <c r="H170" s="40"/>
     </row>
     <row r="171" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="29"/>
@@ -3421,9 +3431,9 @@
       <c r="C171" s="30"/>
       <c r="D171" s="31"/>
       <c r="E171" s="31"/>
-      <c r="F171" s="35"/>
-      <c r="G171" s="36"/>
-      <c r="H171" s="37"/>
+      <c r="F171" s="38"/>
+      <c r="G171" s="39"/>
+      <c r="H171" s="40"/>
     </row>
     <row r="172" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="29"/>
@@ -3431,9 +3441,9 @@
       <c r="C172" s="30"/>
       <c r="D172" s="31"/>
       <c r="E172" s="31"/>
-      <c r="F172" s="35"/>
-      <c r="G172" s="36"/>
-      <c r="H172" s="37"/>
+      <c r="F172" s="38"/>
+      <c r="G172" s="39"/>
+      <c r="H172" s="40"/>
     </row>
     <row r="173" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="29"/>
@@ -3441,9 +3451,9 @@
       <c r="C173" s="30"/>
       <c r="D173" s="31"/>
       <c r="E173" s="31"/>
-      <c r="F173" s="35"/>
-      <c r="G173" s="36"/>
-      <c r="H173" s="37"/>
+      <c r="F173" s="38"/>
+      <c r="G173" s="39"/>
+      <c r="H173" s="40"/>
     </row>
     <row r="174" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="29"/>
@@ -3451,9 +3461,9 @@
       <c r="C174" s="30"/>
       <c r="D174" s="31"/>
       <c r="E174" s="31"/>
-      <c r="F174" s="35"/>
-      <c r="G174" s="36"/>
-      <c r="H174" s="37"/>
+      <c r="F174" s="38"/>
+      <c r="G174" s="39"/>
+      <c r="H174" s="40"/>
     </row>
     <row r="175" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="29"/>
@@ -3461,9 +3471,9 @@
       <c r="C175" s="30"/>
       <c r="D175" s="31"/>
       <c r="E175" s="31"/>
-      <c r="F175" s="35"/>
-      <c r="G175" s="36"/>
-      <c r="H175" s="37"/>
+      <c r="F175" s="38"/>
+      <c r="G175" s="39"/>
+      <c r="H175" s="40"/>
     </row>
     <row r="176" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="29"/>
@@ -3471,9 +3481,9 @@
       <c r="C176" s="30"/>
       <c r="D176" s="31"/>
       <c r="E176" s="31"/>
-      <c r="F176" s="35"/>
-      <c r="G176" s="36"/>
-      <c r="H176" s="37"/>
+      <c r="F176" s="38"/>
+      <c r="G176" s="39"/>
+      <c r="H176" s="40"/>
     </row>
     <row r="177" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
@@ -3481,9 +3491,9 @@
       <c r="C177" s="30"/>
       <c r="D177" s="31"/>
       <c r="E177" s="31"/>
-      <c r="F177" s="35"/>
-      <c r="G177" s="36"/>
-      <c r="H177" s="37"/>
+      <c r="F177" s="38"/>
+      <c r="G177" s="39"/>
+      <c r="H177" s="40"/>
     </row>
     <row r="178" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
@@ -3491,9 +3501,9 @@
       <c r="C178" s="30"/>
       <c r="D178" s="31"/>
       <c r="E178" s="31"/>
-      <c r="F178" s="35"/>
-      <c r="G178" s="36"/>
-      <c r="H178" s="37"/>
+      <c r="F178" s="38"/>
+      <c r="G178" s="39"/>
+      <c r="H178" s="40"/>
     </row>
     <row r="179" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
@@ -3501,9 +3511,9 @@
       <c r="C179" s="30"/>
       <c r="D179" s="31"/>
       <c r="E179" s="31"/>
-      <c r="F179" s="35"/>
-      <c r="G179" s="36"/>
-      <c r="H179" s="37"/>
+      <c r="F179" s="38"/>
+      <c r="G179" s="39"/>
+      <c r="H179" s="40"/>
     </row>
     <row r="180" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="29"/>
@@ -3511,9 +3521,9 @@
       <c r="C180" s="30"/>
       <c r="D180" s="31"/>
       <c r="E180" s="31"/>
-      <c r="F180" s="35"/>
-      <c r="G180" s="36"/>
-      <c r="H180" s="37"/>
+      <c r="F180" s="38"/>
+      <c r="G180" s="39"/>
+      <c r="H180" s="40"/>
     </row>
     <row r="181" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="29"/>
@@ -3521,9 +3531,9 @@
       <c r="C181" s="30"/>
       <c r="D181" s="31"/>
       <c r="E181" s="31"/>
-      <c r="F181" s="35"/>
-      <c r="G181" s="36"/>
-      <c r="H181" s="37"/>
+      <c r="F181" s="38"/>
+      <c r="G181" s="39"/>
+      <c r="H181" s="40"/>
     </row>
     <row r="182" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="29"/>
@@ -3531,9 +3541,9 @@
       <c r="C182" s="30"/>
       <c r="D182" s="31"/>
       <c r="E182" s="31"/>
-      <c r="F182" s="35"/>
-      <c r="G182" s="36"/>
-      <c r="H182" s="37"/>
+      <c r="F182" s="38"/>
+      <c r="G182" s="39"/>
+      <c r="H182" s="40"/>
     </row>
     <row r="183" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
@@ -3541,9 +3551,9 @@
       <c r="C183" s="30"/>
       <c r="D183" s="31"/>
       <c r="E183" s="31"/>
-      <c r="F183" s="35"/>
-      <c r="G183" s="36"/>
-      <c r="H183" s="37"/>
+      <c r="F183" s="38"/>
+      <c r="G183" s="39"/>
+      <c r="H183" s="40"/>
     </row>
     <row r="184" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
@@ -3551,9 +3561,9 @@
       <c r="C184" s="30"/>
       <c r="D184" s="31"/>
       <c r="E184" s="31"/>
-      <c r="F184" s="35"/>
-      <c r="G184" s="36"/>
-      <c r="H184" s="37"/>
+      <c r="F184" s="38"/>
+      <c r="G184" s="39"/>
+      <c r="H184" s="40"/>
     </row>
     <row r="185" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
@@ -3561,9 +3571,9 @@
       <c r="C185" s="30"/>
       <c r="D185" s="31"/>
       <c r="E185" s="31"/>
-      <c r="F185" s="35"/>
-      <c r="G185" s="36"/>
-      <c r="H185" s="37"/>
+      <c r="F185" s="38"/>
+      <c r="G185" s="39"/>
+      <c r="H185" s="40"/>
     </row>
     <row r="186" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="29"/>
@@ -3571,9 +3581,9 @@
       <c r="C186" s="30"/>
       <c r="D186" s="31"/>
       <c r="E186" s="31"/>
-      <c r="F186" s="35"/>
-      <c r="G186" s="36"/>
-      <c r="H186" s="37"/>
+      <c r="F186" s="38"/>
+      <c r="G186" s="39"/>
+      <c r="H186" s="40"/>
     </row>
     <row r="187" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="29"/>
@@ -3581,9 +3591,9 @@
       <c r="C187" s="30"/>
       <c r="D187" s="31"/>
       <c r="E187" s="31"/>
-      <c r="F187" s="35"/>
-      <c r="G187" s="36"/>
-      <c r="H187" s="37"/>
+      <c r="F187" s="38"/>
+      <c r="G187" s="39"/>
+      <c r="H187" s="40"/>
     </row>
     <row r="188" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="29"/>
@@ -3591,9 +3601,9 @@
       <c r="C188" s="30"/>
       <c r="D188" s="31"/>
       <c r="E188" s="31"/>
-      <c r="F188" s="35"/>
-      <c r="G188" s="36"/>
-      <c r="H188" s="37"/>
+      <c r="F188" s="38"/>
+      <c r="G188" s="39"/>
+      <c r="H188" s="40"/>
     </row>
     <row r="189" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="29"/>
@@ -3601,9 +3611,9 @@
       <c r="C189" s="30"/>
       <c r="D189" s="31"/>
       <c r="E189" s="31"/>
-      <c r="F189" s="35"/>
-      <c r="G189" s="36"/>
-      <c r="H189" s="37"/>
+      <c r="F189" s="38"/>
+      <c r="G189" s="39"/>
+      <c r="H189" s="40"/>
     </row>
     <row r="190" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="29"/>
@@ -3611,9 +3621,9 @@
       <c r="C190" s="30"/>
       <c r="D190" s="31"/>
       <c r="E190" s="31"/>
-      <c r="F190" s="35"/>
-      <c r="G190" s="36"/>
-      <c r="H190" s="37"/>
+      <c r="F190" s="38"/>
+      <c r="G190" s="39"/>
+      <c r="H190" s="40"/>
     </row>
     <row r="191" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="29"/>
@@ -3621,9 +3631,9 @@
       <c r="C191" s="30"/>
       <c r="D191" s="31"/>
       <c r="E191" s="31"/>
-      <c r="F191" s="35"/>
-      <c r="G191" s="36"/>
-      <c r="H191" s="37"/>
+      <c r="F191" s="38"/>
+      <c r="G191" s="39"/>
+      <c r="H191" s="40"/>
     </row>
     <row r="192" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="29"/>
@@ -3631,9 +3641,9 @@
       <c r="C192" s="30"/>
       <c r="D192" s="31"/>
       <c r="E192" s="31"/>
-      <c r="F192" s="35"/>
-      <c r="G192" s="36"/>
-      <c r="H192" s="37"/>
+      <c r="F192" s="38"/>
+      <c r="G192" s="39"/>
+      <c r="H192" s="40"/>
     </row>
     <row r="193" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="29"/>
@@ -3641,9 +3651,9 @@
       <c r="C193" s="30"/>
       <c r="D193" s="31"/>
       <c r="E193" s="31"/>
-      <c r="F193" s="35"/>
-      <c r="G193" s="36"/>
-      <c r="H193" s="37"/>
+      <c r="F193" s="38"/>
+      <c r="G193" s="39"/>
+      <c r="H193" s="40"/>
     </row>
     <row r="194" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="29"/>
@@ -3651,9 +3661,9 @@
       <c r="C194" s="30"/>
       <c r="D194" s="31"/>
       <c r="E194" s="31"/>
-      <c r="F194" s="35"/>
-      <c r="G194" s="36"/>
-      <c r="H194" s="37"/>
+      <c r="F194" s="38"/>
+      <c r="G194" s="39"/>
+      <c r="H194" s="40"/>
     </row>
     <row r="195" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="29"/>
@@ -3661,9 +3671,9 @@
       <c r="C195" s="30"/>
       <c r="D195" s="31"/>
       <c r="E195" s="31"/>
-      <c r="F195" s="35"/>
-      <c r="G195" s="36"/>
-      <c r="H195" s="37"/>
+      <c r="F195" s="38"/>
+      <c r="G195" s="39"/>
+      <c r="H195" s="40"/>
     </row>
     <row r="196" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="29"/>
@@ -3671,9 +3681,9 @@
       <c r="C196" s="30"/>
       <c r="D196" s="31"/>
       <c r="E196" s="31"/>
-      <c r="F196" s="35"/>
-      <c r="G196" s="36"/>
-      <c r="H196" s="37"/>
+      <c r="F196" s="38"/>
+      <c r="G196" s="39"/>
+      <c r="H196" s="40"/>
     </row>
     <row r="197" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="29"/>
@@ -3681,9 +3691,9 @@
       <c r="C197" s="30"/>
       <c r="D197" s="31"/>
       <c r="E197" s="31"/>
-      <c r="F197" s="35"/>
-      <c r="G197" s="36"/>
-      <c r="H197" s="37"/>
+      <c r="F197" s="38"/>
+      <c r="G197" s="39"/>
+      <c r="H197" s="40"/>
     </row>
     <row r="198" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="29"/>
@@ -3691,9 +3701,9 @@
       <c r="C198" s="30"/>
       <c r="D198" s="31"/>
       <c r="E198" s="31"/>
-      <c r="F198" s="35"/>
-      <c r="G198" s="36"/>
-      <c r="H198" s="37"/>
+      <c r="F198" s="38"/>
+      <c r="G198" s="39"/>
+      <c r="H198" s="40"/>
     </row>
     <row r="199" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="29"/>
@@ -3701,9 +3711,9 @@
       <c r="C199" s="30"/>
       <c r="D199" s="31"/>
       <c r="E199" s="31"/>
-      <c r="F199" s="35"/>
-      <c r="G199" s="36"/>
-      <c r="H199" s="37"/>
+      <c r="F199" s="38"/>
+      <c r="G199" s="39"/>
+      <c r="H199" s="40"/>
     </row>
     <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="32"/>
@@ -3711,13 +3721,203 @@
       <c r="C200" s="33"/>
       <c r="D200" s="34"/>
       <c r="E200" s="34"/>
-      <c r="F200" s="38"/>
-      <c r="G200" s="39"/>
-      <c r="H200" s="40"/>
+      <c r="F200" s="59"/>
+      <c r="G200" s="60"/>
+      <c r="H200" s="61"/>
     </row>
     <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="204">
+    <mergeCell ref="F196:H196"/>
+    <mergeCell ref="F197:H197"/>
+    <mergeCell ref="F198:H198"/>
+    <mergeCell ref="F199:H199"/>
+    <mergeCell ref="F200:H200"/>
+    <mergeCell ref="F191:H191"/>
+    <mergeCell ref="F192:H192"/>
+    <mergeCell ref="F193:H193"/>
+    <mergeCell ref="F194:H194"/>
+    <mergeCell ref="F195:H195"/>
+    <mergeCell ref="F186:H186"/>
+    <mergeCell ref="F187:H187"/>
+    <mergeCell ref="F188:H188"/>
+    <mergeCell ref="F189:H189"/>
+    <mergeCell ref="F190:H190"/>
+    <mergeCell ref="F181:H181"/>
+    <mergeCell ref="F182:H182"/>
+    <mergeCell ref="F183:H183"/>
+    <mergeCell ref="F184:H184"/>
+    <mergeCell ref="F185:H185"/>
+    <mergeCell ref="F176:H176"/>
+    <mergeCell ref="F177:H177"/>
+    <mergeCell ref="F178:H178"/>
+    <mergeCell ref="F179:H179"/>
+    <mergeCell ref="F180:H180"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="F172:H172"/>
+    <mergeCell ref="F173:H173"/>
+    <mergeCell ref="F174:H174"/>
+    <mergeCell ref="F175:H175"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="F167:H167"/>
+    <mergeCell ref="F168:H168"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="F170:H170"/>
+    <mergeCell ref="F161:H161"/>
+    <mergeCell ref="F162:H162"/>
+    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="F164:H164"/>
+    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="F156:H156"/>
+    <mergeCell ref="F157:H157"/>
+    <mergeCell ref="F158:H158"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="F152:H152"/>
+    <mergeCell ref="F153:H153"/>
+    <mergeCell ref="F154:H154"/>
+    <mergeCell ref="F155:H155"/>
+    <mergeCell ref="F146:H146"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F148:H148"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="F150:H150"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="F144:H144"/>
+    <mergeCell ref="F145:H145"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -3732,196 +3932,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F146:H146"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F148:H148"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="F150:H150"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="F143:H143"/>
-    <mergeCell ref="F144:H144"/>
-    <mergeCell ref="F145:H145"/>
-    <mergeCell ref="F156:H156"/>
-    <mergeCell ref="F157:H157"/>
-    <mergeCell ref="F158:H158"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="F151:H151"/>
-    <mergeCell ref="F152:H152"/>
-    <mergeCell ref="F153:H153"/>
-    <mergeCell ref="F154:H154"/>
-    <mergeCell ref="F155:H155"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="F167:H167"/>
-    <mergeCell ref="F168:H168"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="F170:H170"/>
-    <mergeCell ref="F161:H161"/>
-    <mergeCell ref="F162:H162"/>
-    <mergeCell ref="F163:H163"/>
-    <mergeCell ref="F164:H164"/>
-    <mergeCell ref="F165:H165"/>
-    <mergeCell ref="F176:H176"/>
-    <mergeCell ref="F177:H177"/>
-    <mergeCell ref="F178:H178"/>
-    <mergeCell ref="F179:H179"/>
-    <mergeCell ref="F180:H180"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="F172:H172"/>
-    <mergeCell ref="F173:H173"/>
-    <mergeCell ref="F174:H174"/>
-    <mergeCell ref="F175:H175"/>
-    <mergeCell ref="F186:H186"/>
-    <mergeCell ref="F187:H187"/>
-    <mergeCell ref="F188:H188"/>
-    <mergeCell ref="F189:H189"/>
-    <mergeCell ref="F190:H190"/>
-    <mergeCell ref="F181:H181"/>
-    <mergeCell ref="F182:H182"/>
-    <mergeCell ref="F183:H183"/>
-    <mergeCell ref="F184:H184"/>
-    <mergeCell ref="F185:H185"/>
-    <mergeCell ref="F196:H196"/>
-    <mergeCell ref="F197:H197"/>
-    <mergeCell ref="F198:H198"/>
-    <mergeCell ref="F199:H199"/>
-    <mergeCell ref="F200:H200"/>
-    <mergeCell ref="F191:H191"/>
-    <mergeCell ref="F192:H192"/>
-    <mergeCell ref="F193:H193"/>
-    <mergeCell ref="F194:H194"/>
-    <mergeCell ref="F195:H195"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3935,6 +3945,91 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>470</v>
+      </c>
+      <c r="B2">
+        <v>1.577762987E-6</v>
+      </c>
+      <c r="C2">
+        <v>-1.2518171072006199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>470</v>
+      </c>
+      <c r="B3">
+        <v>1.9652070477605001E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.42159372568130499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>470</v>
+      </c>
+      <c r="B4">
+        <v>3.9930999279022002E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.3459901809692298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>470</v>
+      </c>
+      <c r="B5">
+        <v>6.0378383845090998E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.8428088426589899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>470</v>
+      </c>
+      <c r="B6">
+        <v>8.0073416233062994E-2</v>
+      </c>
+      <c r="C6">
+        <v>-345.81799316406199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -4048,7 +4143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
@@ -4238,21 +4333,21 @@
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Small changes from the MBpro
</commit_message>
<xml_diff>
--- a/EMX_3.xlsx
+++ b/EMX_3.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\GitHub\docubase\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="135" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1180" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -964,6 +959,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -973,15 +986,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1035,15 +1039,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1436,18 +1431,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="62.375" style="28" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" style="28" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="6" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +1450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="38" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
@@ -1463,13 +1458,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="38" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="38" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1477,7 +1472,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="38" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1485,7 +1480,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
       <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
@@ -1493,19 +1488,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="38.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:2" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="38" customHeight="1" thickTop="1"/>
+    <row r="8" spans="1:2" ht="38" customHeight="1"/>
+    <row r="9" spans="1:2" ht="38" customHeight="1"/>
+    <row r="10" spans="1:2" ht="38" customHeight="1"/>
+    <row r="11" spans="1:2" ht="38" customHeight="1"/>
+    <row r="12" spans="1:2" ht="38" customHeight="1"/>
+    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1">
       <c r="A13" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1518,34 +1513,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31:H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" style="18" customWidth="1"/>
     <col min="6" max="6" width="34.5" style="18" customWidth="1"/>
-    <col min="7" max="7" width="8.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1">
+      <c r="A1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
       <c r="G1" s="21" t="s">
         <v>31</v>
       </c>
@@ -1553,17 +1548,17 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:8" ht="39" customHeight="1">
+      <c r="A2" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
       <c r="G2" s="22" t="s">
         <v>31</v>
       </c>
@@ -1571,45 +1566,45 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:8" ht="39" customHeight="1">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="45"/>
-    </row>
-    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
+    </row>
+    <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1">
+      <c r="A4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-    </row>
-    <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-    </row>
-    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+    </row>
+    <row r="5" spans="1:8" ht="26" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+    </row>
+    <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1625,13 +1620,13 @@
       <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-    </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
+    </row>
+    <row r="7" spans="1:8" ht="39" customHeight="1">
       <c r="A7" s="29">
         <v>1</v>
       </c>
@@ -1641,13 +1636,13 @@
       <c r="C7" s="30"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
-    </row>
-    <row r="8" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" ht="39" customHeight="1">
       <c r="A8" s="29">
         <v>1</v>
       </c>
@@ -1659,13 +1654,13 @@
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
-    </row>
-    <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:8" ht="39" customHeight="1">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1677,13 +1672,13 @@
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="36"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="10" spans="1:8" ht="39" customHeight="1">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -1695,13 +1690,13 @@
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="36"/>
+      <c r="H10" s="37"/>
+    </row>
+    <row r="11" spans="1:8" ht="39" customHeight="1">
       <c r="A11" s="29">
         <v>1</v>
       </c>
@@ -1713,13 +1708,13 @@
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="38" t="s">
+      <c r="F11" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="40"/>
-    </row>
-    <row r="12" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
+    </row>
+    <row r="12" spans="1:8" ht="39" customHeight="1">
       <c r="A12" s="29">
         <v>1</v>
       </c>
@@ -1731,13 +1726,13 @@
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
-    </row>
-    <row r="13" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:8" ht="39" customHeight="1">
       <c r="A13" s="29">
         <v>1</v>
       </c>
@@ -1747,13 +1742,13 @@
       <c r="C13" s="30"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40"/>
-    </row>
-    <row r="14" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:8" ht="39" customHeight="1">
       <c r="A14" s="29">
         <v>1</v>
       </c>
@@ -1763,11 +1758,11 @@
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
-    </row>
-    <row r="15" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:8" ht="39" customHeight="1">
       <c r="A15" s="29">
         <v>1</v>
       </c>
@@ -1777,11 +1772,11 @@
       <c r="C15" s="30"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
-    </row>
-    <row r="16" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" ht="39" customHeight="1">
       <c r="A16" s="29">
         <v>1</v>
       </c>
@@ -1791,11 +1786,11 @@
       <c r="C16" s="30"/>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-    </row>
-    <row r="17" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+    </row>
+    <row r="17" spans="1:8" ht="39" customHeight="1">
       <c r="A17" s="29">
         <v>1</v>
       </c>
@@ -1805,11 +1800,11 @@
       <c r="C17" s="30"/>
       <c r="D17" s="31"/>
       <c r="E17" s="31"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
-    </row>
-    <row r="18" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="35"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+    </row>
+    <row r="18" spans="1:8" ht="39" customHeight="1">
       <c r="A18" s="29">
         <v>1</v>
       </c>
@@ -1819,11 +1814,11 @@
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40"/>
-    </row>
-    <row r="19" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="35"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+    </row>
+    <row r="19" spans="1:8" ht="39" customHeight="1">
       <c r="A19" s="29">
         <v>1</v>
       </c>
@@ -1835,13 +1830,13 @@
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
-      <c r="F19" s="38" t="s">
+      <c r="F19" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
-    </row>
-    <row r="20" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+    </row>
+    <row r="20" spans="1:8" ht="56.25" customHeight="1">
       <c r="A20" s="29">
         <v>1</v>
       </c>
@@ -1851,13 +1846,13 @@
       <c r="C20" s="30"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="40"/>
-    </row>
-    <row r="21" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
+    </row>
+    <row r="21" spans="1:8" ht="39" customHeight="1">
       <c r="A21" s="29">
         <v>1</v>
       </c>
@@ -1867,13 +1862,13 @@
       <c r="C21" s="30"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="40"/>
-    </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" ht="39" customHeight="1">
       <c r="A22" s="29">
         <v>1</v>
       </c>
@@ -1883,11 +1878,11 @@
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" ht="39" customHeight="1">
       <c r="A23" s="29">
         <v>1</v>
       </c>
@@ -1897,11 +1892,11 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
-    </row>
-    <row r="24" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" ht="39" customHeight="1">
       <c r="A24" s="29">
         <v>1</v>
       </c>
@@ -1911,11 +1906,11 @@
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
-    </row>
-    <row r="25" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
+    </row>
+    <row r="25" spans="1:8" ht="39" customHeight="1">
       <c r="A25" s="29">
         <v>1</v>
       </c>
@@ -1925,11 +1920,11 @@
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-    </row>
-    <row r="26" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
+    </row>
+    <row r="26" spans="1:8" ht="39" customHeight="1">
       <c r="A26" s="29">
         <v>1</v>
       </c>
@@ -1939,13 +1934,13 @@
       <c r="C26" s="30"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
-      <c r="F26" s="38" t="s">
+      <c r="F26" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-    </row>
-    <row r="27" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" ht="39" customHeight="1">
       <c r="A27" s="29">
         <v>1</v>
       </c>
@@ -1955,11 +1950,11 @@
       <c r="C27" s="30"/>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
-    </row>
-    <row r="28" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" ht="39" customHeight="1">
       <c r="A28" s="29">
         <v>1</v>
       </c>
@@ -1969,11 +1964,11 @@
       <c r="C28" s="30"/>
       <c r="D28" s="31"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" ht="39" customHeight="1">
       <c r="A29" s="29">
         <v>1</v>
       </c>
@@ -1983,13 +1978,13 @@
       <c r="C29" s="30"/>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
-      <c r="F29" s="38" t="s">
+      <c r="F29" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="39"/>
-      <c r="H29" s="40"/>
-    </row>
-    <row r="30" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" ht="39" customHeight="1">
       <c r="A30" s="29">
         <v>1</v>
       </c>
@@ -2001,13 +1996,13 @@
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
-      <c r="F30" s="38" t="s">
+      <c r="F30" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
-    </row>
-    <row r="31" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" ht="39" customHeight="1">
       <c r="A31" s="29">
         <v>1</v>
       </c>
@@ -2017,11 +2012,11 @@
       <c r="C31" s="30"/>
       <c r="D31" s="31"/>
       <c r="E31" s="31"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="40"/>
-    </row>
-    <row r="32" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
+    </row>
+    <row r="32" spans="1:8" ht="39" customHeight="1">
       <c r="A32" s="29">
         <v>1</v>
       </c>
@@ -2031,11 +2026,11 @@
       <c r="C32" s="30"/>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
-    </row>
-    <row r="33" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="35"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="33" spans="1:8" ht="39" customHeight="1">
       <c r="A33" s="29">
         <v>1</v>
       </c>
@@ -2045,11 +2040,11 @@
       <c r="C33" s="30"/>
       <c r="D33" s="31"/>
       <c r="E33" s="31"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="40"/>
-    </row>
-    <row r="34" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="35"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" ht="39" customHeight="1">
       <c r="A34" s="29">
         <v>1</v>
       </c>
@@ -2059,1865 +2054,1675 @@
       <c r="C34" s="30"/>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="38" t="s">
+      <c r="F34" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
-    </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" ht="39" customHeight="1">
       <c r="A35" s="29"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
-    </row>
-    <row r="36" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
+    </row>
+    <row r="36" spans="1:8" ht="39" customHeight="1">
       <c r="A36" s="29"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="40"/>
-    </row>
-    <row r="37" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
+    </row>
+    <row r="37" spans="1:8" ht="39" customHeight="1">
       <c r="A37" s="29"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
       <c r="D37" s="31"/>
       <c r="E37" s="31"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="35"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
+    </row>
+    <row r="38" spans="1:8" ht="39" customHeight="1">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
-    </row>
-    <row r="39" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="37"/>
+    </row>
+    <row r="39" spans="1:8" ht="39" customHeight="1">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
       <c r="D39" s="31"/>
       <c r="E39" s="31"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
-    </row>
-    <row r="40" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
+    </row>
+    <row r="40" spans="1:8" ht="39" customHeight="1">
       <c r="A40" s="29"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
       <c r="D40" s="31"/>
       <c r="E40" s="31"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
-    </row>
-    <row r="41" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="37"/>
+    </row>
+    <row r="41" spans="1:8" ht="39" customHeight="1">
       <c r="A41" s="29"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
       <c r="D41" s="31"/>
       <c r="E41" s="31"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="40"/>
-    </row>
-    <row r="42" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
+    </row>
+    <row r="42" spans="1:8" ht="39" customHeight="1">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
       <c r="D42" s="31"/>
       <c r="E42" s="31"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
-    </row>
-    <row r="43" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="35"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
+    </row>
+    <row r="43" spans="1:8" ht="39" customHeight="1">
       <c r="A43" s="29"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="40"/>
-    </row>
-    <row r="44" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
+    </row>
+    <row r="44" spans="1:8" ht="39" customHeight="1">
       <c r="A44" s="29"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
       <c r="D44" s="31"/>
       <c r="E44" s="31"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
-    </row>
-    <row r="45" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="35"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
+    </row>
+    <row r="45" spans="1:8" ht="39" customHeight="1">
       <c r="A45" s="29"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
       <c r="D45" s="31"/>
       <c r="E45" s="31"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="40"/>
-    </row>
-    <row r="46" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="35"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
+    </row>
+    <row r="46" spans="1:8" ht="39" customHeight="1">
       <c r="A46" s="29"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
       <c r="D46" s="31"/>
       <c r="E46" s="31"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="40"/>
-    </row>
-    <row r="47" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="35"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
+    </row>
+    <row r="47" spans="1:8" ht="39" customHeight="1">
       <c r="A47" s="29"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
       <c r="D47" s="31"/>
       <c r="E47" s="31"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40"/>
-    </row>
-    <row r="48" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="35"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
+    </row>
+    <row r="48" spans="1:8" ht="39" customHeight="1">
       <c r="A48" s="29"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
-    </row>
-    <row r="49" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="35"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
+    </row>
+    <row r="49" spans="1:8" ht="39" customHeight="1">
       <c r="A49" s="29"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
       <c r="D49" s="31"/>
       <c r="E49" s="31"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="40"/>
-    </row>
-    <row r="50" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
+    </row>
+    <row r="50" spans="1:8" ht="39" customHeight="1">
       <c r="A50" s="29"/>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
       <c r="D50" s="31"/>
       <c r="E50" s="31"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="40"/>
-    </row>
-    <row r="51" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F50" s="35"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="37"/>
+    </row>
+    <row r="51" spans="1:8" ht="39" customHeight="1">
       <c r="A51" s="29"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
       <c r="D51" s="31"/>
       <c r="E51" s="31"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
-    </row>
-    <row r="52" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F51" s="35"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="37"/>
+    </row>
+    <row r="52" spans="1:8" ht="39" customHeight="1">
       <c r="A52" s="29"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
       <c r="D52" s="31"/>
       <c r="E52" s="31"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="40"/>
-    </row>
-    <row r="53" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="37"/>
+    </row>
+    <row r="53" spans="1:8" ht="39" customHeight="1">
       <c r="A53" s="29"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
       <c r="D53" s="31"/>
       <c r="E53" s="31"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
-    </row>
-    <row r="54" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="35"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
+    </row>
+    <row r="54" spans="1:8" ht="39" customHeight="1">
       <c r="A54" s="29"/>
       <c r="B54" s="30"/>
       <c r="C54" s="30"/>
       <c r="D54" s="31"/>
       <c r="E54" s="31"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
-    </row>
-    <row r="55" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F54" s="35"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
+    </row>
+    <row r="55" spans="1:8" ht="39" customHeight="1">
       <c r="A55" s="29"/>
       <c r="B55" s="30"/>
       <c r="C55" s="30"/>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
-    </row>
-    <row r="56" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="35"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
+    </row>
+    <row r="56" spans="1:8" ht="39" customHeight="1">
       <c r="A56" s="29"/>
       <c r="B56" s="30"/>
       <c r="C56" s="30"/>
       <c r="D56" s="31"/>
       <c r="E56" s="31"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="40"/>
-    </row>
-    <row r="57" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="35"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
+    </row>
+    <row r="57" spans="1:8" ht="39" customHeight="1">
       <c r="A57" s="29"/>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="40"/>
-    </row>
-    <row r="58" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="35"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
+    </row>
+    <row r="58" spans="1:8" ht="39" customHeight="1">
       <c r="A58" s="29"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
       <c r="D58" s="31"/>
       <c r="E58" s="31"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="40"/>
-    </row>
-    <row r="59" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="37"/>
+    </row>
+    <row r="59" spans="1:8" ht="39" customHeight="1">
       <c r="A59" s="29"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="40"/>
-    </row>
-    <row r="60" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="35"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
+    </row>
+    <row r="60" spans="1:8" ht="39" customHeight="1">
       <c r="A60" s="29"/>
       <c r="B60" s="30"/>
       <c r="C60" s="30"/>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="40"/>
-    </row>
-    <row r="61" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="35"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="37"/>
+    </row>
+    <row r="61" spans="1:8" ht="39" customHeight="1">
       <c r="A61" s="29"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30"/>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
-    </row>
-    <row r="62" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="35"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="37"/>
+    </row>
+    <row r="62" spans="1:8" ht="39" customHeight="1">
       <c r="A62" s="29"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30"/>
       <c r="D62" s="31"/>
       <c r="E62" s="31"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
-    </row>
-    <row r="63" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="35"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="37"/>
+    </row>
+    <row r="63" spans="1:8" ht="39" customHeight="1">
       <c r="A63" s="29"/>
       <c r="B63" s="30"/>
       <c r="C63" s="30"/>
       <c r="D63" s="31"/>
       <c r="E63" s="31"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
-    </row>
-    <row r="64" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="35"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
+    </row>
+    <row r="64" spans="1:8" ht="39" customHeight="1">
       <c r="A64" s="29"/>
       <c r="B64" s="30"/>
       <c r="C64" s="30"/>
       <c r="D64" s="31"/>
       <c r="E64" s="31"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40"/>
-    </row>
-    <row r="65" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="35"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="37"/>
+    </row>
+    <row r="65" spans="1:8" ht="39" customHeight="1">
       <c r="A65" s="29"/>
       <c r="B65" s="30"/>
       <c r="C65" s="30"/>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
-    </row>
-    <row r="66" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F65" s="35"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="37"/>
+    </row>
+    <row r="66" spans="1:8" ht="39" customHeight="1">
       <c r="A66" s="29"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
       <c r="D66" s="31"/>
       <c r="E66" s="31"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
-    </row>
-    <row r="67" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F66" s="35"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
+    </row>
+    <row r="67" spans="1:8" ht="39" customHeight="1">
       <c r="A67" s="29"/>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="40"/>
-    </row>
-    <row r="68" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="35"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
+    </row>
+    <row r="68" spans="1:8" ht="39" customHeight="1">
       <c r="A68" s="29"/>
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
       <c r="D68" s="31"/>
       <c r="E68" s="31"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="40"/>
-    </row>
-    <row r="69" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="35"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
+    </row>
+    <row r="69" spans="1:8" ht="39" customHeight="1">
       <c r="A69" s="29"/>
       <c r="B69" s="30"/>
       <c r="C69" s="30"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="40"/>
-    </row>
-    <row r="70" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
+    </row>
+    <row r="70" spans="1:8" ht="39" customHeight="1">
       <c r="A70" s="29"/>
       <c r="B70" s="30"/>
       <c r="C70" s="30"/>
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="40"/>
-    </row>
-    <row r="71" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
+    </row>
+    <row r="71" spans="1:8" ht="39" customHeight="1">
       <c r="A71" s="29"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="40"/>
-    </row>
-    <row r="72" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
+    </row>
+    <row r="72" spans="1:8" ht="39" customHeight="1">
       <c r="A72" s="29"/>
       <c r="B72" s="30"/>
       <c r="C72" s="30"/>
       <c r="D72" s="31"/>
       <c r="E72" s="31"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="40"/>
-    </row>
-    <row r="73" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
+    </row>
+    <row r="73" spans="1:8" ht="39" customHeight="1">
       <c r="A73" s="29"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
-      <c r="F73" s="38"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="40"/>
-    </row>
-    <row r="74" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F73" s="35"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
+    </row>
+    <row r="74" spans="1:8" ht="39" customHeight="1">
       <c r="A74" s="29"/>
       <c r="B74" s="30"/>
       <c r="C74" s="30"/>
       <c r="D74" s="31"/>
       <c r="E74" s="31"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="40"/>
-    </row>
-    <row r="75" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F74" s="35"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
+    </row>
+    <row r="75" spans="1:8" ht="39" customHeight="1">
       <c r="A75" s="29"/>
       <c r="B75" s="30"/>
       <c r="C75" s="30"/>
       <c r="D75" s="31"/>
       <c r="E75" s="31"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="40"/>
-    </row>
-    <row r="76" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F75" s="35"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
+    </row>
+    <row r="76" spans="1:8" ht="39" customHeight="1">
       <c r="A76" s="29"/>
       <c r="B76" s="30"/>
       <c r="C76" s="30"/>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
-      <c r="F76" s="38"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="40"/>
-    </row>
-    <row r="77" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F76" s="35"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
+    </row>
+    <row r="77" spans="1:8" ht="39" customHeight="1">
       <c r="A77" s="29"/>
       <c r="B77" s="30"/>
       <c r="C77" s="30"/>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
-      <c r="F77" s="38"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="40"/>
-    </row>
-    <row r="78" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F77" s="35"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
+    </row>
+    <row r="78" spans="1:8" ht="39" customHeight="1">
       <c r="A78" s="29"/>
       <c r="B78" s="30"/>
       <c r="C78" s="30"/>
       <c r="D78" s="31"/>
       <c r="E78" s="31"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="40"/>
-    </row>
-    <row r="79" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F78" s="35"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
+    </row>
+    <row r="79" spans="1:8" ht="39" customHeight="1">
       <c r="A79" s="29"/>
       <c r="B79" s="30"/>
       <c r="C79" s="30"/>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
-      <c r="F79" s="38"/>
-      <c r="G79" s="39"/>
-      <c r="H79" s="40"/>
-    </row>
-    <row r="80" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="35"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
+    </row>
+    <row r="80" spans="1:8" ht="39" customHeight="1">
       <c r="A80" s="29"/>
       <c r="B80" s="30"/>
       <c r="C80" s="30"/>
       <c r="D80" s="31"/>
       <c r="E80" s="31"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="40"/>
-    </row>
-    <row r="81" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F80" s="35"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="37"/>
+    </row>
+    <row r="81" spans="1:8" ht="39" customHeight="1">
       <c r="A81" s="29"/>
       <c r="B81" s="30"/>
       <c r="C81" s="30"/>
       <c r="D81" s="31"/>
       <c r="E81" s="31"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="40"/>
-    </row>
-    <row r="82" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F81" s="35"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="37"/>
+    </row>
+    <row r="82" spans="1:8" ht="39" customHeight="1">
       <c r="A82" s="29"/>
       <c r="B82" s="30"/>
       <c r="C82" s="30"/>
       <c r="D82" s="31"/>
       <c r="E82" s="31"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="39"/>
-      <c r="H82" s="40"/>
-    </row>
-    <row r="83" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F82" s="35"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
+    </row>
+    <row r="83" spans="1:8" ht="39" customHeight="1">
       <c r="A83" s="29"/>
       <c r="B83" s="30"/>
       <c r="C83" s="30"/>
       <c r="D83" s="31"/>
       <c r="E83" s="31"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
-    </row>
-    <row r="84" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
+    </row>
+    <row r="84" spans="1:8" ht="39" customHeight="1">
       <c r="A84" s="29"/>
       <c r="B84" s="30"/>
       <c r="C84" s="30"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
-      <c r="F84" s="38"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="40"/>
-    </row>
-    <row r="85" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F84" s="35"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
+    </row>
+    <row r="85" spans="1:8" ht="39" customHeight="1">
       <c r="A85" s="29"/>
       <c r="B85" s="30"/>
       <c r="C85" s="30"/>
       <c r="D85" s="31"/>
       <c r="E85" s="31"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="40"/>
-    </row>
-    <row r="86" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F85" s="35"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
+    </row>
+    <row r="86" spans="1:8" ht="39" customHeight="1">
       <c r="A86" s="29"/>
       <c r="B86" s="30"/>
       <c r="C86" s="30"/>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="40"/>
-    </row>
-    <row r="87" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F86" s="35"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
+    </row>
+    <row r="87" spans="1:8" ht="39" customHeight="1">
       <c r="A87" s="29"/>
       <c r="B87" s="30"/>
       <c r="C87" s="30"/>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="40"/>
-    </row>
-    <row r="88" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
+    </row>
+    <row r="88" spans="1:8" ht="39" customHeight="1">
       <c r="A88" s="29"/>
       <c r="B88" s="30"/>
       <c r="C88" s="30"/>
       <c r="D88" s="31"/>
       <c r="E88" s="31"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="40"/>
-    </row>
-    <row r="89" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F88" s="35"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
+    </row>
+    <row r="89" spans="1:8" ht="39" customHeight="1">
       <c r="A89" s="29"/>
       <c r="B89" s="30"/>
       <c r="C89" s="30"/>
       <c r="D89" s="31"/>
       <c r="E89" s="31"/>
-      <c r="F89" s="38"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="40"/>
-    </row>
-    <row r="90" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F89" s="35"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
+    </row>
+    <row r="90" spans="1:8" ht="39" customHeight="1">
       <c r="A90" s="29"/>
       <c r="B90" s="30"/>
       <c r="C90" s="30"/>
       <c r="D90" s="31"/>
       <c r="E90" s="31"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="40"/>
-    </row>
-    <row r="91" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F90" s="35"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
+    </row>
+    <row r="91" spans="1:8" ht="39" customHeight="1">
       <c r="A91" s="29"/>
       <c r="B91" s="30"/>
       <c r="C91" s="30"/>
       <c r="D91" s="31"/>
       <c r="E91" s="31"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="40"/>
-    </row>
-    <row r="92" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F91" s="35"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
+    </row>
+    <row r="92" spans="1:8" ht="39" customHeight="1">
       <c r="A92" s="29"/>
       <c r="B92" s="30"/>
       <c r="C92" s="30"/>
       <c r="D92" s="31"/>
       <c r="E92" s="31"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="40"/>
-    </row>
-    <row r="93" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F92" s="35"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
+    </row>
+    <row r="93" spans="1:8" ht="39" customHeight="1">
       <c r="A93" s="29"/>
       <c r="B93" s="30"/>
       <c r="C93" s="30"/>
       <c r="D93" s="31"/>
       <c r="E93" s="31"/>
-      <c r="F93" s="38"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="40"/>
-    </row>
-    <row r="94" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F93" s="35"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
+    </row>
+    <row r="94" spans="1:8" ht="39" customHeight="1">
       <c r="A94" s="29"/>
       <c r="B94" s="30"/>
       <c r="C94" s="30"/>
       <c r="D94" s="31"/>
       <c r="E94" s="31"/>
-      <c r="F94" s="38"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="40"/>
-    </row>
-    <row r="95" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F94" s="35"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
+    </row>
+    <row r="95" spans="1:8" ht="39" customHeight="1">
       <c r="A95" s="29"/>
       <c r="B95" s="30"/>
       <c r="C95" s="30"/>
       <c r="D95" s="31"/>
       <c r="E95" s="31"/>
-      <c r="F95" s="38"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="40"/>
-    </row>
-    <row r="96" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
+    </row>
+    <row r="96" spans="1:8" ht="39" customHeight="1">
       <c r="A96" s="29"/>
       <c r="B96" s="30"/>
       <c r="C96" s="30"/>
       <c r="D96" s="31"/>
       <c r="E96" s="31"/>
-      <c r="F96" s="38"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="40"/>
-    </row>
-    <row r="97" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
+    </row>
+    <row r="97" spans="1:8" ht="39" customHeight="1">
       <c r="A97" s="29"/>
       <c r="B97" s="30"/>
       <c r="C97" s="30"/>
       <c r="D97" s="31"/>
       <c r="E97" s="31"/>
-      <c r="F97" s="38"/>
-      <c r="G97" s="39"/>
-      <c r="H97" s="40"/>
-    </row>
-    <row r="98" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
+    </row>
+    <row r="98" spans="1:8" ht="39" customHeight="1">
       <c r="A98" s="29"/>
       <c r="B98" s="30"/>
       <c r="C98" s="30"/>
       <c r="D98" s="31"/>
       <c r="E98" s="31"/>
-      <c r="F98" s="38"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="40"/>
-    </row>
-    <row r="99" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F98" s="35"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
+    </row>
+    <row r="99" spans="1:8" ht="39" customHeight="1">
       <c r="A99" s="29"/>
       <c r="B99" s="30"/>
       <c r="C99" s="30"/>
       <c r="D99" s="31"/>
       <c r="E99" s="31"/>
-      <c r="F99" s="38"/>
-      <c r="G99" s="39"/>
-      <c r="H99" s="40"/>
-    </row>
-    <row r="100" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F99" s="35"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
+    </row>
+    <row r="100" spans="1:8" ht="39" customHeight="1">
       <c r="A100" s="29"/>
       <c r="B100" s="30"/>
       <c r="C100" s="30"/>
       <c r="D100" s="31"/>
       <c r="E100" s="31"/>
-      <c r="F100" s="38"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="40"/>
-    </row>
-    <row r="101" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F100" s="35"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
+    </row>
+    <row r="101" spans="1:8" ht="39" customHeight="1">
       <c r="A101" s="29"/>
       <c r="B101" s="30"/>
       <c r="C101" s="30"/>
       <c r="D101" s="31"/>
       <c r="E101" s="31"/>
-      <c r="F101" s="38"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="40"/>
-    </row>
-    <row r="102" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F101" s="35"/>
+      <c r="G101" s="36"/>
+      <c r="H101" s="37"/>
+    </row>
+    <row r="102" spans="1:8" ht="39" customHeight="1">
       <c r="A102" s="29"/>
       <c r="B102" s="30"/>
       <c r="C102" s="30"/>
       <c r="D102" s="31"/>
       <c r="E102" s="31"/>
-      <c r="F102" s="38"/>
-      <c r="G102" s="39"/>
-      <c r="H102" s="40"/>
-    </row>
-    <row r="103" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F102" s="35"/>
+      <c r="G102" s="36"/>
+      <c r="H102" s="37"/>
+    </row>
+    <row r="103" spans="1:8" ht="39" customHeight="1">
       <c r="A103" s="29"/>
       <c r="B103" s="30"/>
       <c r="C103" s="30"/>
       <c r="D103" s="31"/>
       <c r="E103" s="31"/>
-      <c r="F103" s="38"/>
-      <c r="G103" s="39"/>
-      <c r="H103" s="40"/>
-    </row>
-    <row r="104" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F103" s="35"/>
+      <c r="G103" s="36"/>
+      <c r="H103" s="37"/>
+    </row>
+    <row r="104" spans="1:8" ht="39" customHeight="1">
       <c r="A104" s="29"/>
       <c r="B104" s="30"/>
       <c r="C104" s="30"/>
       <c r="D104" s="31"/>
       <c r="E104" s="31"/>
-      <c r="F104" s="38"/>
-      <c r="G104" s="39"/>
-      <c r="H104" s="40"/>
-    </row>
-    <row r="105" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F104" s="35"/>
+      <c r="G104" s="36"/>
+      <c r="H104" s="37"/>
+    </row>
+    <row r="105" spans="1:8" ht="39" customHeight="1">
       <c r="A105" s="29"/>
       <c r="B105" s="30"/>
       <c r="C105" s="30"/>
       <c r="D105" s="31"/>
       <c r="E105" s="31"/>
-      <c r="F105" s="38"/>
-      <c r="G105" s="39"/>
-      <c r="H105" s="40"/>
-    </row>
-    <row r="106" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F105" s="35"/>
+      <c r="G105" s="36"/>
+      <c r="H105" s="37"/>
+    </row>
+    <row r="106" spans="1:8" ht="39" customHeight="1">
       <c r="A106" s="29"/>
       <c r="B106" s="30"/>
       <c r="C106" s="30"/>
       <c r="D106" s="31"/>
       <c r="E106" s="31"/>
-      <c r="F106" s="38"/>
-      <c r="G106" s="39"/>
-      <c r="H106" s="40"/>
-    </row>
-    <row r="107" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F106" s="35"/>
+      <c r="G106" s="36"/>
+      <c r="H106" s="37"/>
+    </row>
+    <row r="107" spans="1:8" ht="39" customHeight="1">
       <c r="A107" s="29"/>
       <c r="B107" s="30"/>
       <c r="C107" s="30"/>
       <c r="D107" s="31"/>
       <c r="E107" s="31"/>
-      <c r="F107" s="38"/>
-      <c r="G107" s="39"/>
-      <c r="H107" s="40"/>
-    </row>
-    <row r="108" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F107" s="35"/>
+      <c r="G107" s="36"/>
+      <c r="H107" s="37"/>
+    </row>
+    <row r="108" spans="1:8" ht="39" customHeight="1">
       <c r="A108" s="29"/>
       <c r="B108" s="30"/>
       <c r="C108" s="30"/>
       <c r="D108" s="31"/>
       <c r="E108" s="31"/>
-      <c r="F108" s="38"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="40"/>
-    </row>
-    <row r="109" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F108" s="35"/>
+      <c r="G108" s="36"/>
+      <c r="H108" s="37"/>
+    </row>
+    <row r="109" spans="1:8" ht="39" customHeight="1">
       <c r="A109" s="29"/>
       <c r="B109" s="30"/>
       <c r="C109" s="30"/>
       <c r="D109" s="31"/>
       <c r="E109" s="31"/>
-      <c r="F109" s="38"/>
-      <c r="G109" s="39"/>
-      <c r="H109" s="40"/>
-    </row>
-    <row r="110" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F109" s="35"/>
+      <c r="G109" s="36"/>
+      <c r="H109" s="37"/>
+    </row>
+    <row r="110" spans="1:8" ht="39" customHeight="1">
       <c r="A110" s="29"/>
       <c r="B110" s="30"/>
       <c r="C110" s="30"/>
       <c r="D110" s="31"/>
       <c r="E110" s="31"/>
-      <c r="F110" s="38"/>
-      <c r="G110" s="39"/>
-      <c r="H110" s="40"/>
-    </row>
-    <row r="111" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F110" s="35"/>
+      <c r="G110" s="36"/>
+      <c r="H110" s="37"/>
+    </row>
+    <row r="111" spans="1:8" ht="39" customHeight="1">
       <c r="A111" s="29"/>
       <c r="B111" s="30"/>
       <c r="C111" s="30"/>
       <c r="D111" s="31"/>
       <c r="E111" s="31"/>
-      <c r="F111" s="38"/>
-      <c r="G111" s="39"/>
-      <c r="H111" s="40"/>
-    </row>
-    <row r="112" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111" s="35"/>
+      <c r="G111" s="36"/>
+      <c r="H111" s="37"/>
+    </row>
+    <row r="112" spans="1:8" ht="39" customHeight="1">
       <c r="A112" s="29"/>
       <c r="B112" s="30"/>
       <c r="C112" s="30"/>
       <c r="D112" s="31"/>
       <c r="E112" s="31"/>
-      <c r="F112" s="38"/>
-      <c r="G112" s="39"/>
-      <c r="H112" s="40"/>
-    </row>
-    <row r="113" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F112" s="35"/>
+      <c r="G112" s="36"/>
+      <c r="H112" s="37"/>
+    </row>
+    <row r="113" spans="1:8" ht="39" customHeight="1">
       <c r="A113" s="29"/>
       <c r="B113" s="30"/>
       <c r="C113" s="30"/>
       <c r="D113" s="31"/>
       <c r="E113" s="31"/>
-      <c r="F113" s="38"/>
-      <c r="G113" s="39"/>
-      <c r="H113" s="40"/>
-    </row>
-    <row r="114" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F113" s="35"/>
+      <c r="G113" s="36"/>
+      <c r="H113" s="37"/>
+    </row>
+    <row r="114" spans="1:8" ht="39" customHeight="1">
       <c r="A114" s="29"/>
       <c r="B114" s="30"/>
       <c r="C114" s="30"/>
       <c r="D114" s="31"/>
       <c r="E114" s="31"/>
-      <c r="F114" s="38"/>
-      <c r="G114" s="39"/>
-      <c r="H114" s="40"/>
-    </row>
-    <row r="115" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F114" s="35"/>
+      <c r="G114" s="36"/>
+      <c r="H114" s="37"/>
+    </row>
+    <row r="115" spans="1:8" ht="39" customHeight="1">
       <c r="A115" s="29"/>
       <c r="B115" s="30"/>
       <c r="C115" s="30"/>
       <c r="D115" s="31"/>
       <c r="E115" s="31"/>
-      <c r="F115" s="38"/>
-      <c r="G115" s="39"/>
-      <c r="H115" s="40"/>
-    </row>
-    <row r="116" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F115" s="35"/>
+      <c r="G115" s="36"/>
+      <c r="H115" s="37"/>
+    </row>
+    <row r="116" spans="1:8" ht="39" customHeight="1">
       <c r="A116" s="29"/>
       <c r="B116" s="30"/>
       <c r="C116" s="30"/>
       <c r="D116" s="31"/>
       <c r="E116" s="31"/>
-      <c r="F116" s="38"/>
-      <c r="G116" s="39"/>
-      <c r="H116" s="40"/>
-    </row>
-    <row r="117" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F116" s="35"/>
+      <c r="G116" s="36"/>
+      <c r="H116" s="37"/>
+    </row>
+    <row r="117" spans="1:8" ht="39" customHeight="1">
       <c r="A117" s="29"/>
       <c r="B117" s="30"/>
       <c r="C117" s="30"/>
       <c r="D117" s="31"/>
       <c r="E117" s="31"/>
-      <c r="F117" s="38"/>
-      <c r="G117" s="39"/>
-      <c r="H117" s="40"/>
-    </row>
-    <row r="118" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F117" s="35"/>
+      <c r="G117" s="36"/>
+      <c r="H117" s="37"/>
+    </row>
+    <row r="118" spans="1:8" ht="39" customHeight="1">
       <c r="A118" s="29"/>
       <c r="B118" s="30"/>
       <c r="C118" s="30"/>
       <c r="D118" s="31"/>
       <c r="E118" s="31"/>
-      <c r="F118" s="38"/>
-      <c r="G118" s="39"/>
-      <c r="H118" s="40"/>
-    </row>
-    <row r="119" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F118" s="35"/>
+      <c r="G118" s="36"/>
+      <c r="H118" s="37"/>
+    </row>
+    <row r="119" spans="1:8" ht="39" customHeight="1">
       <c r="A119" s="29"/>
       <c r="B119" s="30"/>
       <c r="C119" s="30"/>
       <c r="D119" s="31"/>
       <c r="E119" s="31"/>
-      <c r="F119" s="38"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="40"/>
-    </row>
-    <row r="120" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F119" s="35"/>
+      <c r="G119" s="36"/>
+      <c r="H119" s="37"/>
+    </row>
+    <row r="120" spans="1:8" ht="39" customHeight="1">
       <c r="A120" s="29"/>
       <c r="B120" s="30"/>
       <c r="C120" s="30"/>
       <c r="D120" s="31"/>
       <c r="E120" s="31"/>
-      <c r="F120" s="38"/>
-      <c r="G120" s="39"/>
-      <c r="H120" s="40"/>
-    </row>
-    <row r="121" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F120" s="35"/>
+      <c r="G120" s="36"/>
+      <c r="H120" s="37"/>
+    </row>
+    <row r="121" spans="1:8" ht="39" customHeight="1">
       <c r="A121" s="29"/>
       <c r="B121" s="30"/>
       <c r="C121" s="30"/>
       <c r="D121" s="31"/>
       <c r="E121" s="31"/>
-      <c r="F121" s="38"/>
-      <c r="G121" s="39"/>
-      <c r="H121" s="40"/>
-    </row>
-    <row r="122" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F121" s="35"/>
+      <c r="G121" s="36"/>
+      <c r="H121" s="37"/>
+    </row>
+    <row r="122" spans="1:8" ht="39" customHeight="1">
       <c r="A122" s="29"/>
       <c r="B122" s="30"/>
       <c r="C122" s="30"/>
       <c r="D122" s="31"/>
       <c r="E122" s="31"/>
-      <c r="F122" s="38"/>
-      <c r="G122" s="39"/>
-      <c r="H122" s="40"/>
-    </row>
-    <row r="123" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F122" s="35"/>
+      <c r="G122" s="36"/>
+      <c r="H122" s="37"/>
+    </row>
+    <row r="123" spans="1:8" ht="39" customHeight="1">
       <c r="A123" s="29"/>
       <c r="B123" s="30"/>
       <c r="C123" s="30"/>
       <c r="D123" s="31"/>
       <c r="E123" s="31"/>
-      <c r="F123" s="38"/>
-      <c r="G123" s="39"/>
-      <c r="H123" s="40"/>
-    </row>
-    <row r="124" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F123" s="35"/>
+      <c r="G123" s="36"/>
+      <c r="H123" s="37"/>
+    </row>
+    <row r="124" spans="1:8" ht="39" customHeight="1">
       <c r="A124" s="29"/>
       <c r="B124" s="30"/>
       <c r="C124" s="30"/>
       <c r="D124" s="31"/>
       <c r="E124" s="31"/>
-      <c r="F124" s="38"/>
-      <c r="G124" s="39"/>
-      <c r="H124" s="40"/>
-    </row>
-    <row r="125" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F124" s="35"/>
+      <c r="G124" s="36"/>
+      <c r="H124" s="37"/>
+    </row>
+    <row r="125" spans="1:8" ht="39" customHeight="1">
       <c r="A125" s="29"/>
       <c r="B125" s="30"/>
       <c r="C125" s="30"/>
       <c r="D125" s="31"/>
       <c r="E125" s="31"/>
-      <c r="F125" s="38"/>
-      <c r="G125" s="39"/>
-      <c r="H125" s="40"/>
-    </row>
-    <row r="126" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F125" s="35"/>
+      <c r="G125" s="36"/>
+      <c r="H125" s="37"/>
+    </row>
+    <row r="126" spans="1:8" ht="39" customHeight="1">
       <c r="A126" s="29"/>
       <c r="B126" s="30"/>
       <c r="C126" s="30"/>
       <c r="D126" s="31"/>
       <c r="E126" s="31"/>
-      <c r="F126" s="38"/>
-      <c r="G126" s="39"/>
-      <c r="H126" s="40"/>
-    </row>
-    <row r="127" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F126" s="35"/>
+      <c r="G126" s="36"/>
+      <c r="H126" s="37"/>
+    </row>
+    <row r="127" spans="1:8" ht="39" customHeight="1">
       <c r="A127" s="29"/>
       <c r="B127" s="30"/>
       <c r="C127" s="30"/>
       <c r="D127" s="31"/>
       <c r="E127" s="31"/>
-      <c r="F127" s="38"/>
-      <c r="G127" s="39"/>
-      <c r="H127" s="40"/>
-    </row>
-    <row r="128" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F127" s="35"/>
+      <c r="G127" s="36"/>
+      <c r="H127" s="37"/>
+    </row>
+    <row r="128" spans="1:8" ht="39" customHeight="1">
       <c r="A128" s="29"/>
       <c r="B128" s="30"/>
       <c r="C128" s="30"/>
       <c r="D128" s="31"/>
       <c r="E128" s="31"/>
-      <c r="F128" s="38"/>
-      <c r="G128" s="39"/>
-      <c r="H128" s="40"/>
-    </row>
-    <row r="129" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F128" s="35"/>
+      <c r="G128" s="36"/>
+      <c r="H128" s="37"/>
+    </row>
+    <row r="129" spans="1:8" ht="39" customHeight="1">
       <c r="A129" s="29"/>
       <c r="B129" s="30"/>
       <c r="C129" s="30"/>
       <c r="D129" s="31"/>
       <c r="E129" s="31"/>
-      <c r="F129" s="38"/>
-      <c r="G129" s="39"/>
-      <c r="H129" s="40"/>
-    </row>
-    <row r="130" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F129" s="35"/>
+      <c r="G129" s="36"/>
+      <c r="H129" s="37"/>
+    </row>
+    <row r="130" spans="1:8" ht="39" customHeight="1">
       <c r="A130" s="29"/>
       <c r="B130" s="30"/>
       <c r="C130" s="30"/>
       <c r="D130" s="31"/>
       <c r="E130" s="31"/>
-      <c r="F130" s="38"/>
-      <c r="G130" s="39"/>
-      <c r="H130" s="40"/>
-    </row>
-    <row r="131" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F130" s="35"/>
+      <c r="G130" s="36"/>
+      <c r="H130" s="37"/>
+    </row>
+    <row r="131" spans="1:8" ht="39" customHeight="1">
       <c r="A131" s="29"/>
       <c r="B131" s="30"/>
       <c r="C131" s="30"/>
       <c r="D131" s="31"/>
       <c r="E131" s="31"/>
-      <c r="F131" s="38"/>
-      <c r="G131" s="39"/>
-      <c r="H131" s="40"/>
-    </row>
-    <row r="132" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F131" s="35"/>
+      <c r="G131" s="36"/>
+      <c r="H131" s="37"/>
+    </row>
+    <row r="132" spans="1:8" ht="39" customHeight="1">
       <c r="A132" s="29"/>
       <c r="B132" s="30"/>
       <c r="C132" s="30"/>
       <c r="D132" s="31"/>
       <c r="E132" s="31"/>
-      <c r="F132" s="38"/>
-      <c r="G132" s="39"/>
-      <c r="H132" s="40"/>
-    </row>
-    <row r="133" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F132" s="35"/>
+      <c r="G132" s="36"/>
+      <c r="H132" s="37"/>
+    </row>
+    <row r="133" spans="1:8" ht="39" customHeight="1">
       <c r="A133" s="29"/>
       <c r="B133" s="30"/>
       <c r="C133" s="30"/>
       <c r="D133" s="31"/>
       <c r="E133" s="31"/>
-      <c r="F133" s="38"/>
-      <c r="G133" s="39"/>
-      <c r="H133" s="40"/>
-    </row>
-    <row r="134" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F133" s="35"/>
+      <c r="G133" s="36"/>
+      <c r="H133" s="37"/>
+    </row>
+    <row r="134" spans="1:8" ht="39" customHeight="1">
       <c r="A134" s="29"/>
       <c r="B134" s="30"/>
       <c r="C134" s="30"/>
       <c r="D134" s="31"/>
       <c r="E134" s="31"/>
-      <c r="F134" s="38"/>
-      <c r="G134" s="39"/>
-      <c r="H134" s="40"/>
-    </row>
-    <row r="135" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F134" s="35"/>
+      <c r="G134" s="36"/>
+      <c r="H134" s="37"/>
+    </row>
+    <row r="135" spans="1:8" ht="39" customHeight="1">
       <c r="A135" s="29"/>
       <c r="B135" s="30"/>
       <c r="C135" s="30"/>
       <c r="D135" s="31"/>
       <c r="E135" s="31"/>
-      <c r="F135" s="38"/>
-      <c r="G135" s="39"/>
-      <c r="H135" s="40"/>
-    </row>
-    <row r="136" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F135" s="35"/>
+      <c r="G135" s="36"/>
+      <c r="H135" s="37"/>
+    </row>
+    <row r="136" spans="1:8" ht="39" customHeight="1">
       <c r="A136" s="29"/>
       <c r="B136" s="30"/>
       <c r="C136" s="30"/>
       <c r="D136" s="31"/>
       <c r="E136" s="31"/>
-      <c r="F136" s="38"/>
-      <c r="G136" s="39"/>
-      <c r="H136" s="40"/>
-    </row>
-    <row r="137" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F136" s="35"/>
+      <c r="G136" s="36"/>
+      <c r="H136" s="37"/>
+    </row>
+    <row r="137" spans="1:8" ht="39" customHeight="1">
       <c r="A137" s="29"/>
       <c r="B137" s="30"/>
       <c r="C137" s="30"/>
       <c r="D137" s="31"/>
       <c r="E137" s="31"/>
-      <c r="F137" s="38"/>
-      <c r="G137" s="39"/>
-      <c r="H137" s="40"/>
-    </row>
-    <row r="138" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F137" s="35"/>
+      <c r="G137" s="36"/>
+      <c r="H137" s="37"/>
+    </row>
+    <row r="138" spans="1:8" ht="39" customHeight="1">
       <c r="A138" s="29"/>
       <c r="B138" s="30"/>
       <c r="C138" s="30"/>
       <c r="D138" s="31"/>
       <c r="E138" s="31"/>
-      <c r="F138" s="38"/>
-      <c r="G138" s="39"/>
-      <c r="H138" s="40"/>
-    </row>
-    <row r="139" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F138" s="35"/>
+      <c r="G138" s="36"/>
+      <c r="H138" s="37"/>
+    </row>
+    <row r="139" spans="1:8" ht="39" customHeight="1">
       <c r="A139" s="29"/>
       <c r="B139" s="30"/>
       <c r="C139" s="30"/>
       <c r="D139" s="31"/>
       <c r="E139" s="31"/>
-      <c r="F139" s="38"/>
-      <c r="G139" s="39"/>
-      <c r="H139" s="40"/>
-    </row>
-    <row r="140" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F139" s="35"/>
+      <c r="G139" s="36"/>
+      <c r="H139" s="37"/>
+    </row>
+    <row r="140" spans="1:8" ht="39" customHeight="1">
       <c r="A140" s="29"/>
       <c r="B140" s="30"/>
       <c r="C140" s="30"/>
       <c r="D140" s="31"/>
       <c r="E140" s="31"/>
-      <c r="F140" s="38"/>
-      <c r="G140" s="39"/>
-      <c r="H140" s="40"/>
-    </row>
-    <row r="141" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F140" s="35"/>
+      <c r="G140" s="36"/>
+      <c r="H140" s="37"/>
+    </row>
+    <row r="141" spans="1:8" ht="39" customHeight="1">
       <c r="A141" s="29"/>
       <c r="B141" s="30"/>
       <c r="C141" s="30"/>
       <c r="D141" s="31"/>
       <c r="E141" s="31"/>
-      <c r="F141" s="38"/>
-      <c r="G141" s="39"/>
-      <c r="H141" s="40"/>
-    </row>
-    <row r="142" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F141" s="35"/>
+      <c r="G141" s="36"/>
+      <c r="H141" s="37"/>
+    </row>
+    <row r="142" spans="1:8" ht="39" customHeight="1">
       <c r="A142" s="29"/>
       <c r="B142" s="30"/>
       <c r="C142" s="30"/>
       <c r="D142" s="31"/>
       <c r="E142" s="31"/>
-      <c r="F142" s="38"/>
-      <c r="G142" s="39"/>
-      <c r="H142" s="40"/>
-    </row>
-    <row r="143" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F142" s="35"/>
+      <c r="G142" s="36"/>
+      <c r="H142" s="37"/>
+    </row>
+    <row r="143" spans="1:8" ht="39" customHeight="1">
       <c r="A143" s="29"/>
       <c r="B143" s="30"/>
       <c r="C143" s="30"/>
       <c r="D143" s="31"/>
       <c r="E143" s="31"/>
-      <c r="F143" s="38"/>
-      <c r="G143" s="39"/>
-      <c r="H143" s="40"/>
-    </row>
-    <row r="144" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F143" s="35"/>
+      <c r="G143" s="36"/>
+      <c r="H143" s="37"/>
+    </row>
+    <row r="144" spans="1:8" ht="39" customHeight="1">
       <c r="A144" s="29"/>
       <c r="B144" s="30"/>
       <c r="C144" s="30"/>
       <c r="D144" s="31"/>
       <c r="E144" s="31"/>
-      <c r="F144" s="38"/>
-      <c r="G144" s="39"/>
-      <c r="H144" s="40"/>
-    </row>
-    <row r="145" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F144" s="35"/>
+      <c r="G144" s="36"/>
+      <c r="H144" s="37"/>
+    </row>
+    <row r="145" spans="1:8" ht="39" customHeight="1">
       <c r="A145" s="29"/>
       <c r="B145" s="30"/>
       <c r="C145" s="30"/>
       <c r="D145" s="31"/>
       <c r="E145" s="31"/>
-      <c r="F145" s="38"/>
-      <c r="G145" s="39"/>
-      <c r="H145" s="40"/>
-    </row>
-    <row r="146" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F145" s="35"/>
+      <c r="G145" s="36"/>
+      <c r="H145" s="37"/>
+    </row>
+    <row r="146" spans="1:8" ht="39" customHeight="1">
       <c r="A146" s="29"/>
       <c r="B146" s="30"/>
       <c r="C146" s="30"/>
       <c r="D146" s="31"/>
       <c r="E146" s="31"/>
-      <c r="F146" s="38"/>
-      <c r="G146" s="39"/>
-      <c r="H146" s="40"/>
-    </row>
-    <row r="147" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F146" s="35"/>
+      <c r="G146" s="36"/>
+      <c r="H146" s="37"/>
+    </row>
+    <row r="147" spans="1:8" ht="39" customHeight="1">
       <c r="A147" s="29"/>
       <c r="B147" s="30"/>
       <c r="C147" s="30"/>
       <c r="D147" s="31"/>
       <c r="E147" s="31"/>
-      <c r="F147" s="38"/>
-      <c r="G147" s="39"/>
-      <c r="H147" s="40"/>
-    </row>
-    <row r="148" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F147" s="35"/>
+      <c r="G147" s="36"/>
+      <c r="H147" s="37"/>
+    </row>
+    <row r="148" spans="1:8" ht="39" customHeight="1">
       <c r="A148" s="29"/>
       <c r="B148" s="30"/>
       <c r="C148" s="30"/>
       <c r="D148" s="31"/>
       <c r="E148" s="31"/>
-      <c r="F148" s="38"/>
-      <c r="G148" s="39"/>
-      <c r="H148" s="40"/>
-    </row>
-    <row r="149" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F148" s="35"/>
+      <c r="G148" s="36"/>
+      <c r="H148" s="37"/>
+    </row>
+    <row r="149" spans="1:8" ht="39" customHeight="1">
       <c r="A149" s="29"/>
       <c r="B149" s="30"/>
       <c r="C149" s="30"/>
       <c r="D149" s="31"/>
       <c r="E149" s="31"/>
-      <c r="F149" s="38"/>
-      <c r="G149" s="39"/>
-      <c r="H149" s="40"/>
-    </row>
-    <row r="150" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F149" s="35"/>
+      <c r="G149" s="36"/>
+      <c r="H149" s="37"/>
+    </row>
+    <row r="150" spans="1:8" ht="39" customHeight="1">
       <c r="A150" s="29"/>
       <c r="B150" s="30"/>
       <c r="C150" s="30"/>
       <c r="D150" s="31"/>
       <c r="E150" s="31"/>
-      <c r="F150" s="38"/>
-      <c r="G150" s="39"/>
-      <c r="H150" s="40"/>
-    </row>
-    <row r="151" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F150" s="35"/>
+      <c r="G150" s="36"/>
+      <c r="H150" s="37"/>
+    </row>
+    <row r="151" spans="1:8" ht="39" customHeight="1">
       <c r="A151" s="29"/>
       <c r="B151" s="30"/>
       <c r="C151" s="30"/>
       <c r="D151" s="31"/>
       <c r="E151" s="31"/>
-      <c r="F151" s="38"/>
-      <c r="G151" s="39"/>
-      <c r="H151" s="40"/>
-    </row>
-    <row r="152" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F151" s="35"/>
+      <c r="G151" s="36"/>
+      <c r="H151" s="37"/>
+    </row>
+    <row r="152" spans="1:8" ht="39" customHeight="1">
       <c r="A152" s="29"/>
       <c r="B152" s="30"/>
       <c r="C152" s="30"/>
       <c r="D152" s="31"/>
       <c r="E152" s="31"/>
-      <c r="F152" s="38"/>
-      <c r="G152" s="39"/>
-      <c r="H152" s="40"/>
-    </row>
-    <row r="153" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F152" s="35"/>
+      <c r="G152" s="36"/>
+      <c r="H152" s="37"/>
+    </row>
+    <row r="153" spans="1:8" ht="39" customHeight="1">
       <c r="A153" s="29"/>
       <c r="B153" s="30"/>
       <c r="C153" s="30"/>
       <c r="D153" s="31"/>
       <c r="E153" s="31"/>
-      <c r="F153" s="38"/>
-      <c r="G153" s="39"/>
-      <c r="H153" s="40"/>
-    </row>
-    <row r="154" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F153" s="35"/>
+      <c r="G153" s="36"/>
+      <c r="H153" s="37"/>
+    </row>
+    <row r="154" spans="1:8" ht="39" customHeight="1">
       <c r="A154" s="29"/>
       <c r="B154" s="30"/>
       <c r="C154" s="30"/>
       <c r="D154" s="31"/>
       <c r="E154" s="31"/>
-      <c r="F154" s="38"/>
-      <c r="G154" s="39"/>
-      <c r="H154" s="40"/>
-    </row>
-    <row r="155" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F154" s="35"/>
+      <c r="G154" s="36"/>
+      <c r="H154" s="37"/>
+    </row>
+    <row r="155" spans="1:8" ht="39" customHeight="1">
       <c r="A155" s="29"/>
       <c r="B155" s="30"/>
       <c r="C155" s="30"/>
       <c r="D155" s="31"/>
       <c r="E155" s="31"/>
-      <c r="F155" s="38"/>
-      <c r="G155" s="39"/>
-      <c r="H155" s="40"/>
-    </row>
-    <row r="156" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F155" s="35"/>
+      <c r="G155" s="36"/>
+      <c r="H155" s="37"/>
+    </row>
+    <row r="156" spans="1:8" ht="39" customHeight="1">
       <c r="A156" s="29"/>
       <c r="B156" s="30"/>
       <c r="C156" s="30"/>
       <c r="D156" s="31"/>
       <c r="E156" s="31"/>
-      <c r="F156" s="38"/>
-      <c r="G156" s="39"/>
-      <c r="H156" s="40"/>
-    </row>
-    <row r="157" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F156" s="35"/>
+      <c r="G156" s="36"/>
+      <c r="H156" s="37"/>
+    </row>
+    <row r="157" spans="1:8" ht="39" customHeight="1">
       <c r="A157" s="29"/>
       <c r="B157" s="30"/>
       <c r="C157" s="30"/>
       <c r="D157" s="31"/>
       <c r="E157" s="31"/>
-      <c r="F157" s="38"/>
-      <c r="G157" s="39"/>
-      <c r="H157" s="40"/>
-    </row>
-    <row r="158" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F157" s="35"/>
+      <c r="G157" s="36"/>
+      <c r="H157" s="37"/>
+    </row>
+    <row r="158" spans="1:8" ht="39" customHeight="1">
       <c r="A158" s="29"/>
       <c r="B158" s="30"/>
       <c r="C158" s="30"/>
       <c r="D158" s="31"/>
       <c r="E158" s="31"/>
-      <c r="F158" s="38"/>
-      <c r="G158" s="39"/>
-      <c r="H158" s="40"/>
-    </row>
-    <row r="159" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F158" s="35"/>
+      <c r="G158" s="36"/>
+      <c r="H158" s="37"/>
+    </row>
+    <row r="159" spans="1:8" ht="39" customHeight="1">
       <c r="A159" s="29"/>
       <c r="B159" s="30"/>
       <c r="C159" s="30"/>
       <c r="D159" s="31"/>
       <c r="E159" s="31"/>
-      <c r="F159" s="38"/>
-      <c r="G159" s="39"/>
-      <c r="H159" s="40"/>
-    </row>
-    <row r="160" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F159" s="35"/>
+      <c r="G159" s="36"/>
+      <c r="H159" s="37"/>
+    </row>
+    <row r="160" spans="1:8" ht="39" customHeight="1">
       <c r="A160" s="29"/>
       <c r="B160" s="30"/>
       <c r="C160" s="30"/>
       <c r="D160" s="31"/>
       <c r="E160" s="31"/>
-      <c r="F160" s="38"/>
-      <c r="G160" s="39"/>
-      <c r="H160" s="40"/>
-    </row>
-    <row r="161" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F160" s="35"/>
+      <c r="G160" s="36"/>
+      <c r="H160" s="37"/>
+    </row>
+    <row r="161" spans="1:8" ht="39" customHeight="1">
       <c r="A161" s="29"/>
       <c r="B161" s="30"/>
       <c r="C161" s="30"/>
       <c r="D161" s="31"/>
       <c r="E161" s="31"/>
-      <c r="F161" s="38"/>
-      <c r="G161" s="39"/>
-      <c r="H161" s="40"/>
-    </row>
-    <row r="162" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F161" s="35"/>
+      <c r="G161" s="36"/>
+      <c r="H161" s="37"/>
+    </row>
+    <row r="162" spans="1:8" ht="39" customHeight="1">
       <c r="A162" s="29"/>
       <c r="B162" s="30"/>
       <c r="C162" s="30"/>
       <c r="D162" s="31"/>
       <c r="E162" s="31"/>
-      <c r="F162" s="38"/>
-      <c r="G162" s="39"/>
-      <c r="H162" s="40"/>
-    </row>
-    <row r="163" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F162" s="35"/>
+      <c r="G162" s="36"/>
+      <c r="H162" s="37"/>
+    </row>
+    <row r="163" spans="1:8" ht="39" customHeight="1">
       <c r="A163" s="29"/>
       <c r="B163" s="30"/>
       <c r="C163" s="30"/>
       <c r="D163" s="31"/>
       <c r="E163" s="31"/>
-      <c r="F163" s="38"/>
-      <c r="G163" s="39"/>
-      <c r="H163" s="40"/>
-    </row>
-    <row r="164" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F163" s="35"/>
+      <c r="G163" s="36"/>
+      <c r="H163" s="37"/>
+    </row>
+    <row r="164" spans="1:8" ht="39" customHeight="1">
       <c r="A164" s="29"/>
       <c r="B164" s="30"/>
       <c r="C164" s="30"/>
       <c r="D164" s="31"/>
       <c r="E164" s="31"/>
-      <c r="F164" s="38"/>
-      <c r="G164" s="39"/>
-      <c r="H164" s="40"/>
-    </row>
-    <row r="165" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F164" s="35"/>
+      <c r="G164" s="36"/>
+      <c r="H164" s="37"/>
+    </row>
+    <row r="165" spans="1:8" ht="39" customHeight="1">
       <c r="A165" s="29"/>
       <c r="B165" s="30"/>
       <c r="C165" s="30"/>
       <c r="D165" s="31"/>
       <c r="E165" s="31"/>
-      <c r="F165" s="38"/>
-      <c r="G165" s="39"/>
-      <c r="H165" s="40"/>
-    </row>
-    <row r="166" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F165" s="35"/>
+      <c r="G165" s="36"/>
+      <c r="H165" s="37"/>
+    </row>
+    <row r="166" spans="1:8" ht="39" customHeight="1">
       <c r="A166" s="29"/>
       <c r="B166" s="30"/>
       <c r="C166" s="30"/>
       <c r="D166" s="31"/>
       <c r="E166" s="31"/>
-      <c r="F166" s="38"/>
-      <c r="G166" s="39"/>
-      <c r="H166" s="40"/>
-    </row>
-    <row r="167" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F166" s="35"/>
+      <c r="G166" s="36"/>
+      <c r="H166" s="37"/>
+    </row>
+    <row r="167" spans="1:8" ht="39" customHeight="1">
       <c r="A167" s="29"/>
       <c r="B167" s="30"/>
       <c r="C167" s="30"/>
       <c r="D167" s="31"/>
       <c r="E167" s="31"/>
-      <c r="F167" s="38"/>
-      <c r="G167" s="39"/>
-      <c r="H167" s="40"/>
-    </row>
-    <row r="168" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F167" s="35"/>
+      <c r="G167" s="36"/>
+      <c r="H167" s="37"/>
+    </row>
+    <row r="168" spans="1:8" ht="39" customHeight="1">
       <c r="A168" s="29"/>
       <c r="B168" s="30"/>
       <c r="C168" s="30"/>
       <c r="D168" s="31"/>
       <c r="E168" s="31"/>
-      <c r="F168" s="38"/>
-      <c r="G168" s="39"/>
-      <c r="H168" s="40"/>
-    </row>
-    <row r="169" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F168" s="35"/>
+      <c r="G168" s="36"/>
+      <c r="H168" s="37"/>
+    </row>
+    <row r="169" spans="1:8" ht="39" customHeight="1">
       <c r="A169" s="29"/>
       <c r="B169" s="30"/>
       <c r="C169" s="30"/>
       <c r="D169" s="31"/>
       <c r="E169" s="31"/>
-      <c r="F169" s="38"/>
-      <c r="G169" s="39"/>
-      <c r="H169" s="40"/>
-    </row>
-    <row r="170" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F169" s="35"/>
+      <c r="G169" s="36"/>
+      <c r="H169" s="37"/>
+    </row>
+    <row r="170" spans="1:8" ht="39" customHeight="1">
       <c r="A170" s="29"/>
       <c r="B170" s="30"/>
       <c r="C170" s="30"/>
       <c r="D170" s="31"/>
       <c r="E170" s="31"/>
-      <c r="F170" s="38"/>
-      <c r="G170" s="39"/>
-      <c r="H170" s="40"/>
-    </row>
-    <row r="171" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F170" s="35"/>
+      <c r="G170" s="36"/>
+      <c r="H170" s="37"/>
+    </row>
+    <row r="171" spans="1:8" ht="39" customHeight="1">
       <c r="A171" s="29"/>
       <c r="B171" s="30"/>
       <c r="C171" s="30"/>
       <c r="D171" s="31"/>
       <c r="E171" s="31"/>
-      <c r="F171" s="38"/>
-      <c r="G171" s="39"/>
-      <c r="H171" s="40"/>
-    </row>
-    <row r="172" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F171" s="35"/>
+      <c r="G171" s="36"/>
+      <c r="H171" s="37"/>
+    </row>
+    <row r="172" spans="1:8" ht="39" customHeight="1">
       <c r="A172" s="29"/>
       <c r="B172" s="30"/>
       <c r="C172" s="30"/>
       <c r="D172" s="31"/>
       <c r="E172" s="31"/>
-      <c r="F172" s="38"/>
-      <c r="G172" s="39"/>
-      <c r="H172" s="40"/>
-    </row>
-    <row r="173" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F172" s="35"/>
+      <c r="G172" s="36"/>
+      <c r="H172" s="37"/>
+    </row>
+    <row r="173" spans="1:8" ht="39" customHeight="1">
       <c r="A173" s="29"/>
       <c r="B173" s="30"/>
       <c r="C173" s="30"/>
       <c r="D173" s="31"/>
       <c r="E173" s="31"/>
-      <c r="F173" s="38"/>
-      <c r="G173" s="39"/>
-      <c r="H173" s="40"/>
-    </row>
-    <row r="174" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F173" s="35"/>
+      <c r="G173" s="36"/>
+      <c r="H173" s="37"/>
+    </row>
+    <row r="174" spans="1:8" ht="39" customHeight="1">
       <c r="A174" s="29"/>
       <c r="B174" s="30"/>
       <c r="C174" s="30"/>
       <c r="D174" s="31"/>
       <c r="E174" s="31"/>
-      <c r="F174" s="38"/>
-      <c r="G174" s="39"/>
-      <c r="H174" s="40"/>
-    </row>
-    <row r="175" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F174" s="35"/>
+      <c r="G174" s="36"/>
+      <c r="H174" s="37"/>
+    </row>
+    <row r="175" spans="1:8" ht="39" customHeight="1">
       <c r="A175" s="29"/>
       <c r="B175" s="30"/>
       <c r="C175" s="30"/>
       <c r="D175" s="31"/>
       <c r="E175" s="31"/>
-      <c r="F175" s="38"/>
-      <c r="G175" s="39"/>
-      <c r="H175" s="40"/>
-    </row>
-    <row r="176" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F175" s="35"/>
+      <c r="G175" s="36"/>
+      <c r="H175" s="37"/>
+    </row>
+    <row r="176" spans="1:8" ht="39" customHeight="1">
       <c r="A176" s="29"/>
       <c r="B176" s="30"/>
       <c r="C176" s="30"/>
       <c r="D176" s="31"/>
       <c r="E176" s="31"/>
-      <c r="F176" s="38"/>
-      <c r="G176" s="39"/>
-      <c r="H176" s="40"/>
-    </row>
-    <row r="177" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F176" s="35"/>
+      <c r="G176" s="36"/>
+      <c r="H176" s="37"/>
+    </row>
+    <row r="177" spans="1:8" ht="39" customHeight="1">
       <c r="A177" s="29"/>
       <c r="B177" s="30"/>
       <c r="C177" s="30"/>
       <c r="D177" s="31"/>
       <c r="E177" s="31"/>
-      <c r="F177" s="38"/>
-      <c r="G177" s="39"/>
-      <c r="H177" s="40"/>
-    </row>
-    <row r="178" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F177" s="35"/>
+      <c r="G177" s="36"/>
+      <c r="H177" s="37"/>
+    </row>
+    <row r="178" spans="1:8" ht="39" customHeight="1">
       <c r="A178" s="29"/>
       <c r="B178" s="30"/>
       <c r="C178" s="30"/>
       <c r="D178" s="31"/>
       <c r="E178" s="31"/>
-      <c r="F178" s="38"/>
-      <c r="G178" s="39"/>
-      <c r="H178" s="40"/>
-    </row>
-    <row r="179" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F178" s="35"/>
+      <c r="G178" s="36"/>
+      <c r="H178" s="37"/>
+    </row>
+    <row r="179" spans="1:8" ht="39" customHeight="1">
       <c r="A179" s="29"/>
       <c r="B179" s="30"/>
       <c r="C179" s="30"/>
       <c r="D179" s="31"/>
       <c r="E179" s="31"/>
-      <c r="F179" s="38"/>
-      <c r="G179" s="39"/>
-      <c r="H179" s="40"/>
-    </row>
-    <row r="180" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F179" s="35"/>
+      <c r="G179" s="36"/>
+      <c r="H179" s="37"/>
+    </row>
+    <row r="180" spans="1:8" ht="39" customHeight="1">
       <c r="A180" s="29"/>
       <c r="B180" s="30"/>
       <c r="C180" s="30"/>
       <c r="D180" s="31"/>
       <c r="E180" s="31"/>
-      <c r="F180" s="38"/>
-      <c r="G180" s="39"/>
-      <c r="H180" s="40"/>
-    </row>
-    <row r="181" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F180" s="35"/>
+      <c r="G180" s="36"/>
+      <c r="H180" s="37"/>
+    </row>
+    <row r="181" spans="1:8" ht="39" customHeight="1">
       <c r="A181" s="29"/>
       <c r="B181" s="30"/>
       <c r="C181" s="30"/>
       <c r="D181" s="31"/>
       <c r="E181" s="31"/>
-      <c r="F181" s="38"/>
-      <c r="G181" s="39"/>
-      <c r="H181" s="40"/>
-    </row>
-    <row r="182" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F181" s="35"/>
+      <c r="G181" s="36"/>
+      <c r="H181" s="37"/>
+    </row>
+    <row r="182" spans="1:8" ht="39" customHeight="1">
       <c r="A182" s="29"/>
       <c r="B182" s="30"/>
       <c r="C182" s="30"/>
       <c r="D182" s="31"/>
       <c r="E182" s="31"/>
-      <c r="F182" s="38"/>
-      <c r="G182" s="39"/>
-      <c r="H182" s="40"/>
-    </row>
-    <row r="183" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F182" s="35"/>
+      <c r="G182" s="36"/>
+      <c r="H182" s="37"/>
+    </row>
+    <row r="183" spans="1:8" ht="39" customHeight="1">
       <c r="A183" s="29"/>
       <c r="B183" s="30"/>
       <c r="C183" s="30"/>
       <c r="D183" s="31"/>
       <c r="E183" s="31"/>
-      <c r="F183" s="38"/>
-      <c r="G183" s="39"/>
-      <c r="H183" s="40"/>
-    </row>
-    <row r="184" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F183" s="35"/>
+      <c r="G183" s="36"/>
+      <c r="H183" s="37"/>
+    </row>
+    <row r="184" spans="1:8" ht="39" customHeight="1">
       <c r="A184" s="29"/>
       <c r="B184" s="30"/>
       <c r="C184" s="30"/>
       <c r="D184" s="31"/>
       <c r="E184" s="31"/>
-      <c r="F184" s="38"/>
-      <c r="G184" s="39"/>
-      <c r="H184" s="40"/>
-    </row>
-    <row r="185" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F184" s="35"/>
+      <c r="G184" s="36"/>
+      <c r="H184" s="37"/>
+    </row>
+    <row r="185" spans="1:8" ht="39" customHeight="1">
       <c r="A185" s="29"/>
       <c r="B185" s="30"/>
       <c r="C185" s="30"/>
       <c r="D185" s="31"/>
       <c r="E185" s="31"/>
-      <c r="F185" s="38"/>
-      <c r="G185" s="39"/>
-      <c r="H185" s="40"/>
-    </row>
-    <row r="186" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F185" s="35"/>
+      <c r="G185" s="36"/>
+      <c r="H185" s="37"/>
+    </row>
+    <row r="186" spans="1:8" ht="39" customHeight="1">
       <c r="A186" s="29"/>
       <c r="B186" s="30"/>
       <c r="C186" s="30"/>
       <c r="D186" s="31"/>
       <c r="E186" s="31"/>
-      <c r="F186" s="38"/>
-      <c r="G186" s="39"/>
-      <c r="H186" s="40"/>
-    </row>
-    <row r="187" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F186" s="35"/>
+      <c r="G186" s="36"/>
+      <c r="H186" s="37"/>
+    </row>
+    <row r="187" spans="1:8" ht="39" customHeight="1">
       <c r="A187" s="29"/>
       <c r="B187" s="30"/>
       <c r="C187" s="30"/>
       <c r="D187" s="31"/>
       <c r="E187" s="31"/>
-      <c r="F187" s="38"/>
-      <c r="G187" s="39"/>
-      <c r="H187" s="40"/>
-    </row>
-    <row r="188" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F187" s="35"/>
+      <c r="G187" s="36"/>
+      <c r="H187" s="37"/>
+    </row>
+    <row r="188" spans="1:8" ht="39" customHeight="1">
       <c r="A188" s="29"/>
       <c r="B188" s="30"/>
       <c r="C188" s="30"/>
       <c r="D188" s="31"/>
       <c r="E188" s="31"/>
-      <c r="F188" s="38"/>
-      <c r="G188" s="39"/>
-      <c r="H188" s="40"/>
-    </row>
-    <row r="189" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F188" s="35"/>
+      <c r="G188" s="36"/>
+      <c r="H188" s="37"/>
+    </row>
+    <row r="189" spans="1:8" ht="39" customHeight="1">
       <c r="A189" s="29"/>
       <c r="B189" s="30"/>
       <c r="C189" s="30"/>
       <c r="D189" s="31"/>
       <c r="E189" s="31"/>
-      <c r="F189" s="38"/>
-      <c r="G189" s="39"/>
-      <c r="H189" s="40"/>
-    </row>
-    <row r="190" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F189" s="35"/>
+      <c r="G189" s="36"/>
+      <c r="H189" s="37"/>
+    </row>
+    <row r="190" spans="1:8" ht="39" customHeight="1">
       <c r="A190" s="29"/>
       <c r="B190" s="30"/>
       <c r="C190" s="30"/>
       <c r="D190" s="31"/>
       <c r="E190" s="31"/>
-      <c r="F190" s="38"/>
-      <c r="G190" s="39"/>
-      <c r="H190" s="40"/>
-    </row>
-    <row r="191" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F190" s="35"/>
+      <c r="G190" s="36"/>
+      <c r="H190" s="37"/>
+    </row>
+    <row r="191" spans="1:8" ht="39" customHeight="1">
       <c r="A191" s="29"/>
       <c r="B191" s="30"/>
       <c r="C191" s="30"/>
       <c r="D191" s="31"/>
       <c r="E191" s="31"/>
-      <c r="F191" s="38"/>
-      <c r="G191" s="39"/>
-      <c r="H191" s="40"/>
-    </row>
-    <row r="192" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F191" s="35"/>
+      <c r="G191" s="36"/>
+      <c r="H191" s="37"/>
+    </row>
+    <row r="192" spans="1:8" ht="39" customHeight="1">
       <c r="A192" s="29"/>
       <c r="B192" s="30"/>
       <c r="C192" s="30"/>
       <c r="D192" s="31"/>
       <c r="E192" s="31"/>
-      <c r="F192" s="38"/>
-      <c r="G192" s="39"/>
-      <c r="H192" s="40"/>
-    </row>
-    <row r="193" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F192" s="35"/>
+      <c r="G192" s="36"/>
+      <c r="H192" s="37"/>
+    </row>
+    <row r="193" spans="1:8" ht="39" customHeight="1">
       <c r="A193" s="29"/>
       <c r="B193" s="30"/>
       <c r="C193" s="30"/>
       <c r="D193" s="31"/>
       <c r="E193" s="31"/>
-      <c r="F193" s="38"/>
-      <c r="G193" s="39"/>
-      <c r="H193" s="40"/>
-    </row>
-    <row r="194" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F193" s="35"/>
+      <c r="G193" s="36"/>
+      <c r="H193" s="37"/>
+    </row>
+    <row r="194" spans="1:8" ht="39" customHeight="1">
       <c r="A194" s="29"/>
       <c r="B194" s="30"/>
       <c r="C194" s="30"/>
       <c r="D194" s="31"/>
       <c r="E194" s="31"/>
-      <c r="F194" s="38"/>
-      <c r="G194" s="39"/>
-      <c r="H194" s="40"/>
-    </row>
-    <row r="195" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F194" s="35"/>
+      <c r="G194" s="36"/>
+      <c r="H194" s="37"/>
+    </row>
+    <row r="195" spans="1:8" ht="39" customHeight="1">
       <c r="A195" s="29"/>
       <c r="B195" s="30"/>
       <c r="C195" s="30"/>
       <c r="D195" s="31"/>
       <c r="E195" s="31"/>
-      <c r="F195" s="38"/>
-      <c r="G195" s="39"/>
-      <c r="H195" s="40"/>
-    </row>
-    <row r="196" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F195" s="35"/>
+      <c r="G195" s="36"/>
+      <c r="H195" s="37"/>
+    </row>
+    <row r="196" spans="1:8" ht="39" customHeight="1">
       <c r="A196" s="29"/>
       <c r="B196" s="30"/>
       <c r="C196" s="30"/>
       <c r="D196" s="31"/>
       <c r="E196" s="31"/>
-      <c r="F196" s="38"/>
-      <c r="G196" s="39"/>
-      <c r="H196" s="40"/>
-    </row>
-    <row r="197" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F196" s="35"/>
+      <c r="G196" s="36"/>
+      <c r="H196" s="37"/>
+    </row>
+    <row r="197" spans="1:8" ht="39" customHeight="1">
       <c r="A197" s="29"/>
       <c r="B197" s="30"/>
       <c r="C197" s="30"/>
       <c r="D197" s="31"/>
       <c r="E197" s="31"/>
-      <c r="F197" s="38"/>
-      <c r="G197" s="39"/>
-      <c r="H197" s="40"/>
-    </row>
-    <row r="198" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F197" s="35"/>
+      <c r="G197" s="36"/>
+      <c r="H197" s="37"/>
+    </row>
+    <row r="198" spans="1:8" ht="39" customHeight="1">
       <c r="A198" s="29"/>
       <c r="B198" s="30"/>
       <c r="C198" s="30"/>
       <c r="D198" s="31"/>
       <c r="E198" s="31"/>
-      <c r="F198" s="38"/>
-      <c r="G198" s="39"/>
-      <c r="H198" s="40"/>
-    </row>
-    <row r="199" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F198" s="35"/>
+      <c r="G198" s="36"/>
+      <c r="H198" s="37"/>
+    </row>
+    <row r="199" spans="1:8" ht="39" customHeight="1">
       <c r="A199" s="29"/>
       <c r="B199" s="30"/>
       <c r="C199" s="30"/>
       <c r="D199" s="31"/>
       <c r="E199" s="31"/>
-      <c r="F199" s="38"/>
-      <c r="G199" s="39"/>
-      <c r="H199" s="40"/>
-    </row>
-    <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F199" s="35"/>
+      <c r="G199" s="36"/>
+      <c r="H199" s="37"/>
+    </row>
+    <row r="200" spans="1:8" ht="39" customHeight="1" thickBot="1">
       <c r="A200" s="32"/>
       <c r="B200" s="33"/>
       <c r="C200" s="33"/>
       <c r="D200" s="34"/>
       <c r="E200" s="34"/>
-      <c r="F200" s="59"/>
-      <c r="G200" s="60"/>
-      <c r="H200" s="61"/>
-    </row>
-    <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F200" s="38"/>
+      <c r="G200" s="39"/>
+      <c r="H200" s="40"/>
+    </row>
+    <row r="201" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="204">
-    <mergeCell ref="F196:H196"/>
-    <mergeCell ref="F197:H197"/>
-    <mergeCell ref="F198:H198"/>
-    <mergeCell ref="F199:H199"/>
-    <mergeCell ref="F200:H200"/>
-    <mergeCell ref="F191:H191"/>
-    <mergeCell ref="F192:H192"/>
-    <mergeCell ref="F193:H193"/>
-    <mergeCell ref="F194:H194"/>
-    <mergeCell ref="F195:H195"/>
-    <mergeCell ref="F186:H186"/>
-    <mergeCell ref="F187:H187"/>
-    <mergeCell ref="F188:H188"/>
-    <mergeCell ref="F189:H189"/>
-    <mergeCell ref="F190:H190"/>
-    <mergeCell ref="F181:H181"/>
-    <mergeCell ref="F182:H182"/>
-    <mergeCell ref="F183:H183"/>
-    <mergeCell ref="F184:H184"/>
-    <mergeCell ref="F185:H185"/>
-    <mergeCell ref="F176:H176"/>
-    <mergeCell ref="F177:H177"/>
-    <mergeCell ref="F178:H178"/>
-    <mergeCell ref="F179:H179"/>
-    <mergeCell ref="F180:H180"/>
-    <mergeCell ref="F171:H171"/>
-    <mergeCell ref="F172:H172"/>
-    <mergeCell ref="F173:H173"/>
-    <mergeCell ref="F174:H174"/>
-    <mergeCell ref="F175:H175"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="F167:H167"/>
-    <mergeCell ref="F168:H168"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="F170:H170"/>
-    <mergeCell ref="F161:H161"/>
-    <mergeCell ref="F162:H162"/>
-    <mergeCell ref="F163:H163"/>
-    <mergeCell ref="F164:H164"/>
-    <mergeCell ref="F165:H165"/>
-    <mergeCell ref="F156:H156"/>
-    <mergeCell ref="F157:H157"/>
-    <mergeCell ref="F158:H158"/>
-    <mergeCell ref="F159:H159"/>
-    <mergeCell ref="F160:H160"/>
-    <mergeCell ref="F151:H151"/>
-    <mergeCell ref="F152:H152"/>
-    <mergeCell ref="F153:H153"/>
-    <mergeCell ref="F154:H154"/>
-    <mergeCell ref="F155:H155"/>
-    <mergeCell ref="F146:H146"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F148:H148"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="F150:H150"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="F143:H143"/>
-    <mergeCell ref="F144:H144"/>
-    <mergeCell ref="F145:H145"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -3932,10 +3737,200 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F146:H146"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F148:H148"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="F150:H150"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="F143:H143"/>
+    <mergeCell ref="F144:H144"/>
+    <mergeCell ref="F145:H145"/>
+    <mergeCell ref="F156:H156"/>
+    <mergeCell ref="F157:H157"/>
+    <mergeCell ref="F158:H158"/>
+    <mergeCell ref="F159:H159"/>
+    <mergeCell ref="F160:H160"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="F152:H152"/>
+    <mergeCell ref="F153:H153"/>
+    <mergeCell ref="F154:H154"/>
+    <mergeCell ref="F155:H155"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="F167:H167"/>
+    <mergeCell ref="F168:H168"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="F170:H170"/>
+    <mergeCell ref="F161:H161"/>
+    <mergeCell ref="F162:H162"/>
+    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="F164:H164"/>
+    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="F176:H176"/>
+    <mergeCell ref="F177:H177"/>
+    <mergeCell ref="F178:H178"/>
+    <mergeCell ref="F179:H179"/>
+    <mergeCell ref="F180:H180"/>
+    <mergeCell ref="F171:H171"/>
+    <mergeCell ref="F172:H172"/>
+    <mergeCell ref="F173:H173"/>
+    <mergeCell ref="F174:H174"/>
+    <mergeCell ref="F175:H175"/>
+    <mergeCell ref="F186:H186"/>
+    <mergeCell ref="F187:H187"/>
+    <mergeCell ref="F188:H188"/>
+    <mergeCell ref="F189:H189"/>
+    <mergeCell ref="F190:H190"/>
+    <mergeCell ref="F181:H181"/>
+    <mergeCell ref="F182:H182"/>
+    <mergeCell ref="F183:H183"/>
+    <mergeCell ref="F184:H184"/>
+    <mergeCell ref="F185:H185"/>
+    <mergeCell ref="F196:H196"/>
+    <mergeCell ref="F197:H197"/>
+    <mergeCell ref="F198:H198"/>
+    <mergeCell ref="F199:H199"/>
+    <mergeCell ref="F200:H200"/>
+    <mergeCell ref="F191:H191"/>
+    <mergeCell ref="F192:H192"/>
+    <mergeCell ref="F193:H193"/>
+    <mergeCell ref="F194:H194"/>
+    <mergeCell ref="F195:H195"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -3948,17 +3943,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -3969,7 +3964,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>470</v>
       </c>
@@ -3980,7 +3975,7 @@
         <v>-1.2518171072006199</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>470</v>
       </c>
@@ -3991,7 +3986,7 @@
         <v>0.42159372568130499</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>470</v>
       </c>
@@ -4002,7 +3997,7 @@
         <v>2.3459901809692298</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>470</v>
       </c>
@@ -4013,7 +4008,7 @@
         <v>1.8428088426589899</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>470</v>
       </c>
@@ -4026,6 +4021,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4033,19 +4033,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="14" customWidth="1"/>
     <col min="2" max="4" width="15" style="14" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="14" customWidth="1"/>
     <col min="6" max="16384" width="15" style="14" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="36" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
@@ -4056,7 +4056,7 @@
       <c r="D1" s="62"/>
       <c r="E1" s="63"/>
     </row>
-    <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="36" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
@@ -4067,7 +4067,7 @@
       <c r="D2" s="64"/>
       <c r="E2" s="65"/>
     </row>
-    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="136" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -4076,7 +4076,7 @@
       <c r="D3" s="66"/>
       <c r="E3" s="67"/>
     </row>
-    <row r="4" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="46" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -4085,7 +4085,7 @@
       <c r="D4" s="71"/>
       <c r="E4" s="72"/>
     </row>
-    <row r="5" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="46" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="D5" s="66"/>
       <c r="E5" s="67"/>
     </row>
-    <row r="6" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="46" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="D6" s="66"/>
       <c r="E6" s="67"/>
     </row>
-    <row r="7" spans="1:5" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="46" customHeight="1">
       <c r="A7" s="17" t="s">
         <v>56</v>
       </c>
@@ -4112,7 +4112,7 @@
       <c r="D7" s="71"/>
       <c r="E7" s="72"/>
     </row>
-    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>30</v>
       </c>
@@ -4134,7 +4134,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -4147,19 +4147,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="36" customHeight="1">
       <c r="A1" s="73" t="s">
         <v>23</v>
       </c>
@@ -4170,7 +4170,7 @@
       <c r="F1" s="74"/>
       <c r="G1" s="75"/>
     </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="36" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>24</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="F2" s="66"/>
       <c r="G2" s="67"/>
     </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="36" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
@@ -4194,7 +4194,7 @@
       <c r="F3" s="66"/>
       <c r="G3" s="67"/>
     </row>
-    <row r="4" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="112" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -4205,7 +4205,7 @@
       <c r="F4" s="66"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
         <v>26</v>
       </c>
@@ -4216,8 +4216,8 @@
       <c r="F5" s="68"/>
       <c r="G5" s="69"/>
     </row>
-    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:7" ht="36" customHeight="1">
       <c r="A7" s="73" t="s">
         <v>27</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="F7" s="74"/>
       <c r="G7" s="75"/>
     </row>
-    <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="36" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -4239,7 +4239,7 @@
       <c r="F8" s="66"/>
       <c r="G8" s="67"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="36" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>25</v>
       </c>
@@ -4250,7 +4250,7 @@
       <c r="F9" s="66"/>
       <c r="G9" s="67"/>
     </row>
-    <row r="10" spans="1:7" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="112" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
@@ -4261,7 +4261,7 @@
       <c r="F10" s="66"/>
       <c r="G10" s="67"/>
     </row>
-    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
@@ -4272,9 +4272,9 @@
       <c r="F11" s="68"/>
       <c r="G11" s="69"/>
     </row>
-    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="36" customHeight="1"/>
+    <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
+    <row r="14" spans="1:7" ht="36" customHeight="1">
       <c r="A14" s="73" t="s">
         <v>28</v>
       </c>
@@ -4285,7 +4285,7 @@
       <c r="F14" s="74"/>
       <c r="G14" s="75"/>
     </row>
-    <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="36" customHeight="1">
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
@@ -4296,7 +4296,7 @@
       <c r="F15" s="66"/>
       <c r="G15" s="67"/>
     </row>
-    <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="36" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
@@ -4307,7 +4307,7 @@
       <c r="F16" s="66"/>
       <c r="G16" s="67"/>
     </row>
-    <row r="17" spans="1:7" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="113" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>6</v>
       </c>
@@ -4318,7 +4318,7 @@
       <c r="F17" s="66"/>
       <c r="G17" s="67"/>
     </row>
-    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A18" s="16" t="s">
         <v>26</v>
       </c>
@@ -4329,29 +4329,29 @@
       <c r="F18" s="68"/>
       <c r="G18" s="69"/>
     </row>
-    <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="36" customHeight="1"/>
+    <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>